<commit_message>
update generated data Triggered by a5fe440ae3f4416dbd54f745df2930d13be02663
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -9162,10 +9162,10 @@
         </is>
       </c>
       <c r="C282" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D282" t="n">
         <v>17.1077</v>
-      </c>
-      <c r="D282" t="n">
-        <v>48.1486</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update generated data Triggered by 6ce2f1e08c30cad1a48a7fbd4b44ea77d6772d0f
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -5539,23 +5539,23 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D172" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5565,96 +5565,96 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D173" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D174" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D175" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5664,26 +5664,26 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D176" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5697,26 +5697,26 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D177" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -5730,30 +5730,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D178" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5763,30 +5763,30 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D179" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5796,30 +5796,30 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D180" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5829,30 +5829,30 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D181" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5862,30 +5862,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D182" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5895,30 +5895,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D183" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5928,30 +5928,30 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D184" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5961,96 +5961,96 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>18.5799999237</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D185" t="n">
-        <v>-72.2925033569</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Port-Au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-0.1291666667</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D186" t="n">
-        <v>-78.3575</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-21.1363887787</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D187" t="n">
-        <v>-47.7766685486</v>
+        <v>-78.3575</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -6060,26 +6060,26 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D188" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -6093,26 +6093,26 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D189" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -6126,30 +6126,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D190" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6159,30 +6159,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D191" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6192,30 +6192,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-20.807157</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D192" t="n">
-        <v>-49.378994</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6225,26 +6225,26 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-23.4355564117</v>
+        <v>-20.807157</v>
       </c>
       <c r="D193" t="n">
-        <v>-46.4730567932</v>
+        <v>-49.378994</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -6258,26 +6258,26 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D194" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6291,30 +6291,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D195" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6324,30 +6324,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D196" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6357,30 +6357,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-18.8836116791</v>
+        <v>14.0608</v>
       </c>
       <c r="D197" t="n">
-        <v>-48.225276947</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6390,30 +6390,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>12.1888999939</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D198" t="n">
-        <v>-68.95980072019999</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6423,63 +6423,63 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>31.7226009369</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D199" t="n">
-        <v>35.9931983948</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D200" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -6489,30 +6489,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D201" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6522,30 +6522,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D202" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6555,30 +6555,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D203" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6588,30 +6588,30 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D204" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6621,30 +6621,30 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D205" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6654,30 +6654,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D206" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6687,30 +6687,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D207" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6720,30 +6720,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D208" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6753,30 +6753,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D209" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6786,30 +6786,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>29.226600647</v>
+        <v>32.78492</v>
       </c>
       <c r="D210" t="n">
-        <v>47.9688987732</v>
+        <v>34.96069</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6819,30 +6819,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D211" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6852,30 +6852,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D212" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6885,30 +6885,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D213" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6918,26 +6918,26 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D214" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -6951,30 +6951,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D215" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6984,30 +6984,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D216" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7017,30 +7017,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D217" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7050,59 +7050,59 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D218" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D219" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -7116,26 +7116,26 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D220" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -7149,26 +7149,26 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D221" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -7182,30 +7182,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D222" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7215,30 +7215,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D223" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7248,26 +7248,26 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D224" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -7281,26 +7281,26 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D225" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -7314,26 +7314,26 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D226" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -7347,26 +7347,26 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D227" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -7380,26 +7380,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D228" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7413,26 +7413,26 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D229" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7446,26 +7446,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D230" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7479,26 +7479,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D231" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7512,26 +7512,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D232" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7545,26 +7545,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D233" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7578,26 +7578,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D234" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7611,26 +7611,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D235" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7644,26 +7644,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D236" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7677,26 +7677,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D237" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7710,30 +7710,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D238" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7743,30 +7743,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D239" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7776,26 +7776,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D240" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7809,26 +7809,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D241" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7842,30 +7842,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D242" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7875,76 +7875,76 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Nashville, TN, United States</t>
-        </is>
-      </c>
-      <c r="C243" t="inlineStr"/>
-      <c r="D243" t="inlineStr"/>
-      <c r="E243" t="inlineStr"/>
-      <c r="F243" t="inlineStr"/>
-      <c r="G243" t="inlineStr"/>
+          <t>Montréal, QC, Canada</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>45.4706001282</v>
+      </c>
+      <c r="D243" t="n">
+        <v>-73.7407989502</v>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>Montréal</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
-        </is>
-      </c>
-      <c r="C244" t="n">
-        <v>40.6925010681</v>
-      </c>
-      <c r="D244" t="n">
-        <v>-74.1687011719</v>
-      </c>
-      <c r="E244" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F244" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G244" t="inlineStr">
-        <is>
-          <t>Newark</t>
-        </is>
-      </c>
+          <t>Nashville, TN, United States</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr"/>
+      <c r="E244" t="inlineStr"/>
+      <c r="F244" t="inlineStr"/>
+      <c r="G244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D245" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7958,26 +7958,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D246" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -7991,30 +7991,30 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D247" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -8024,30 +8024,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D248" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8057,26 +8057,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D249" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8090,26 +8090,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D250" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8123,26 +8123,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D251" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8156,30 +8156,30 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D252" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8189,30 +8189,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D253" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8222,26 +8222,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D254" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8255,26 +8255,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D255" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8288,26 +8288,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D256" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8321,26 +8321,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D257" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8354,30 +8354,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D258" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8387,30 +8387,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D259" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8420,26 +8420,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>38.7486991882</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D260" t="n">
-        <v>-90.37000274659999</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8453,26 +8453,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D261" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8486,26 +8486,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D262" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8519,30 +8519,30 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D263" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8552,26 +8552,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D264" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8585,26 +8585,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D265" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8618,63 +8618,63 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D266" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D267" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8684,30 +8684,30 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D268" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8717,26 +8717,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D269" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8750,96 +8750,96 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D270" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D271" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D272" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8849,30 +8849,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D273" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -8882,26 +8882,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D274" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -8915,106 +8915,106 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-31.31</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D275" t="n">
-        <v>-64.208333</v>
+        <v>151.177001953</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>OUA</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Ouagadougou, Burkina Faso</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>12.3531999588</v>
+        <v>-31.31</v>
       </c>
       <c r="D276" t="n">
-        <v>-1.5124200583</v>
+        <v>-64.208333</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>BF</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Ouagadougou</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>OUA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Ouagadougou, Burkina Faso</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>6.825648</v>
+        <v>12.3531999588</v>
       </c>
       <c r="D277" t="n">
-        <v>-58.163756</v>
+        <v>-1.5124200583</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BF</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Ouagadougou</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by de768f40b02907fa3323a2ab3935c171f38ac654
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G283"/>
+  <dimension ref="A1:G284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5440,23 +5440,23 @@
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-25.5284996033</v>
+        <v>-31.31</v>
       </c>
       <c r="D169" t="n">
-        <v>-49.1758003235</v>
+        <v>-64.208333</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5466,26 +5466,26 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D170" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5499,26 +5499,26 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D171" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -5532,30 +5532,30 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D172" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5565,30 +5565,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D173" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5598,96 +5598,96 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D174" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D175" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D176" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -5697,26 +5697,26 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D177" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -5730,26 +5730,26 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D178" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -5763,30 +5763,30 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D179" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5796,30 +5796,30 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D180" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5829,30 +5829,30 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D181" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5862,30 +5862,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D182" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5895,30 +5895,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D183" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5928,30 +5928,30 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D184" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5961,30 +5961,30 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D185" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5994,96 +5994,96 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>18.5799999237</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D186" t="n">
-        <v>-72.2925033569</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Port-Au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-0.1291666667</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D187" t="n">
-        <v>-78.3575</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-21.1363887787</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D188" t="n">
-        <v>-47.7766685486</v>
+        <v>-78.3575</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6093,26 +6093,26 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D189" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -6126,26 +6126,26 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D190" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -6159,30 +6159,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D191" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6192,30 +6192,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D192" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6225,30 +6225,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-20.807157</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D193" t="n">
-        <v>-49.378994</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6258,26 +6258,26 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-23.4355564117</v>
+        <v>-20.807157</v>
       </c>
       <c r="D194" t="n">
-        <v>-46.4730567932</v>
+        <v>-49.378994</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6291,26 +6291,26 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D195" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -6324,30 +6324,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D196" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6357,30 +6357,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D197" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6390,30 +6390,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-18.8836116791</v>
+        <v>14.0608</v>
       </c>
       <c r="D198" t="n">
-        <v>-48.225276947</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6423,30 +6423,30 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>12.1888999939</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D199" t="n">
-        <v>-68.95980072019999</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6456,63 +6456,63 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>31.7226009369</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D200" t="n">
-        <v>35.9931983948</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D201" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6522,30 +6522,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D202" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6555,30 +6555,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D203" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6588,30 +6588,30 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D204" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6621,30 +6621,30 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D205" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6654,30 +6654,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D206" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6687,30 +6687,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D207" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6720,30 +6720,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D208" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6753,30 +6753,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D209" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6786,30 +6786,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D210" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6819,30 +6819,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>29.226600647</v>
+        <v>32.78492</v>
       </c>
       <c r="D211" t="n">
-        <v>47.9688987732</v>
+        <v>34.96069</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6852,30 +6852,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D212" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6885,30 +6885,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D213" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6918,30 +6918,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D214" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6951,26 +6951,26 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D215" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -6984,30 +6984,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D216" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7017,30 +7017,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D217" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7050,30 +7050,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D218" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7083,59 +7083,59 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D219" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D220" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -7149,26 +7149,26 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D221" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -7182,26 +7182,26 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D222" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -7215,30 +7215,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D223" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7248,30 +7248,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D224" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7281,26 +7281,26 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D225" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -7314,26 +7314,26 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D226" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -7347,26 +7347,26 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D227" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -7380,26 +7380,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D228" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7413,26 +7413,26 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D229" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7446,26 +7446,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D230" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7479,26 +7479,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D231" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7512,26 +7512,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D232" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7545,26 +7545,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D233" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7578,26 +7578,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D234" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7611,26 +7611,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D235" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7644,26 +7644,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D236" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7677,26 +7677,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D237" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7710,26 +7710,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D238" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7743,30 +7743,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D239" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7776,30 +7776,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D240" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7809,26 +7809,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D241" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7842,26 +7842,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D242" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7875,30 +7875,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D243" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7908,76 +7908,76 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Nashville, TN, United States</t>
-        </is>
-      </c>
-      <c r="C244" t="inlineStr"/>
-      <c r="D244" t="inlineStr"/>
-      <c r="E244" t="inlineStr"/>
-      <c r="F244" t="inlineStr"/>
-      <c r="G244" t="inlineStr"/>
+          <t>Montréal, QC, Canada</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>45.4706001282</v>
+      </c>
+      <c r="D244" t="n">
+        <v>-73.7407989502</v>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>Montréal</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
-        </is>
-      </c>
-      <c r="C245" t="n">
-        <v>40.6925010681</v>
-      </c>
-      <c r="D245" t="n">
-        <v>-74.1687011719</v>
-      </c>
-      <c r="E245" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F245" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G245" t="inlineStr">
-        <is>
-          <t>Newark</t>
-        </is>
-      </c>
+          <t>Nashville, TN, United States</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr"/>
+      <c r="E245" t="inlineStr"/>
+      <c r="F245" t="inlineStr"/>
+      <c r="G245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D246" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -7991,26 +7991,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D247" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8024,30 +8024,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D248" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8057,30 +8057,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D249" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8090,26 +8090,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D250" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8123,26 +8123,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D251" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8156,26 +8156,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D252" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8189,30 +8189,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D253" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8222,30 +8222,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D254" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8255,26 +8255,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D255" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8288,26 +8288,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D256" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8321,26 +8321,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D257" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8354,26 +8354,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D258" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8387,30 +8387,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D259" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8420,30 +8420,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D260" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8453,26 +8453,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>38.7486991882</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D261" t="n">
-        <v>-90.37000274659999</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8486,26 +8486,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D262" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8519,26 +8519,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D263" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8552,30 +8552,30 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D264" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8585,26 +8585,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D265" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8618,26 +8618,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D266" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8651,63 +8651,63 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D267" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D268" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8717,30 +8717,30 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D269" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8750,26 +8750,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D270" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8783,96 +8783,96 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D271" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D272" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D273" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -8882,30 +8882,30 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D274" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -8915,26 +8915,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D275" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -8948,63 +8948,63 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-31.31</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D276" t="n">
-        <v>-64.208333</v>
+        <v>151.177001953</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>OUA</t>
+          <t>GBE</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Ouagadougou, Burkina Faso</t>
+          <t>Gaborone, Botswana</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>12.3531999588</v>
+        <v>-24.6282</v>
       </c>
       <c r="D277" t="n">
-        <v>-1.5124200583</v>
+        <v>25.9231</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>BF</t>
+          <t>BW</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9014,63 +9014,63 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Ouagadougou</t>
+          <t>Gaborone</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>OKA</t>
+          <t>OUA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Naha, Japan</t>
+          <t>Ouagadougou, Burkina Faso</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>26.1958</v>
+        <v>12.3531999588</v>
       </c>
       <c r="D278" t="n">
-        <v>127.646</v>
+        <v>-1.5124200583</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>BF</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Naha</t>
+          <t>Ouagadougou</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>MDL</t>
+          <t>OKA</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Mandalay, Myanmar (Burma)</t>
+          <t>Naha, Japan</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>39.2276</v>
+        <v>26.1958</v>
       </c>
       <c r="D279" t="n">
-        <v>-74.63704</v>
+        <v>127.646</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>MM</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9080,30 +9080,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Mandalay</t>
+          <t>Naha</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>MDL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Mandalay, Myanmar (Burma)</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>8.415619850200001</v>
+        <v>39.2276</v>
       </c>
       <c r="D280" t="n">
-        <v>124.611000061</v>
+        <v>-74.63704</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>MM</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9113,104 +9113,137 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Mandalay</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>21.679599762</v>
+        <v>8.415619850200001</v>
       </c>
       <c r="D281" t="n">
-        <v>39.15650177</v>
+        <v>124.611000061</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>48.1486</v>
+        <v>21.679599762</v>
       </c>
       <c r="D282" t="n">
-        <v>17.1077</v>
+        <v>39.15650177</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Bratislava, Slovakia</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D283" t="n">
+        <v>17.1077</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>Bratislava</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B283" t="inlineStr">
+      <c r="B284" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C283" t="n">
+      <c r="C284" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D283" t="n">
+      <c r="D284" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E283" t="inlineStr">
+      <c r="E284" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F283" t="inlineStr">
+      <c r="F284" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G283" t="inlineStr">
+      <c r="G284" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by a4dbfe298760e0bc3c77812f14dfb9e4e9f1231e
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G285"/>
+  <dimension ref="A1:G287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -6892,23 +6892,23 @@
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D213" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6918,30 +6918,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D214" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6951,30 +6951,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D215" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6984,30 +6984,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D216" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7017,26 +7017,26 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D217" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -7050,30 +7050,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D218" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7083,30 +7083,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D219" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7116,30 +7116,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D220" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7149,59 +7149,59 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D221" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D222" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -7215,26 +7215,26 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D223" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -7248,26 +7248,26 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D224" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -7281,30 +7281,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D225" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7314,30 +7314,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D226" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7347,26 +7347,26 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D227" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -7380,26 +7380,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D228" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7413,26 +7413,26 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D229" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7446,26 +7446,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D230" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7479,26 +7479,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D231" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7512,26 +7512,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D232" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7545,26 +7545,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D233" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7578,26 +7578,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D234" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7611,26 +7611,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D235" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7644,26 +7644,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D236" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7677,26 +7677,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D237" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7710,26 +7710,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D238" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7743,26 +7743,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D239" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7776,26 +7776,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D240" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7809,30 +7809,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D241" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7842,30 +7842,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D242" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7875,26 +7875,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D243" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -7908,26 +7908,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D244" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7941,30 +7941,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D245" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -7974,76 +7974,76 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Nashville, TN, United States</t>
-        </is>
-      </c>
-      <c r="C246" t="inlineStr"/>
-      <c r="D246" t="inlineStr"/>
-      <c r="E246" t="inlineStr"/>
-      <c r="F246" t="inlineStr"/>
-      <c r="G246" t="inlineStr"/>
+          <t>Montréal, QC, Canada</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>45.4706001282</v>
+      </c>
+      <c r="D246" t="n">
+        <v>-73.7407989502</v>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>Montréal</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
-        </is>
-      </c>
-      <c r="C247" t="n">
-        <v>40.6925010681</v>
-      </c>
-      <c r="D247" t="n">
-        <v>-74.1687011719</v>
-      </c>
-      <c r="E247" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F247" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G247" t="inlineStr">
-        <is>
-          <t>Newark</t>
-        </is>
-      </c>
+          <t>Nashville, TN, United States</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
+      <c r="E247" t="inlineStr"/>
+      <c r="F247" t="inlineStr"/>
+      <c r="G247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D248" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8057,26 +8057,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D249" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8090,30 +8090,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D250" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8123,30 +8123,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D251" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8156,26 +8156,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D252" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8189,26 +8189,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D253" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8222,26 +8222,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D254" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8255,30 +8255,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D255" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8288,30 +8288,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D256" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8321,26 +8321,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D257" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8354,26 +8354,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D258" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8387,26 +8387,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D259" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8420,26 +8420,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D260" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8453,30 +8453,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D261" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8486,30 +8486,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D262" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8519,26 +8519,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>38.7486991882</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D263" t="n">
-        <v>-90.37000274659999</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8552,26 +8552,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D264" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8585,26 +8585,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D265" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8618,30 +8618,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D266" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8651,26 +8651,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D267" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8684,26 +8684,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D268" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8717,63 +8717,63 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D269" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D270" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8783,30 +8783,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D271" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8816,26 +8816,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D272" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8849,96 +8849,96 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D273" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D274" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D275" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -8948,30 +8948,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D276" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -8981,26 +8981,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D277" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9014,162 +9014,162 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Cuiaba, Brazil</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-15.59611</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D278" t="n">
-        <v>-56.09667</v>
+        <v>151.177001953</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>OUA</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Ouagadougou, Burkina Faso</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>12.3531999588</v>
+        <v>-42.883209</v>
       </c>
       <c r="D279" t="n">
-        <v>-1.5124200583</v>
+        <v>147.331665</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>BF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Ouagadougou</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>OKA</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Naha, Japan</t>
+          <t>Cuiaba, Brazil</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>26.1958</v>
+        <v>-15.59611</v>
       </c>
       <c r="D280" t="n">
-        <v>127.646</v>
+        <v>-56.09667</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Naha</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>MDL</t>
+          <t>OUA</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Mandalay, Myanmar (Burma)</t>
+          <t>Ouagadougou, Burkina Faso</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>39.2276</v>
+        <v>12.3531999588</v>
       </c>
       <c r="D281" t="n">
-        <v>-74.63704</v>
+        <v>-1.5124200583</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>MM</t>
+          <t>BF</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Mandalay</t>
+          <t>Ouagadougou</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>OKA</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Naha, Japan</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>8.415619850200001</v>
+        <v>26.1958</v>
       </c>
       <c r="D282" t="n">
-        <v>124.611000061</v>
+        <v>127.646</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9179,104 +9179,170 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Naha</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>MDL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Mandalay, Myanmar (Burma)</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>21.679599762</v>
+        <v>39.2276</v>
       </c>
       <c r="D283" t="n">
-        <v>39.15650177</v>
+        <v>-74.63704</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>MM</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Mandalay</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>48.1486</v>
+        <v>-43.5465</v>
       </c>
       <c r="D284" t="n">
-        <v>17.1077</v>
+        <v>172.6331</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
+          <t>CGY</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Cagayan de Oro, Philippines</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>8.415619850200001</v>
+      </c>
+      <c r="D285" t="n">
+        <v>124.611000061</v>
+      </c>
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>Cagayan de Oro</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="inlineStr">
+        <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Bratislava, Slovakia</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D286" t="n">
+        <v>17.1077</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>Bratislava</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B285" t="inlineStr">
+      <c r="B287" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C285" t="n">
+      <c r="C287" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D285" t="n">
+      <c r="D287" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E285" t="inlineStr">
+      <c r="E287" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F285" t="inlineStr">
+      <c r="F287" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G285" t="inlineStr">
+      <c r="G287" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 795dacfdd830214eaf247479e9fdd5ee3b3ffbeb
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G287"/>
+  <dimension ref="A1:G288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9285,23 +9285,23 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Tver, Russia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>48.1486</v>
+        <v>56.8587</v>
       </c>
       <c r="D286" t="n">
-        <v>17.1077</v>
+        <v>35.9176</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9311,38 +9311,71 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Tver</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Bratislava, Slovakia</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D287" t="n">
+        <v>17.1077</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>Bratislava</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B287" t="inlineStr">
+      <c r="B288" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C287" t="n">
+      <c r="C288" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D287" t="n">
+      <c r="D288" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E287" t="inlineStr">
+      <c r="E288" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F287" t="inlineStr">
+      <c r="F288" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G287" t="inlineStr">
+      <c r="G288" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by ae3732c4d8011e58d6ffcf1090c7adeb8f5cdc82
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -8922,19 +8922,19 @@
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D275" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -8948,30 +8948,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D276" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -8981,30 +8981,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D277" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9014,26 +9014,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D278" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9047,26 +9047,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-42.883209</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D279" t="n">
-        <v>147.331665</v>
+        <v>151.177001953</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9080,7 +9080,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
@@ -9228,10 +9228,10 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>-43.5465</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D284" t="n">
-        <v>172.6331</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update generated data Triggered by 157c74fe1094412f3a103b8d0205e5bccb0b49fe
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -5506,19 +5506,19 @@
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-25.5284996033</v>
+        <v>-15.59611</v>
       </c>
       <c r="D171" t="n">
-        <v>-49.1758003235</v>
+        <v>-56.09667</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -5532,26 +5532,26 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D172" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -5565,26 +5565,26 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D173" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -5598,30 +5598,30 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D174" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5631,30 +5631,30 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D175" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5664,96 +5664,96 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D176" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D177" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D178" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5763,26 +5763,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D179" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5796,26 +5796,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D180" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5829,30 +5829,30 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D181" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5862,30 +5862,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D182" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5895,30 +5895,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D183" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -5928,30 +5928,30 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D184" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5961,30 +5961,30 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D185" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5994,30 +5994,30 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D186" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6027,30 +6027,30 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D187" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -6060,96 +6060,96 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>18.5799999237</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D188" t="n">
-        <v>-72.2925033569</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Port-Au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-0.1291666667</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D189" t="n">
-        <v>-78.3575</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-21.1363887787</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D190" t="n">
-        <v>-47.7766685486</v>
+        <v>-78.3575</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6159,26 +6159,26 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D191" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -6192,26 +6192,26 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D192" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -6225,30 +6225,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D193" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6258,30 +6258,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D194" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6291,30 +6291,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-20.807157</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D195" t="n">
-        <v>-49.378994</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6324,26 +6324,26 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-23.4355564117</v>
+        <v>-20.807157</v>
       </c>
       <c r="D196" t="n">
-        <v>-46.4730567932</v>
+        <v>-49.378994</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -6357,26 +6357,26 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D197" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -6390,30 +6390,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D198" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6423,30 +6423,30 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D199" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6456,30 +6456,30 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-18.8836116791</v>
+        <v>14.0608</v>
       </c>
       <c r="D200" t="n">
-        <v>-48.225276947</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -6489,30 +6489,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>12.1888999939</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D201" t="n">
-        <v>-68.95980072019999</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6522,63 +6522,63 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>31.7226009369</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D202" t="n">
-        <v>35.9931983948</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D203" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6588,30 +6588,30 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D204" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6621,30 +6621,30 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D205" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6654,30 +6654,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D206" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6687,30 +6687,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D207" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6720,30 +6720,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D208" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6753,30 +6753,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D209" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6786,30 +6786,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D210" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6819,30 +6819,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D211" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6852,30 +6852,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D212" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6885,30 +6885,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D213" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6918,30 +6918,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D214" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6951,30 +6951,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D215" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6984,30 +6984,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D216" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7017,30 +7017,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D217" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7050,26 +7050,26 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D218" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -7083,30 +7083,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D219" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7116,30 +7116,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D220" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7149,30 +7149,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D221" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7182,59 +7182,59 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D222" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D223" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -7248,26 +7248,26 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D224" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -7281,26 +7281,26 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D225" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -7314,30 +7314,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D226" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7347,30 +7347,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D227" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7380,26 +7380,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D228" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7413,26 +7413,26 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D229" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -7446,26 +7446,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D230" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7479,26 +7479,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D231" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7512,26 +7512,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D232" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7545,26 +7545,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D233" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7578,26 +7578,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D234" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7611,26 +7611,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D235" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7644,26 +7644,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D236" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7677,26 +7677,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D237" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7710,26 +7710,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D238" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7743,26 +7743,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D239" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7776,26 +7776,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D240" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7809,26 +7809,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D241" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7842,30 +7842,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D242" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7875,30 +7875,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D243" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7908,26 +7908,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D244" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7941,26 +7941,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D245" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -7974,30 +7974,30 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D246" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8007,76 +8007,76 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Nashville, TN, United States</t>
-        </is>
-      </c>
-      <c r="C247" t="inlineStr"/>
-      <c r="D247" t="inlineStr"/>
-      <c r="E247" t="inlineStr"/>
-      <c r="F247" t="inlineStr"/>
-      <c r="G247" t="inlineStr"/>
+          <t>Montréal, QC, Canada</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>45.4706001282</v>
+      </c>
+      <c r="D247" t="n">
+        <v>-73.7407989502</v>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>Montréal</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
-        </is>
-      </c>
-      <c r="C248" t="n">
-        <v>40.6925010681</v>
-      </c>
-      <c r="D248" t="n">
-        <v>-74.1687011719</v>
-      </c>
-      <c r="E248" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F248" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G248" t="inlineStr">
-        <is>
-          <t>Newark</t>
-        </is>
-      </c>
+          <t>Nashville, TN, United States</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr"/>
+      <c r="D248" t="inlineStr"/>
+      <c r="E248" t="inlineStr"/>
+      <c r="F248" t="inlineStr"/>
+      <c r="G248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D249" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8090,26 +8090,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D250" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8123,30 +8123,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D251" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8156,30 +8156,30 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D252" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8189,26 +8189,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D253" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8222,26 +8222,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D254" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8255,26 +8255,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D255" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8288,30 +8288,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D256" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8321,30 +8321,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D257" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8354,26 +8354,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D258" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8387,26 +8387,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D259" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8420,26 +8420,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D260" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8453,26 +8453,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D261" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8486,30 +8486,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D262" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8519,30 +8519,30 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D263" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8552,26 +8552,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>38.7486991882</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D264" t="n">
-        <v>-90.37000274659999</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8585,26 +8585,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D265" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8618,26 +8618,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D266" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8651,30 +8651,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D267" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8684,26 +8684,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D268" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8717,26 +8717,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D269" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8750,63 +8750,63 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D270" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D271" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8816,30 +8816,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D272" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8849,26 +8849,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D273" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -8882,92 +8882,92 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D274" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D275" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D276" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -8981,30 +8981,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D277" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9014,30 +9014,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D278" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9047,26 +9047,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D279" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9080,40 +9080,40 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Cuiaba, Brazil</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>-15.59611</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D280" t="n">
-        <v>-56.09667</v>
+        <v>151.177001953</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 12b0b3ee1afa1a7b4f20667e0e6bc3c10121eadc
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9252,122 +9252,122 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CCP</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Concepción, Chile</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-43.4893989563</v>
+        <v>-36.8201</v>
       </c>
       <c r="D285" t="n">
-        <v>172.5319976807</v>
+        <v>-73.0444</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Concepción</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>8.415619850200001</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D286" t="n">
-        <v>124.611000061</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>KLD</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Tver, Russia</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>56.8587</v>
+        <v>8.415619850200001</v>
       </c>
       <c r="D287" t="n">
-        <v>35.9176</v>
+        <v>124.611000061</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Tver</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Tver, Russia</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>48.1486</v>
+        <v>56.8587</v>
       </c>
       <c r="D288" t="n">
-        <v>17.1077</v>
+        <v>35.9176</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9377,38 +9377,71 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Tver</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Bratislava, Slovakia</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D289" t="n">
+        <v>17.1077</v>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>Bratislava</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B289" t="inlineStr">
+      <c r="B290" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C289" t="n">
+      <c r="C290" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D289" t="n">
+      <c r="D290" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E289" t="inlineStr">
+      <c r="E290" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F289" t="inlineStr">
+      <c r="F290" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G289" t="inlineStr">
+      <c r="G290" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 3ad5bad9d26ca73885a001144801a3fd1510fb8a
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G290"/>
+  <dimension ref="A1:G291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4978,23 +4978,23 @@
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>VIE</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Vienna, Austria</t>
+          <t>Tirana, Albania</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>48.1102981567</v>
+        <v>41.4146995544</v>
       </c>
       <c r="D155" t="n">
-        <v>16.5697002411</v>
+        <v>19.7206001282</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -5004,30 +5004,30 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Vienna</t>
+          <t>Tirana</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>VNO</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Vilnius, Lithuania</t>
+          <t>Vienna, Austria</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>54.6341018677</v>
+        <v>48.1102981567</v>
       </c>
       <c r="D156" t="n">
-        <v>25.2858009338</v>
+        <v>16.5697002411</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -5037,30 +5037,30 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>Vienna</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>WAW</t>
+          <t>VNO</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Warsaw, Poland</t>
+          <t>Vilnius, Lithuania</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>52.1656990051</v>
+        <v>54.6341018677</v>
       </c>
       <c r="D157" t="n">
-        <v>20.9671001434</v>
+        <v>25.2858009338</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>LT</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -5070,96 +5070,96 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Warsaw</t>
+          <t>Vilnius</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>SVX</t>
+          <t>WAW</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Yekaterinburg, Russia</t>
+          <t>Warsaw, Poland</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>56.8431</v>
+        <v>52.1656990051</v>
       </c>
       <c r="D158" t="n">
-        <v>60.6454</v>
+        <v>20.9671001434</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Yekaterinburg</t>
+          <t>Warsaw</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>ZAG</t>
+          <t>SVX</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Zagreb, Croatia</t>
+          <t>Yekaterinburg, Russia</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>45.7429008484</v>
+        <v>56.8431</v>
       </c>
       <c r="D159" t="n">
-        <v>16.0687999725</v>
+        <v>60.6454</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Zagreb</t>
+          <t>Yekaterinburg</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>ZAG</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Zürich, Switzerland</t>
+          <t>Zagreb, Croatia</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>47.4646987915</v>
+        <v>45.7429008484</v>
       </c>
       <c r="D160" t="n">
-        <v>8.549169540399999</v>
+        <v>16.0687999725</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -5169,63 +5169,63 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Zurich</t>
+          <t>Zagreb</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Zürich, Switzerland</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>-22.738</v>
+        <v>47.4646987915</v>
       </c>
       <c r="D161" t="n">
-        <v>-47.334</v>
+        <v>8.549169540399999</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Zurich</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>-18.348611</v>
+        <v>-22.738</v>
       </c>
       <c r="D162" t="n">
-        <v>-70.33888899999999</v>
+        <v>-47.334</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -5235,30 +5235,30 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>-25.2399997711</v>
+        <v>-18.348611</v>
       </c>
       <c r="D163" t="n">
-        <v>-57.5200004578</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5268,30 +5268,30 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>-1.4563</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="D164" t="n">
-        <v>-48.5013</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5301,26 +5301,26 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-19.624444</v>
+        <v>-1.4563</v>
       </c>
       <c r="D165" t="n">
-        <v>-43.971944</v>
+        <v>-48.5013</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -5334,26 +5334,26 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-26.89245</v>
+        <v>-19.624444</v>
       </c>
       <c r="D166" t="n">
-        <v>-49.07696</v>
+        <v>-43.971944</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -5367,30 +5367,30 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>4.70159</v>
+        <v>-26.89245</v>
       </c>
       <c r="D167" t="n">
-        <v>-74.1469</v>
+        <v>-49.07696</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5400,30 +5400,30 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-15.79824</v>
+        <v>4.70159</v>
       </c>
       <c r="D168" t="n">
-        <v>-47.90859</v>
+        <v>-74.1469</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5433,30 +5433,30 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-34.8222</v>
+        <v>-15.79824</v>
       </c>
       <c r="D169" t="n">
-        <v>-58.5358</v>
+        <v>-47.90859</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5466,30 +5466,30 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-26.7762</v>
+        <v>-34.8222</v>
       </c>
       <c r="D170" t="n">
-        <v>-51.0125</v>
+        <v>-58.5358</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5499,26 +5499,26 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-22.90662</v>
+        <v>-26.7762</v>
       </c>
       <c r="D171" t="n">
-        <v>-47.08576</v>
+        <v>-51.0125</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -5532,30 +5532,30 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-31.31</v>
+        <v>-22.90662</v>
       </c>
       <c r="D172" t="n">
-        <v>-64.208333</v>
+        <v>-47.08576</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5565,30 +5565,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-15.59611</v>
+        <v>-31.31</v>
       </c>
       <c r="D173" t="n">
-        <v>-56.09667</v>
+        <v>-64.208333</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5598,26 +5598,26 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-25.5284996033</v>
+        <v>-15.59611</v>
       </c>
       <c r="D174" t="n">
-        <v>-49.1758003235</v>
+        <v>-56.09667</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -5631,26 +5631,26 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D175" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -5664,26 +5664,26 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D176" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5697,30 +5697,30 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D177" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5730,30 +5730,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D178" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5763,96 +5763,96 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D179" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D180" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D181" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5862,26 +5862,26 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D182" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -5895,26 +5895,26 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D183" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -5928,30 +5928,30 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D184" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -5961,30 +5961,30 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D185" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5994,30 +5994,30 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D186" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6027,30 +6027,30 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D187" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -6060,30 +6060,30 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D188" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6093,30 +6093,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D189" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6126,30 +6126,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D190" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6159,96 +6159,96 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>18.5799999237</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D191" t="n">
-        <v>-72.2925033569</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Port-Au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-0.1291666667</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D192" t="n">
-        <v>-78.3575</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-21.1363887787</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D193" t="n">
-        <v>-47.7766685486</v>
+        <v>-78.3575</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6258,26 +6258,26 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D194" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6291,26 +6291,26 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D195" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -6324,30 +6324,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D196" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6357,30 +6357,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D197" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6390,30 +6390,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-20.807157</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D198" t="n">
-        <v>-49.378994</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6423,26 +6423,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-23.4355564117</v>
+        <v>-20.807157</v>
       </c>
       <c r="D199" t="n">
-        <v>-46.4730567932</v>
+        <v>-49.378994</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6456,26 +6456,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D200" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6489,30 +6489,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D201" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6522,30 +6522,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D202" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6555,30 +6555,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-18.8836116791</v>
+        <v>14.0608</v>
       </c>
       <c r="D203" t="n">
-        <v>-48.225276947</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6588,30 +6588,30 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>12.1888999939</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D204" t="n">
-        <v>-68.95980072019999</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6621,63 +6621,63 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>31.7226009369</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D205" t="n">
-        <v>35.9931983948</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D206" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6687,30 +6687,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D207" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6720,30 +6720,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D208" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6753,30 +6753,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D209" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6786,30 +6786,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D210" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6819,30 +6819,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D211" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6852,30 +6852,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D212" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6885,30 +6885,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D213" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -6918,30 +6918,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D214" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6951,30 +6951,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D215" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -6984,30 +6984,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D216" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7017,30 +7017,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D217" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7050,30 +7050,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D218" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7083,30 +7083,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D219" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7116,30 +7116,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D220" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7149,26 +7149,26 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D221" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -7182,30 +7182,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D222" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7215,30 +7215,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D223" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7248,30 +7248,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D224" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7281,59 +7281,59 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D225" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D226" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -7347,26 +7347,26 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D227" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -7380,26 +7380,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D228" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7413,30 +7413,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D229" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7446,30 +7446,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D230" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7479,26 +7479,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D231" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7512,26 +7512,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D232" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7545,26 +7545,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D233" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7578,26 +7578,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D234" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7611,26 +7611,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D235" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7644,26 +7644,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D236" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7677,26 +7677,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D237" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7710,26 +7710,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D238" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7743,26 +7743,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D239" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7776,26 +7776,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D240" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7809,26 +7809,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D241" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7842,26 +7842,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D242" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7875,26 +7875,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D243" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -7908,26 +7908,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D244" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -7941,30 +7941,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D245" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -7974,30 +7974,30 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D246" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8007,26 +8007,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D247" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8040,26 +8040,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D248" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8073,30 +8073,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D249" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8106,76 +8106,76 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Nashville, TN, United States</t>
-        </is>
-      </c>
-      <c r="C250" t="inlineStr"/>
-      <c r="D250" t="inlineStr"/>
-      <c r="E250" t="inlineStr"/>
-      <c r="F250" t="inlineStr"/>
-      <c r="G250" t="inlineStr"/>
+          <t>Montréal, QC, Canada</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>45.4706001282</v>
+      </c>
+      <c r="D250" t="n">
+        <v>-73.7407989502</v>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>Montréal</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
-        </is>
-      </c>
-      <c r="C251" t="n">
-        <v>40.6925010681</v>
-      </c>
-      <c r="D251" t="n">
-        <v>-74.1687011719</v>
-      </c>
-      <c r="E251" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F251" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G251" t="inlineStr">
-        <is>
-          <t>Newark</t>
-        </is>
-      </c>
+          <t>Nashville, TN, United States</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr"/>
+      <c r="D251" t="inlineStr"/>
+      <c r="E251" t="inlineStr"/>
+      <c r="F251" t="inlineStr"/>
+      <c r="G251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D252" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8189,26 +8189,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D253" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8222,30 +8222,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D254" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8255,30 +8255,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D255" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8288,26 +8288,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D256" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8321,26 +8321,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D257" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8354,26 +8354,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D258" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8387,30 +8387,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D259" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8420,30 +8420,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D260" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8453,26 +8453,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D261" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8486,26 +8486,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D262" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8519,26 +8519,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D263" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8552,26 +8552,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D264" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8585,30 +8585,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D265" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8618,30 +8618,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D266" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8651,26 +8651,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>38.7486991882</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D267" t="n">
-        <v>-90.37000274659999</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8684,26 +8684,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D268" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8717,26 +8717,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D269" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8750,30 +8750,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D270" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8783,26 +8783,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D271" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8816,26 +8816,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D272" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8849,63 +8849,63 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D273" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D274" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -8915,30 +8915,30 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D275" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -8948,26 +8948,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D276" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -8981,63 +8981,63 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D277" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-42.883209</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D278" t="n">
-        <v>147.331665</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9047,63 +9047,63 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D279" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>-22.0146007538</v>
+        <v>-42.883209</v>
       </c>
       <c r="D280" t="n">
-        <v>166.212997436</v>
+        <v>147.331665</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9113,26 +9113,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>-31.9402999878</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D281" t="n">
-        <v>115.967002869</v>
+        <v>144.843002319</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9146,30 +9146,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-33.9460983276</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D282" t="n">
-        <v>151.177001953</v>
+        <v>166.212997436</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9179,228 +9179,228 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Tirana, Albania</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>41.4146995544</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D283" t="n">
-        <v>19.7206001282</v>
+        <v>115.967002869</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Tirana</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>OUA</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Ouagadougou, Burkina Faso</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>12.3531999588</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D284" t="n">
-        <v>-1.5124200583</v>
+        <v>151.177001953</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>BF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Ouagadougou</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>CCP</t>
+          <t>OUA</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Concepción, Chile</t>
+          <t>Ouagadougou, Burkina Faso</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-36.8201</v>
+        <v>12.3531999588</v>
       </c>
       <c r="D285" t="n">
-        <v>-73.0444</v>
+        <v>-1.5124200583</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BF</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Africa</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Concepción</t>
+          <t>Ouagadougou</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CCP</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Concepción, Chile</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-43.4893989563</v>
+        <v>-36.8201</v>
       </c>
       <c r="D286" t="n">
-        <v>172.5319976807</v>
+        <v>-73.0444</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Concepción</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>8.415619850200001</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D287" t="n">
-        <v>124.611000061</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>KLD</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Tver, Russia</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>56.8587</v>
+        <v>8.415619850200001</v>
       </c>
       <c r="D288" t="n">
-        <v>35.9176</v>
+        <v>124.611000061</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Tver</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Tver, Russia</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>48.1486</v>
+        <v>56.8587</v>
       </c>
       <c r="D289" t="n">
-        <v>17.1077</v>
+        <v>35.9176</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9410,38 +9410,71 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Tver</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
+          <t>BTS</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Bratislava, Slovakia</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>48.1486</v>
+      </c>
+      <c r="D290" t="n">
+        <v>17.1077</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>Bratislava</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B290" t="inlineStr">
+      <c r="B291" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C290" t="n">
+      <c r="C291" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D290" t="n">
+      <c r="D291" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E290" t="inlineStr">
+      <c r="E291" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F290" t="inlineStr">
+      <c r="F291" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G290" t="inlineStr">
+      <c r="G291" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by f036faf7b54d61aa3a288caa58169c0b8e60f282
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G282"/>
+  <dimension ref="A1:G283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9297,31 +9297,64 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
+          <t>KHH</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Kaohsiung City, Taiwan</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>22.5771007538</v>
+      </c>
+      <c r="D282" t="n">
+        <v>120.3499984741</v>
+      </c>
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>Kaohsiung City</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B282" t="inlineStr">
+      <c r="B283" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C282" t="n">
+      <c r="C283" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D282" t="n">
+      <c r="D283" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E282" t="inlineStr">
+      <c r="E283" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F282" t="inlineStr">
+      <c r="F283" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G282" t="inlineStr">
+      <c r="G283" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 2425b7a7927fac0147c4dbfeaa979f4a23f3471c
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -4388,27 +4388,11 @@
           <t>Minsk, Belarus</t>
         </is>
       </c>
-      <c r="C133" t="n">
-        <v>53.9006</v>
-      </c>
-      <c r="D133" t="n">
-        <v>27.599</v>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>BY</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>Minsk</t>
-        </is>
-      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by bbb91394a4f20e6d30e08e0110431ad357c66d66
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -1042,27 +1042,11 @@
           <t>Monrovia, Liberia</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>6.239127</v>
-      </c>
-      <c r="D19" t="n">
-        <v>-10.35462</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LR</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Africa</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Monrovia</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by f4e0149b646dd84313aa72f500b4d61c2b705bb8
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G283"/>
+  <dimension ref="A1:G284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9298,31 +9298,64 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
+          <t>ISU</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Sulaymaniyah, Iraq</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>35.5668</v>
+      </c>
+      <c r="D283" t="n">
+        <v>45.4161</v>
+      </c>
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>IQ</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Middle East</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>Sulaymaniyah</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B283" t="inlineStr">
+      <c r="B284" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C283" t="n">
+      <c r="C284" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D283" t="n">
+      <c r="D284" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E283" t="inlineStr">
+      <c r="E284" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F283" t="inlineStr">
+      <c r="F284" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G283" t="inlineStr">
+      <c r="G284" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 0108dc57856ee14831f04d27dc1ac346b83dcced
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -2134,7 +2134,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Kaohsiung City, Taiwan</t>
+          <t>Kaohsiung City</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Taipei - Taiwan</t>
+          <t>Taipei</t>
         </is>
       </c>
       <c r="C85" t="n">

</xml_diff>

<commit_message>
update generated data Triggered by 1be9218539420386a975ce1a70bb71e254129b12
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -4405,11 +4405,27 @@
           <t>Minsk, Belarus</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr"/>
-      <c r="E134" t="inlineStr"/>
-      <c r="F134" t="inlineStr"/>
-      <c r="G134" t="inlineStr"/>
+      <c r="C134" t="n">
+        <v>53.9006</v>
+      </c>
+      <c r="D134" t="n">
+        <v>27.599</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>BY</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Minsk</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 18f3ed8784e3ec65e3e438457c59ec9fe5c06664
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G284"/>
+  <dimension ref="A1:G285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9314,64 +9314,97 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Timbo, Brazil</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>35.5668</v>
+        <v>-26.8251</v>
       </c>
       <c r="D283" t="n">
-        <v>45.4161</v>
+        <v>-49.2695</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
+          <t>ISU</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Sulaymaniyah, Iraq</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>35.5668</v>
+      </c>
+      <c r="D284" t="n">
+        <v>45.4161</v>
+      </c>
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>IQ</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Middle East</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>Sulaymaniyah</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B284" t="inlineStr">
+      <c r="B285" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C284" t="n">
+      <c r="C285" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D284" t="n">
+      <c r="D285" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E284" t="inlineStr">
+      <c r="E285" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F284" t="inlineStr">
+      <c r="F285" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G284" t="inlineStr">
+      <c r="G285" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 40318e5d5e02b60db13df2c0bba054ace7853c47
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G285"/>
+  <dimension ref="A1:G286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9410,6 +9410,39 @@
         </is>
       </c>
     </row>
+    <row r="286">
+      <c r="A286" s="1" t="inlineStr">
+        <is>
+          <t>BNA</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Nashville, United States</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>36.1245002747</v>
+      </c>
+      <c r="D286" t="n">
+        <v>-86.6781997681</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>Nashville</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by 5f72e6b4aaf3d65620fdfaf0de5ff69ae82c7ed9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -6641,19 +6641,19 @@
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-18.8836116791</v>
+        <v>-26.8251</v>
       </c>
       <c r="D202" t="n">
-        <v>-48.225276947</v>
+        <v>-49.2695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -6667,30 +6667,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>12.1888999939</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D203" t="n">
-        <v>-68.95980072019999</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6700,96 +6700,96 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>18.4297008514</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D204" t="n">
-        <v>-69.6688995361</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>31.7226009369</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D205" t="n">
-        <v>35.9931983948</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D206" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6799,30 +6799,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D207" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6832,30 +6832,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D208" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6865,30 +6865,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D209" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6898,30 +6898,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D210" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6931,30 +6931,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D211" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6964,30 +6964,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D212" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -6997,30 +6997,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D213" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7030,30 +7030,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D214" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7063,30 +7063,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D215" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7096,30 +7096,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D216" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7129,30 +7129,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D217" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7162,30 +7162,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D218" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7195,30 +7195,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D219" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7228,30 +7228,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D220" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7261,26 +7261,26 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D221" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -7294,30 +7294,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D222" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7327,30 +7327,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D223" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7360,30 +7360,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>32.0113983154</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D224" t="n">
-        <v>34.8866996765</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7393,92 +7393,92 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>38.94449997</v>
+        <v>35.5668</v>
       </c>
       <c r="D225" t="n">
-        <v>-77.45580292</v>
+        <v>45.4161</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>33.6366996765</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D226" t="n">
-        <v>-84.4281005859</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>42.36429977</v>
+        <v>38.94449997</v>
       </c>
       <c r="D227" t="n">
-        <v>-71.00520324999999</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -7492,26 +7492,26 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>42.94049835</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D228" t="n">
-        <v>-78.73220062</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -7525,30 +7525,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>51.113899231</v>
+        <v>42.36429977</v>
       </c>
       <c r="D229" t="n">
-        <v>-114.019996643</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7558,26 +7558,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>35.2140007019</v>
+        <v>42.94049835</v>
       </c>
       <c r="D230" t="n">
-        <v>-80.94309997560001</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7591,30 +7591,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>41.97859955</v>
+        <v>51.113899231</v>
       </c>
       <c r="D231" t="n">
-        <v>-87.90480042</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7624,26 +7624,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>39.9980010986</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D232" t="n">
-        <v>-82.89189910890001</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7657,26 +7657,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.8968009949</v>
+        <v>41.97859955</v>
       </c>
       <c r="D233" t="n">
-        <v>-97.0380020142</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7690,26 +7690,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>39.8616981506</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D234" t="n">
-        <v>-104.672996521</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7723,26 +7723,26 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>42.2123985291</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D235" t="n">
-        <v>-83.35340118409999</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7756,26 +7756,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>21.3187007904</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D236" t="n">
-        <v>-157.9219970703</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7789,26 +7789,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>29.9843997955</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D237" t="n">
-        <v>-95.34140014650001</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7822,26 +7822,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>39.717300415</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D238" t="n">
-        <v>-86.2944030762</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7855,26 +7855,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>30.4941005707</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D239" t="n">
-        <v>-81.68789672849999</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7888,26 +7888,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>39.2975997925</v>
+        <v>39.717300415</v>
       </c>
       <c r="D240" t="n">
-        <v>-94.7138977051</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7921,26 +7921,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>36.08010101</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D241" t="n">
-        <v>-115.1520004</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7954,26 +7954,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>33.94250107</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D242" t="n">
-        <v>-118.4079971</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -7987,26 +7987,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>26.17580032</v>
+        <v>36.08010101</v>
       </c>
       <c r="D243" t="n">
-        <v>-98.23860168</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8020,26 +8020,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>35.0424003601</v>
+        <v>33.94250107</v>
       </c>
       <c r="D244" t="n">
-        <v>-89.9766998291</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8053,30 +8053,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>19.4363002777</v>
+        <v>26.17580032</v>
       </c>
       <c r="D245" t="n">
-        <v>-99.07209777830001</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -8086,26 +8086,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>25.7931995392</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D246" t="n">
-        <v>-80.2906036377</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8119,30 +8119,30 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>44.8819999695</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D247" t="n">
-        <v>-93.22180175779999</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -8152,26 +8152,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>32.30059814</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D248" t="n">
-        <v>-86.39399718999999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8185,30 +8185,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D249" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8218,26 +8218,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>40.6925010681</v>
+        <v>32.30059814</v>
       </c>
       <c r="D250" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8251,30 +8251,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>36.8945999146</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D251" t="n">
-        <v>-76.2012023926</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8284,26 +8284,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>41.3031997681</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D252" t="n">
-        <v>-95.89409637449999</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8317,30 +8317,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>45.3224983215</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D253" t="n">
-        <v>-75.66919708250001</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8350,26 +8350,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>39.8718986511</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D254" t="n">
-        <v>-75.24109649659999</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8383,30 +8383,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>33.434299469</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D255" t="n">
-        <v>-112.012001038</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8416,26 +8416,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>40.49150085</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D256" t="n">
-        <v>-80.23290253</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8449,26 +8449,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>45.58869934</v>
+        <v>33.434299469</v>
       </c>
       <c r="D257" t="n">
-        <v>-122.5979996</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8482,30 +8482,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>20.6173000336</v>
+        <v>40.49150085</v>
       </c>
       <c r="D258" t="n">
-        <v>-100.185997009</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8515,26 +8515,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>37.5051994324</v>
+        <v>45.58869934</v>
       </c>
       <c r="D259" t="n">
-        <v>-77.3197021484</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8548,30 +8548,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>38.695400238</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D260" t="n">
-        <v>-121.591003418</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8581,26 +8581,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>40.7883987427</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D261" t="n">
-        <v>-111.977996826</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8614,26 +8614,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>32.7336006165</v>
+        <v>38.695400238</v>
       </c>
       <c r="D262" t="n">
-        <v>-117.190002441</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8647,26 +8647,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>37.3625984192</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D263" t="n">
-        <v>-121.929000855</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8680,30 +8680,30 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>52.1707992554</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D264" t="n">
-        <v>-106.699996948</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8713,26 +8713,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>47.4490013123</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D265" t="n">
-        <v>-122.308998108</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8746,30 +8746,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>38.7486991882</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D266" t="n">
-        <v>-90.37000274659999</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8779,26 +8779,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>30.3964996338</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D267" t="n">
-        <v>-84.3503036499</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8812,26 +8812,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>27.9755001068</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D268" t="n">
-        <v>-82.533203125</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8845,30 +8845,30 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D269" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8878,30 +8878,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>49.193901062</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D270" t="n">
-        <v>-123.183998108</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8911,26 +8911,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>49.9099998474</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D271" t="n">
-        <v>-97.2398986816</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8944,92 +8944,92 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>-34.9431729</v>
+        <v>49.193901062</v>
       </c>
       <c r="D272" t="n">
-        <v>138.5335637</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>-37.0080986023</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D273" t="n">
-        <v>174.792007446</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>-27.3841991425</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D274" t="n">
-        <v>153.117004394</v>
+        <v>138.5335637</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9043,30 +9043,30 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-35.3069000244</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D275" t="n">
-        <v>149.1950073242</v>
+        <v>174.792007446</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -9076,30 +9076,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-43.4893989563</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D276" t="n">
-        <v>172.5319976807</v>
+        <v>153.117004394</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9109,63 +9109,63 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D277" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-42.883209</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D278" t="n">
-        <v>147.331665</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9175,63 +9175,63 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D279" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>-22.0146007538</v>
+        <v>-42.883209</v>
       </c>
       <c r="D280" t="n">
-        <v>166.212997436</v>
+        <v>147.331665</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9241,26 +9241,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>-31.9402999878</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D281" t="n">
-        <v>115.967002869</v>
+        <v>144.843002319</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9274,30 +9274,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-33.9460983276</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D282" t="n">
-        <v>151.177001953</v>
+        <v>166.212997436</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9307,73 +9307,73 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Timbo, Brazil</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>-26.8251</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D283" t="n">
-        <v>-49.2695</v>
+        <v>115.967002869</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>35.5668</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D284" t="n">
-        <v>45.4161</v>
+        <v>151.177001953</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by a78740ad61331c508210193c126ab84bd72354c6
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G286"/>
+  <dimension ref="A1:G287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9413,31 +9413,64 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Kochi, India</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>9.9312</v>
+      </c>
+      <c r="D286" t="n">
+        <v>76.26730000000001</v>
+      </c>
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>Kochi</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B286" t="inlineStr">
+      <c r="B287" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C286" t="n">
+      <c r="C287" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D286" t="n">
+      <c r="D287" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E286" t="inlineStr">
+      <c r="E287" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F286" t="inlineStr">
+      <c r="F287" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G286" t="inlineStr">
+      <c r="G287" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by f5bddeeab77b96894a6e0b345fa267584b3298b5
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G287"/>
+  <dimension ref="A1:G288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9413,64 +9413,97 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>9.9312</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D286" t="n">
-        <v>76.26730000000001</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Kochi, India</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>9.9312</v>
+      </c>
+      <c r="D287" t="n">
+        <v>76.26730000000001</v>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>Kochi</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B287" t="inlineStr">
+      <c r="B288" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C287" t="n">
+      <c r="C288" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D287" t="n">
+      <c r="D288" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E287" t="inlineStr">
+      <c r="E288" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F287" t="inlineStr">
+      <c r="F288" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G287" t="inlineStr">
+      <c r="G288" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 7cd26f1b83fdf5bd683e6e7b74c7418c2c2efeeb
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -5197,27 +5197,11 @@
           <t>Tver, Russian Federation</t>
         </is>
       </c>
-      <c r="C158" t="n">
-        <v>56.8587</v>
-      </c>
-      <c r="D158" t="n">
-        <v>35.9176</v>
-      </c>
-      <c r="E158" t="inlineStr">
-        <is>
-          <t>RU</t>
-        </is>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>Tver</t>
-        </is>
-      </c>
+      <c r="C158" t="inlineStr"/>
+      <c r="D158" t="inlineStr"/>
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="inlineStr"/>
+      <c r="G158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by d737cfd5bb949a76cbe465a904cb2602aa6e860d
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -5197,11 +5197,27 @@
           <t>Tver, Russian Federation</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr"/>
-      <c r="D158" t="inlineStr"/>
-      <c r="E158" t="inlineStr"/>
-      <c r="F158" t="inlineStr"/>
-      <c r="G158" t="inlineStr"/>
+      <c r="C158" t="n">
+        <v>56.8587</v>
+      </c>
+      <c r="D158" t="n">
+        <v>35.9176</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>RU</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Tver</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by a6e6ebc8f3f02bd7087f178cc5689c87f6ce10e7
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G288"/>
+  <dimension ref="A1:G289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9479,31 +9479,64 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
+          <t>ADB</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Izmir, Turkey</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>38.32377</v>
+      </c>
+      <c r="D288" t="n">
+        <v>27.14317</v>
+      </c>
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>TR</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>Izmir</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="inlineStr">
+        <is>
           <t>SFO</t>
         </is>
       </c>
-      <c r="B288" t="inlineStr">
+      <c r="B289" t="inlineStr">
         <is>
           <t>San Francisco, United States</t>
         </is>
       </c>
-      <c r="C288" t="n">
+      <c r="C289" t="n">
         <v>37.6189994812</v>
       </c>
-      <c r="D288" t="n">
+      <c r="D289" t="n">
         <v>-122.375</v>
       </c>
-      <c r="E288" t="inlineStr">
+      <c r="E289" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F288" t="inlineStr">
+      <c r="F289" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G288" t="inlineStr">
+      <c r="G289" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 33c42a38479112fda6e0f9302bab9a25b28da275
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G289"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9542,6 +9542,39 @@
         </is>
       </c>
     </row>
+    <row r="290">
+      <c r="A290" s="1" t="inlineStr">
+        <is>
+          <t>FSD</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Sioux Falls, United States</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>43.546</v>
+      </c>
+      <c r="D290" t="n">
+        <v>96.7313</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>Sioux Falls</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by 880f00b24e51b9892e157c4d9757c536b9d651d1
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -9554,10 +9554,10 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>43.546</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D290" t="n">
-        <v>96.7313</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update generated data Triggered by 360e1ce8c8f7833ee8e9f01c21c459d4b23dcce1
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G290"/>
+  <dimension ref="A1:G291"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9446,130 +9446,163 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>9.9312</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D287" t="n">
-        <v>76.26730000000001</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>38.32377</v>
+        <v>9.9312</v>
       </c>
       <c r="D288" t="n">
-        <v>27.14317</v>
+        <v>76.26730000000001</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Kochi</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>37.6189994812</v>
+        <v>38.32377</v>
       </c>
       <c r="D289" t="n">
-        <v>-122.375</v>
+        <v>27.14317</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
+          <t>SFO</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>San Francisco, United States</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>37.6189994812</v>
+      </c>
+      <c r="D290" t="n">
+        <v>-122.375</v>
+      </c>
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="inlineStr">
+        <is>
           <t>FSD</t>
         </is>
       </c>
-      <c r="B290" t="inlineStr">
+      <c r="B291" t="inlineStr">
         <is>
           <t>Sioux Falls, United States</t>
         </is>
       </c>
-      <c r="C290" t="n">
+      <c r="C291" t="n">
         <v>43.540819819502</v>
       </c>
-      <c r="D290" t="n">
+      <c r="D291" t="n">
         <v>-96.65511577730963</v>
       </c>
-      <c r="E290" t="inlineStr">
+      <c r="E291" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F290" t="inlineStr">
+      <c r="F291" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G290" t="inlineStr">
+      <c r="G291" t="inlineStr">
         <is>
           <t>Sioux Falls</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by c66bb4d21ddb2721dbeb9c6d2f4fb962a792567c
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G291"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9512,97 +9512,130 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>FUK</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Fukuoka, Japan</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>38.32377</v>
+        <v>33.5902</v>
       </c>
       <c r="D289" t="n">
-        <v>27.14317</v>
+        <v>130.4017</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Fukuoka</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>37.6189994812</v>
+        <v>38.32377</v>
       </c>
       <c r="D290" t="n">
-        <v>-122.375</v>
+        <v>27.14317</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
+          <t>SFO</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>San Francisco, United States</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>37.6189994812</v>
+      </c>
+      <c r="D291" t="n">
+        <v>-122.375</v>
+      </c>
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="inlineStr">
+        <is>
           <t>FSD</t>
         </is>
       </c>
-      <c r="B291" t="inlineStr">
+      <c r="B292" t="inlineStr">
         <is>
           <t>Sioux Falls, United States</t>
         </is>
       </c>
-      <c r="C291" t="n">
+      <c r="C292" t="n">
         <v>43.540819819502</v>
       </c>
-      <c r="D291" t="n">
+      <c r="D292" t="n">
         <v>-96.65511577730963</v>
       </c>
-      <c r="E291" t="inlineStr">
+      <c r="E292" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F291" t="inlineStr">
+      <c r="F292" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G291" t="inlineStr">
+      <c r="G292" t="inlineStr">
         <is>
           <t>Sioux Falls</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by a3d01d060af19d5885e82310e5dd8d92aef0595d
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G292"/>
+  <dimension ref="A1:G293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9413,122 +9413,122 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-8.126489639300001</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D286" t="n">
-        <v>-34.9235992432</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-17.5536994934</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D287" t="n">
-        <v>-149.606994629</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Stuttgart, Germany</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>9.9312</v>
+        <v>48.783333</v>
       </c>
       <c r="D288" t="n">
-        <v>76.26730000000001</v>
+        <v>9.183332999999999</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Stuttgart</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>FUK</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Fukuoka, Japan</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>33.5902</v>
+        <v>9.9312</v>
       </c>
       <c r="D289" t="n">
-        <v>130.4017</v>
+        <v>76.26730000000001</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9538,104 +9538,137 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Fukuoka</t>
+          <t>Kochi</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>FUK</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Fukuoka, Japan</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>38.32377</v>
+        <v>33.5902</v>
       </c>
       <c r="D290" t="n">
-        <v>27.14317</v>
+        <v>130.4017</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Fukuoka</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>37.6189994812</v>
+        <v>38.32377</v>
       </c>
       <c r="D291" t="n">
-        <v>-122.375</v>
+        <v>27.14317</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
+          <t>SFO</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>San Francisco, United States</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>37.6189994812</v>
+      </c>
+      <c r="D292" t="n">
+        <v>-122.375</v>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="inlineStr">
+        <is>
           <t>FSD</t>
         </is>
       </c>
-      <c r="B292" t="inlineStr">
+      <c r="B293" t="inlineStr">
         <is>
           <t>Sioux Falls, United States</t>
         </is>
       </c>
-      <c r="C292" t="n">
+      <c r="C293" t="n">
         <v>43.540819819502</v>
       </c>
-      <c r="D292" t="n">
+      <c r="D293" t="n">
         <v>-96.65511577730963</v>
       </c>
-      <c r="E292" t="inlineStr">
+      <c r="E293" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="F292" t="inlineStr">
+      <c r="F293" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="G292" t="inlineStr">
+      <c r="G293" t="inlineStr">
         <is>
           <t>Sioux Falls</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by f95f7e07428676c911af8d63098e16a2d7e77731
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -8852,19 +8852,19 @@
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D269" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8878,26 +8878,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D270" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8911,26 +8911,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D271" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8944,30 +8944,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D272" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8977,26 +8977,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D273" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9010,26 +9010,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D274" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9043,63 +9043,63 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>-34.9431729</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D275" t="n">
-        <v>138.5335637</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D276" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9109,30 +9109,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D277" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9142,26 +9142,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D278" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9175,30 +9175,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D279" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9208,92 +9208,92 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D280" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D281" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D282" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9307,30 +9307,30 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D283" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -9340,30 +9340,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D284" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9373,26 +9373,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D285" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9406,30 +9406,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D286" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9439,129 +9439,129 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-8.126489639300001</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D287" t="n">
-        <v>-34.9235992432</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Stuttgart, Germany</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>48.783333</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D288" t="n">
-        <v>9.183332999999999</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Stuttgart, Germany</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>9.9312</v>
+        <v>48.783333</v>
       </c>
       <c r="D289" t="n">
-        <v>76.26730000000001</v>
+        <v>9.183332999999999</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Stuttgart</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>FUK</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Fukuoka, Japan</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>33.5902</v>
+        <v>9.9312</v>
       </c>
       <c r="D290" t="n">
-        <v>130.4017</v>
+        <v>76.26730000000001</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9571,92 +9571,92 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Fukuoka</t>
+          <t>Kochi</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>FUK</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Fukuoka, Japan</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>38.32377</v>
+        <v>33.5902</v>
       </c>
       <c r="D291" t="n">
-        <v>27.14317</v>
+        <v>130.4017</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Fukuoka</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>37.6189994812</v>
+        <v>38.32377</v>
       </c>
       <c r="D292" t="n">
-        <v>-122.375</v>
+        <v>27.14317</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Sioux Falls, United States</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>43.540819819502</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D293" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.375</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9670,7 +9670,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 0d6c5f68735abc767bb9eb1195c9fc09cff0cc8d
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G296"/>
+  <dimension ref="A1:G297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9332,56 +9332,56 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-34.9431729</v>
+        <v>17.9951</v>
       </c>
       <c r="D285" t="n">
-        <v>138.5335637</v>
+        <v>-76.7846</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D286" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9391,30 +9391,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D287" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9424,26 +9424,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D288" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9457,30 +9457,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D289" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9490,92 +9490,92 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D290" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D291" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D292" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9589,30 +9589,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D293" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9622,30 +9622,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D294" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9655,26 +9655,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D295" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9688,38 +9688,71 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D296" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B296" t="inlineStr">
+      <c r="B297" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C296" t="n">
+      <c r="C297" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D296" t="n">
+      <c r="D297" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E297" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F296" t="inlineStr">
+      <c r="F297" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G296" t="inlineStr">
+      <c r="G297" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 394de06088c5d216734f7ab62cf6920d6cab57ba
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G292"/>
+  <dimension ref="A1:G293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9673,6 +9673,39 @@
         </is>
       </c>
     </row>
+    <row r="293">
+      <c r="A293" s="1" t="inlineStr">
+        <is>
+          <t>VIX</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Vitoria, Brazil</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>-20.64871</v>
+      </c>
+      <c r="D293" t="n">
+        <v>-41.90857</v>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>South America</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>Vitoria</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by 70c321e1ec96990bb0acce878949b8dbb4571eee
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G293"/>
+  <dimension ref="A1:G295"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6409,19 +6409,19 @@
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Recife</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-21.1363887787</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D194" t="n">
-        <v>-47.7766685486</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -6435,26 +6435,26 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D195" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -6468,26 +6468,26 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D196" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -6501,30 +6501,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D197" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6534,30 +6534,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D198" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6567,30 +6567,30 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-20.807157</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D199" t="n">
-        <v>-49.378994</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6600,59 +6600,59 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-23.4355564117</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D200" t="n">
-        <v>-46.4730567932</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-23.54389</v>
+        <v>-20.807157</v>
       </c>
       <c r="D201" t="n">
-        <v>-46.63445</v>
+        <v>-49.378994</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -6666,30 +6666,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>12.007116</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D202" t="n">
-        <v>-61.7882288</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6699,30 +6699,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>14.0608</v>
+        <v>-23.54389</v>
       </c>
       <c r="D203" t="n">
-        <v>-87.21720000000001</v>
+        <v>-46.63445</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6732,30 +6732,30 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-26.8251</v>
+        <v>12.007116</v>
       </c>
       <c r="D204" t="n">
-        <v>-49.2695</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -6765,30 +6765,30 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-18.8836116791</v>
+        <v>14.0608</v>
       </c>
       <c r="D205" t="n">
-        <v>-48.225276947</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6798,30 +6798,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>12.1888999939</v>
+        <v>-26.8251</v>
       </c>
       <c r="D206" t="n">
-        <v>-68.95980072019999</v>
+        <v>-49.2695</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6831,59 +6831,59 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>18.4297008514</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D207" t="n">
-        <v>-69.6688995361</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-8.126489639300001</v>
+        <v>-20.64871</v>
       </c>
       <c r="D208" t="n">
-        <v>-34.9235992432</v>
+        <v>-41.90857</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -6897,63 +6897,63 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>31.7226009369</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D209" t="n">
-        <v>35.9931983948</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D210" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6963,30 +6963,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D211" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6996,30 +6996,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D212" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -7029,30 +7029,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D213" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7062,30 +7062,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D214" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7095,30 +7095,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D215" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7128,30 +7128,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D216" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7161,30 +7161,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D217" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7194,30 +7194,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D218" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7227,30 +7227,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D219" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7260,30 +7260,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D220" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7293,30 +7293,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D221" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7326,30 +7326,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D222" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7359,30 +7359,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D223" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7392,30 +7392,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D224" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7425,26 +7425,26 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D225" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -7458,30 +7458,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D226" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7491,30 +7491,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D227" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7524,30 +7524,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D228" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7557,30 +7557,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D229" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7590,59 +7590,59 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D230" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D231" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7656,26 +7656,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D232" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7689,26 +7689,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D233" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7722,30 +7722,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D234" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7755,30 +7755,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D235" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7788,26 +7788,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D236" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7821,26 +7821,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D237" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7854,26 +7854,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D238" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7887,26 +7887,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D239" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7920,26 +7920,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D240" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7953,26 +7953,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D241" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7986,26 +7986,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D242" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8019,26 +8019,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D243" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8052,26 +8052,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D244" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8085,26 +8085,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D245" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8118,26 +8118,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D246" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8151,26 +8151,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D247" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8184,26 +8184,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D248" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8217,26 +8217,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D249" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8250,30 +8250,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D250" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8283,30 +8283,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D251" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8316,26 +8316,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D252" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8349,26 +8349,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D253" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8382,30 +8382,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D254" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8415,30 +8415,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D255" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8448,26 +8448,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D256" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8481,26 +8481,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D257" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8514,26 +8514,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D258" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8547,30 +8547,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D259" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8580,30 +8580,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D260" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8613,26 +8613,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D261" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8646,26 +8646,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D262" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8679,26 +8679,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D263" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8712,30 +8712,30 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D264" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8745,30 +8745,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D265" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8778,26 +8778,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D266" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8811,26 +8811,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D267" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8844,26 +8844,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D268" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8877,26 +8877,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D269" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8910,30 +8910,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D270" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8943,30 +8943,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D271" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8976,26 +8976,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D272" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9009,26 +9009,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D273" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9042,26 +9042,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D274" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9075,26 +9075,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D275" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9108,30 +9108,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D276" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9141,26 +9141,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D277" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9174,26 +9174,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D278" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9207,30 +9207,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D279" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9240,30 +9240,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D280" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9273,63 +9273,63 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>-34.9431729</v>
+        <v>17.9951</v>
       </c>
       <c r="D281" t="n">
-        <v>138.5335637</v>
+        <v>-76.7846</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D282" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9339,30 +9339,30 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D283" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -9372,26 +9372,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D284" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9405,30 +9405,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D285" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9438,92 +9438,92 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D286" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D287" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D288" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9537,30 +9537,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D289" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9570,30 +9570,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D290" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9603,26 +9603,26 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D291" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -9636,30 +9636,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D292" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9669,40 +9669,106 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-20.64871</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D293" t="n">
-        <v>-41.90857</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="inlineStr">
+        <is>
+          <t>SJK</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>São José dos Campos, Brazil</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>-23.1791</v>
+      </c>
+      <c r="D294" t="n">
+        <v>-45.8872</v>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
           <t>BR</t>
         </is>
       </c>
-      <c r="F293" t="inlineStr">
+      <c r="F294" t="inlineStr">
         <is>
           <t>South America</t>
         </is>
       </c>
-      <c r="G293" t="inlineStr">
-        <is>
-          <t>Vitoria</t>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>São José dos Campos</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="inlineStr">
+        <is>
+          <t>BGR</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Bangor, United States</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>44.8081</v>
+      </c>
+      <c r="D295" t="n">
+        <v>-68.795</v>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>Bangor</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by e9e65562d5399db77c7649c276e110c419948e24
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -6937,56 +6937,56 @@
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>31.7226009369</v>
+        <v>-23.1791</v>
       </c>
       <c r="D210" t="n">
-        <v>35.9931983948</v>
+        <v>-45.8872</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D211" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6996,30 +6996,30 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D212" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -7029,30 +7029,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D213" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7062,30 +7062,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D214" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7095,30 +7095,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D215" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7128,30 +7128,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D216" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7161,30 +7161,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D217" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7194,30 +7194,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D218" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7227,30 +7227,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D219" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7260,30 +7260,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D220" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7293,30 +7293,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D221" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7326,30 +7326,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D222" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7359,30 +7359,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D223" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7392,30 +7392,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D224" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7425,30 +7425,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D225" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7458,26 +7458,26 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D226" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -7491,30 +7491,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D227" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7524,30 +7524,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D228" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7557,30 +7557,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D229" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7590,30 +7590,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D230" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7623,59 +7623,59 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D231" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D232" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7689,26 +7689,26 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D233" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -7722,26 +7722,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D234" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7755,30 +7755,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D235" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7788,30 +7788,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D236" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7821,26 +7821,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D237" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7854,26 +7854,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D238" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7887,26 +7887,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D239" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7920,26 +7920,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D240" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7953,26 +7953,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D241" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7986,26 +7986,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D242" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8019,26 +8019,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D243" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8052,26 +8052,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D244" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8085,26 +8085,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D245" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8118,26 +8118,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D246" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8151,26 +8151,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D247" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8184,26 +8184,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D248" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8217,26 +8217,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D249" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8250,26 +8250,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D250" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8283,30 +8283,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D251" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8316,30 +8316,30 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D252" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8349,26 +8349,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D253" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8382,26 +8382,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D254" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8415,30 +8415,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D255" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8448,30 +8448,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D256" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8481,26 +8481,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D257" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8514,26 +8514,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D258" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8547,26 +8547,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D259" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8580,30 +8580,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D260" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8613,30 +8613,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D261" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8646,26 +8646,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D262" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8679,26 +8679,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D263" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8712,26 +8712,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D264" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8745,30 +8745,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D265" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8778,30 +8778,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D266" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8811,26 +8811,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D267" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8844,26 +8844,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D268" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8877,26 +8877,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D269" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8910,26 +8910,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D270" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8943,30 +8943,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D271" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8976,30 +8976,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D272" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -9009,26 +9009,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D273" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9042,26 +9042,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D274" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9075,26 +9075,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D275" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9108,26 +9108,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D276" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9141,30 +9141,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D277" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9174,26 +9174,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D278" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9207,26 +9207,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D279" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9240,30 +9240,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D280" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9273,30 +9273,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D281" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9306,92 +9306,92 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>-34.9431729</v>
+        <v>17.9951</v>
       </c>
       <c r="D282" t="n">
-        <v>138.5335637</v>
+        <v>-76.7846</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>-37.0080986023</v>
+        <v>44.8081</v>
       </c>
       <c r="D283" t="n">
-        <v>174.792007446</v>
+        <v>-68.795</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>-27.3841991425</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D284" t="n">
-        <v>153.117004394</v>
+        <v>138.5335637</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9405,30 +9405,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-35.3069000244</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D285" t="n">
-        <v>149.1950073242</v>
+        <v>174.792007446</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9438,30 +9438,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-43.4893989563</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D286" t="n">
-        <v>172.5319976807</v>
+        <v>153.117004394</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9471,63 +9471,63 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D287" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-42.883209</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D288" t="n">
-        <v>147.331665</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9537,63 +9537,63 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D289" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-22.0146007538</v>
+        <v>-42.883209</v>
       </c>
       <c r="D290" t="n">
-        <v>166.212997436</v>
+        <v>147.331665</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9603,26 +9603,26 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-31.9402999878</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D291" t="n">
-        <v>115.967002869</v>
+        <v>144.843002319</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -9636,30 +9636,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-33.9460983276</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D292" t="n">
-        <v>151.177001953</v>
+        <v>166.212997436</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9669,30 +9669,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-17.5536994934</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D293" t="n">
-        <v>-149.606994629</v>
+        <v>115.967002869</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9702,73 +9702,73 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-23.1791</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D294" t="n">
-        <v>-45.8872</v>
+        <v>151.177001953</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>44.8081</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D295" t="n">
-        <v>-68.795</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by ae12eaf4354f1f0a2a93175628264c4871410e80
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -6706,19 +6706,19 @@
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.1791</v>
       </c>
       <c r="D203" t="n">
-        <v>-46.4730567932</v>
+        <v>-45.8872</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -6732,26 +6732,26 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D204" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -6765,30 +6765,30 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D205" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -6798,30 +6798,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D206" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6831,30 +6831,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-26.8251</v>
+        <v>14.0608</v>
       </c>
       <c r="D207" t="n">
-        <v>-49.2695</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6864,26 +6864,26 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-18.8836116791</v>
+        <v>-26.8251</v>
       </c>
       <c r="D208" t="n">
-        <v>-48.225276947</v>
+        <v>-49.2695</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -6897,26 +6897,26 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>-20.64871</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D209" t="n">
-        <v>-41.90857</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -6930,30 +6930,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>12.1888999939</v>
+        <v>-20.64871</v>
       </c>
       <c r="D210" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.90857</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6963,30 +6963,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-23.1791</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D211" t="n">
-        <v>-45.8872</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -6996,7 +6996,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
@@ -7762,19 +7762,19 @@
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>42.36429977</v>
+        <v>44.8081</v>
       </c>
       <c r="D235" t="n">
-        <v>-71.00520324999999</v>
+        <v>-68.795</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -7788,26 +7788,26 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D236" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7821,30 +7821,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D237" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7854,30 +7854,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D238" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7887,26 +7887,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D239" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7920,26 +7920,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D240" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7953,26 +7953,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D241" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7986,26 +7986,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D242" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8019,26 +8019,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D243" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8052,26 +8052,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D244" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8085,26 +8085,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D245" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8118,26 +8118,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D246" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8151,26 +8151,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D247" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8184,26 +8184,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D248" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8217,26 +8217,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D249" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8250,26 +8250,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D250" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8283,26 +8283,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D251" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8316,26 +8316,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D252" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8349,30 +8349,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D253" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8382,30 +8382,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D254" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8415,26 +8415,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D255" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8448,26 +8448,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D256" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8481,30 +8481,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D257" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8514,30 +8514,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D258" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8547,26 +8547,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D259" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8580,26 +8580,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D260" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8613,26 +8613,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D261" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8646,30 +8646,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D262" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8679,30 +8679,30 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D263" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8712,26 +8712,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D264" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8745,26 +8745,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D265" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8778,26 +8778,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D266" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8811,30 +8811,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D267" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8844,30 +8844,30 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D268" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8877,26 +8877,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D269" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8910,26 +8910,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D270" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8943,26 +8943,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D271" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8976,26 +8976,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D272" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9009,30 +9009,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D273" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -9042,30 +9042,30 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D274" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -9075,26 +9075,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D275" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9108,26 +9108,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D276" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9141,26 +9141,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D277" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9174,26 +9174,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D278" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9207,30 +9207,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D279" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9240,26 +9240,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D280" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9273,26 +9273,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D281" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9306,30 +9306,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D282" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9339,30 +9339,30 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D283" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -9372,30 +9372,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D284" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9405,7 +9405,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 57f86d16d215368b8e50e8d9ee7cb761345cde96
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G296"/>
+  <dimension ref="A1:G297"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9412,56 +9412,56 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>-34.9431729</v>
+        <v>30.1975</v>
       </c>
       <c r="D285" t="n">
-        <v>138.5335637</v>
+        <v>-97.6664</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D286" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9471,30 +9471,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D287" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9504,26 +9504,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D288" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9537,30 +9537,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D289" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9570,92 +9570,92 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D290" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D291" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D292" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9669,30 +9669,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D293" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9702,30 +9702,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D294" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9735,26 +9735,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D295" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9768,38 +9768,71 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D296" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B296" t="inlineStr">
+      <c r="B297" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C296" t="n">
+      <c r="C297" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D296" t="n">
+      <c r="D297" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E296" t="inlineStr">
+      <c r="E297" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F296" t="inlineStr">
+      <c r="F297" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G296" t="inlineStr">
+      <c r="G297" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by a23c51b4ee599df7cfe45a034cefc0298bc645c5
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G297"/>
+  <dimension ref="A1:G298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9445,56 +9445,56 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>-34.9431729</v>
+        <v>35.0844</v>
       </c>
       <c r="D286" t="n">
-        <v>138.5335637</v>
+        <v>-106.6504</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D287" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9504,30 +9504,30 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D288" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9537,26 +9537,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D289" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9570,30 +9570,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D290" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9603,92 +9603,92 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D291" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D292" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D293" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9702,30 +9702,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D294" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9735,30 +9735,30 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D295" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -9768,26 +9768,26 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D296" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9801,38 +9801,71 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D297" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B297" t="inlineStr">
+      <c r="B298" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C297" t="n">
+      <c r="C298" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D297" t="n">
+      <c r="D298" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E297" t="inlineStr">
+      <c r="E298" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F297" t="inlineStr">
+      <c r="F298" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G297" t="inlineStr">
+      <c r="G298" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by bfbc98ffad27ff4b2ea52e71fd11d7b0ac8b35fd
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G300"/>
+  <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7053,56 +7053,56 @@
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>31.7226009369</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D214" t="n">
-        <v>35.9931983948</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D215" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7112,30 +7112,30 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D216" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7145,30 +7145,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D217" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7178,30 +7178,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D218" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7211,30 +7211,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D219" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7244,30 +7244,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D220" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7277,30 +7277,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D221" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7310,30 +7310,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D222" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7343,30 +7343,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D223" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7376,30 +7376,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D224" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7409,30 +7409,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D225" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7442,30 +7442,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D226" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7475,30 +7475,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D227" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7508,30 +7508,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D228" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7541,30 +7541,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D229" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7574,26 +7574,26 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D230" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -7607,30 +7607,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D231" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7640,30 +7640,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D232" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7673,30 +7673,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D233" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7706,30 +7706,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D234" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7739,59 +7739,59 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>35.0844</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D235" t="n">
-        <v>-106.6504</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>38.94449997</v>
+        <v>35.0844</v>
       </c>
       <c r="D236" t="n">
-        <v>-77.45580292</v>
+        <v>-106.6504</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -7805,26 +7805,26 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D237" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7838,26 +7838,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>44.8081</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D238" t="n">
-        <v>-68.795</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7871,26 +7871,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.36429977</v>
+        <v>44.8081</v>
       </c>
       <c r="D239" t="n">
-        <v>-71.00520324999999</v>
+        <v>-68.795</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7904,26 +7904,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D240" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7937,30 +7937,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D241" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7970,30 +7970,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D242" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -8003,26 +8003,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D243" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8036,26 +8036,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D244" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8069,26 +8069,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D245" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8102,26 +8102,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D246" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8135,26 +8135,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D247" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8168,26 +8168,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D248" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8201,26 +8201,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D249" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8234,26 +8234,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D250" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8267,26 +8267,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D251" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8300,26 +8300,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D252" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8333,26 +8333,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D253" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8366,26 +8366,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D254" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8399,26 +8399,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D255" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8432,26 +8432,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D256" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8465,30 +8465,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D257" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8498,30 +8498,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D258" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8531,26 +8531,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D259" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8564,26 +8564,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D260" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8597,30 +8597,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D261" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8630,30 +8630,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D262" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8663,26 +8663,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D263" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8696,26 +8696,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D264" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8729,26 +8729,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D265" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8762,30 +8762,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8795,30 +8795,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8828,26 +8828,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D268" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8861,26 +8861,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D269" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8894,26 +8894,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D270" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8927,30 +8927,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D271" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8960,30 +8960,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D272" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8993,26 +8993,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D273" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9026,26 +9026,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D274" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9059,26 +9059,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D275" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9092,26 +9092,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D276" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9125,30 +9125,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D277" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9158,30 +9158,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D278" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9191,26 +9191,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D279" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9224,26 +9224,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D280" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9257,26 +9257,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D281" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9290,26 +9290,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D282" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9323,30 +9323,30 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D283" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -9356,26 +9356,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D284" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9389,26 +9389,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D285" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9422,30 +9422,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D286" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9455,30 +9455,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D287" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9488,30 +9488,30 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>30.1975</v>
+        <v>17.9951</v>
       </c>
       <c r="D288" t="n">
-        <v>-97.6664</v>
+        <v>-76.7846</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9521,63 +9521,63 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>-34.9431729</v>
+        <v>30.1975</v>
       </c>
       <c r="D289" t="n">
-        <v>138.5335637</v>
+        <v>-97.6664</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D290" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9587,30 +9587,30 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D291" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9620,26 +9620,26 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D292" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9653,30 +9653,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D293" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9686,92 +9686,92 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D294" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D295" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D296" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9785,30 +9785,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D297" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9818,30 +9818,30 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D298" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9851,26 +9851,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D299" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9884,38 +9884,71 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D300" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B300" t="inlineStr">
+      <c r="B301" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C300" t="n">
+      <c r="C301" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D300" t="n">
+      <c r="D301" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E300" t="inlineStr">
+      <c r="E301" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F300" t="inlineStr">
+      <c r="F301" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G300" t="inlineStr">
+      <c r="G301" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 59d685ae19118083ce48ef760f1ab9a21b663095
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G301"/>
+  <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5403,56 +5403,56 @@
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>-22.738</v>
+        <v>45.7263</v>
       </c>
       <c r="D164" t="n">
-        <v>-47.334</v>
+        <v>5.0908</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Lyon</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-18.348611</v>
+        <v>-22.738</v>
       </c>
       <c r="D165" t="n">
-        <v>-70.33888899999999</v>
+        <v>-47.334</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5462,30 +5462,30 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-25.2399997711</v>
+        <v>-18.348611</v>
       </c>
       <c r="D166" t="n">
-        <v>-57.5200004578</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -5495,30 +5495,30 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-1.4563</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="D167" t="n">
-        <v>-48.5013</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5528,26 +5528,26 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-19.624444</v>
+        <v>-1.4563</v>
       </c>
       <c r="D168" t="n">
-        <v>-43.971944</v>
+        <v>-48.5013</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -5561,26 +5561,26 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-26.89245</v>
+        <v>-19.624444</v>
       </c>
       <c r="D169" t="n">
-        <v>-49.07696</v>
+        <v>-43.971944</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -5594,30 +5594,30 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>4.70159</v>
+        <v>-26.89245</v>
       </c>
       <c r="D170" t="n">
-        <v>-74.1469</v>
+        <v>-49.07696</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5627,30 +5627,30 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-15.79824</v>
+        <v>4.70159</v>
       </c>
       <c r="D171" t="n">
-        <v>-47.90859</v>
+        <v>-74.1469</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -5660,30 +5660,30 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-34.8222</v>
+        <v>-15.79824</v>
       </c>
       <c r="D172" t="n">
-        <v>-58.5358</v>
+        <v>-47.90859</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5693,30 +5693,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-26.7762</v>
+        <v>-34.8222</v>
       </c>
       <c r="D173" t="n">
-        <v>-51.0125</v>
+        <v>-58.5358</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5726,26 +5726,26 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-22.90662</v>
+        <v>-26.7762</v>
       </c>
       <c r="D174" t="n">
-        <v>-47.08576</v>
+        <v>-51.0125</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -5759,30 +5759,30 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>CCP</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Concepción, Chile</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-36.8201</v>
+        <v>-22.90662</v>
       </c>
       <c r="D175" t="n">
-        <v>-73.0444</v>
+        <v>-47.08576</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5792,30 +5792,30 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Concepción</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CCP</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Concepción, Chile</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-31.31</v>
+        <v>-36.8201</v>
       </c>
       <c r="D176" t="n">
-        <v>-64.208333</v>
+        <v>-73.0444</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -5825,30 +5825,30 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Concepción</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-15.59611</v>
+        <v>-31.31</v>
       </c>
       <c r="D177" t="n">
-        <v>-56.09667</v>
+        <v>-64.208333</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5858,26 +5858,26 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-25.5284996033</v>
+        <v>-15.59611</v>
       </c>
       <c r="D178" t="n">
-        <v>-49.1758003235</v>
+        <v>-56.09667</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -5891,26 +5891,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D179" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5924,26 +5924,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D180" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5957,30 +5957,30 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D181" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -5990,30 +5990,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D182" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -6023,96 +6023,96 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D183" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D184" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D185" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -6122,26 +6122,26 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D186" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -6155,26 +6155,26 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D187" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -6188,30 +6188,30 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D188" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6221,30 +6221,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D189" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6254,30 +6254,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D190" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6287,30 +6287,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D191" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6320,30 +6320,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D192" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6353,30 +6353,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D193" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6386,30 +6386,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D194" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6419,96 +6419,96 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>18.5799999237</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D195" t="n">
-        <v>-72.2925033569</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Port-Au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.1291666667</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D196" t="n">
-        <v>-78.3575</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-8.126489639300001</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D197" t="n">
-        <v>-34.9235992432</v>
+        <v>-78.3575</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6518,26 +6518,26 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Recife</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-21.1363887787</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D198" t="n">
-        <v>-47.7766685486</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -6551,26 +6551,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D199" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6584,26 +6584,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D200" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6617,30 +6617,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D201" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6650,30 +6650,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D202" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6683,92 +6683,92 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>18.4297008514</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D203" t="n">
-        <v>-69.6688995361</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-20.807157</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D204" t="n">
-        <v>-49.378994</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-23.1791</v>
+        <v>-20.807157</v>
       </c>
       <c r="D205" t="n">
-        <v>-45.8872</v>
+        <v>-49.378994</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6782,26 +6782,26 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.1791</v>
       </c>
       <c r="D206" t="n">
-        <v>-46.4730567932</v>
+        <v>-45.8872</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6815,26 +6815,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D207" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6848,30 +6848,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D208" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6881,30 +6881,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D209" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6914,30 +6914,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>-26.8251</v>
+        <v>14.0608</v>
       </c>
       <c r="D210" t="n">
-        <v>-49.2695</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6947,26 +6947,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-18.8836116791</v>
+        <v>-26.8251</v>
       </c>
       <c r="D211" t="n">
-        <v>-48.225276947</v>
+        <v>-49.2695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -6980,26 +6980,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-20.64871</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D212" t="n">
-        <v>-41.90857</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7013,30 +7013,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>12.1888999939</v>
+        <v>-20.64871</v>
       </c>
       <c r="D213" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.90857</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7046,30 +7046,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-21.698299408</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D214" t="n">
-        <v>-41.301700592</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7079,63 +7079,63 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>31.7226009369</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D215" t="n">
-        <v>35.9931983948</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D216" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7145,30 +7145,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D217" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7178,30 +7178,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D218" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7211,30 +7211,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D219" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7244,30 +7244,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D220" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7277,30 +7277,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D221" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7310,30 +7310,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D222" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7343,30 +7343,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D223" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7376,30 +7376,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D224" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7409,30 +7409,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D225" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7442,30 +7442,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D226" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7475,30 +7475,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D227" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7508,30 +7508,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D228" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7541,30 +7541,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D229" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7574,30 +7574,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D230" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7607,26 +7607,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D231" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7640,30 +7640,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D232" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7673,30 +7673,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D233" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7706,30 +7706,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D234" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7739,30 +7739,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D235" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7772,59 +7772,59 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>35.0844</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D236" t="n">
-        <v>-106.6504</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38.94449997</v>
+        <v>35.0844</v>
       </c>
       <c r="D237" t="n">
-        <v>-77.45580292</v>
+        <v>-106.6504</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7838,26 +7838,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D238" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7871,26 +7871,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>44.8081</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D239" t="n">
-        <v>-68.795</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7904,26 +7904,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.36429977</v>
+        <v>44.8081</v>
       </c>
       <c r="D240" t="n">
-        <v>-71.00520324999999</v>
+        <v>-68.795</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7937,26 +7937,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D241" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7970,30 +7970,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D242" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -8003,30 +8003,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D243" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -8036,26 +8036,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D244" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8069,26 +8069,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D245" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8102,26 +8102,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D246" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8135,26 +8135,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D247" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8168,26 +8168,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D248" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8201,26 +8201,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D249" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8234,26 +8234,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D250" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8267,26 +8267,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D251" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8300,26 +8300,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D252" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8333,26 +8333,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D253" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8366,26 +8366,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D254" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8399,26 +8399,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D255" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8432,26 +8432,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D256" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8465,26 +8465,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D257" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8498,30 +8498,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D258" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8531,30 +8531,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D259" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8564,26 +8564,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D260" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8597,26 +8597,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D261" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8630,30 +8630,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D262" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8663,30 +8663,30 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D263" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8696,26 +8696,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D264" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8729,26 +8729,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D265" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8762,26 +8762,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D266" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8795,30 +8795,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8828,30 +8828,30 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D268" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8861,26 +8861,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D269" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8894,26 +8894,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D270" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8927,26 +8927,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D271" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8960,30 +8960,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D272" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8993,30 +8993,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D273" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -9026,26 +9026,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D274" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9059,26 +9059,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D275" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9092,26 +9092,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D276" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9125,26 +9125,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D277" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9158,30 +9158,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D278" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9191,30 +9191,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D279" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9224,26 +9224,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D280" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9257,26 +9257,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D281" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9290,26 +9290,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D282" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9323,26 +9323,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>27.9755001068</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D283" t="n">
-        <v>-82.533203125</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9356,30 +9356,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>43.6772003174</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D284" t="n">
-        <v>-79.63059997560001</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9389,26 +9389,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D285" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9422,26 +9422,26 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D286" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -9455,30 +9455,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D287" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9488,30 +9488,30 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D288" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9521,30 +9521,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>30.1975</v>
+        <v>17.9951</v>
       </c>
       <c r="D289" t="n">
-        <v>-97.6664</v>
+        <v>-76.7846</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9554,63 +9554,63 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-34.9431729</v>
+        <v>30.1975</v>
       </c>
       <c r="D290" t="n">
-        <v>138.5335637</v>
+        <v>-97.6664</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D291" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9620,30 +9620,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D292" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9653,26 +9653,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D293" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9686,30 +9686,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D294" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9719,92 +9719,92 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D295" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D296" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D297" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9818,30 +9818,30 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D298" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9851,30 +9851,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D299" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9884,26 +9884,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D300" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9917,38 +9917,71 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D301" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B301" t="inlineStr">
+      <c r="B302" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C301" t="n">
+      <c r="C302" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D301" t="n">
+      <c r="D302" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E301" t="inlineStr">
+      <c r="E302" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F301" t="inlineStr">
+      <c r="F302" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G301" t="inlineStr">
+      <c r="G302" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 7fadb40c51a0922127993f0d79ec31a6cdcdc555
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G304"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9627,56 +9627,56 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-34.9431729</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D292" t="n">
-        <v>138.5335637</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D293" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9686,30 +9686,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D294" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9719,26 +9719,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D295" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9752,30 +9752,30 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D296" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9785,92 +9785,92 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D297" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D298" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D299" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9884,30 +9884,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D300" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9917,30 +9917,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D301" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9950,26 +9950,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D302" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9983,38 +9983,71 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D303" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B303" t="inlineStr">
+      <c r="B304" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C303" t="n">
+      <c r="C304" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D303" t="n">
+      <c r="D304" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E303" t="inlineStr">
+      <c r="E304" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F303" t="inlineStr">
+      <c r="F304" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G303" t="inlineStr">
+      <c r="G304" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by addf7fd8112528e11dba4f68f90ede7af125a85e
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -9470,27 +9470,11 @@
           <t>Tampa, FL, United States</t>
         </is>
       </c>
-      <c r="C287" t="n">
-        <v>27.9755001068</v>
-      </c>
-      <c r="D287" t="n">
-        <v>-82.533203125</v>
-      </c>
-      <c r="E287" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="F287" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="G287" t="inlineStr">
-        <is>
-          <t>Tampa</t>
-        </is>
-      </c>
+      <c r="C287" t="inlineStr"/>
+      <c r="D287" t="inlineStr"/>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+      <c r="G287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 95ef21852a22933be696ef2a0a066e975b6f6fe1
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -539,23 +539,23 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>TNR</t>
+          <t>AAE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Antananarivo, Madagascar</t>
+          <t>Annaba, Algeria</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-18.91368</v>
+        <v>36.85596</v>
       </c>
       <c r="D4" t="n">
-        <v>47.53613</v>
+        <v>7.79207</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>DZ</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -565,30 +565,30 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Antananarivo</t>
+          <t>Annaba</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>CPT</t>
+          <t>TNR</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cape Town, South Africa</t>
+          <t>Antananarivo, Madagascar</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-33.9648017883</v>
+        <v>-18.91368</v>
       </c>
       <c r="D5" t="n">
-        <v>18.6016998291</v>
+        <v>47.53613</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -598,30 +598,30 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cape Town</t>
+          <t>Antananarivo</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>CMN</t>
+          <t>CPT</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Casablanca, Morocco</t>
+          <t>Cape Town, South Africa</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>33.3675003052</v>
+        <v>-33.9648017883</v>
       </c>
       <c r="D6" t="n">
-        <v>-7.5899701118</v>
+        <v>18.6016998291</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -631,30 +631,30 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Casablanca</t>
+          <t>Cape Town</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>DKR</t>
+          <t>CMN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dakar, Senegal</t>
+          <t>Casablanca, Morocco</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14.7412099</v>
+        <v>33.3675003052</v>
       </c>
       <c r="D7" t="n">
-        <v>-17.4889771</v>
+        <v>-7.5899701118</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>SN</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -664,30 +664,30 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Dakar</t>
+          <t>Casablanca</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>DAR</t>
+          <t>DKR</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dar Es Salaam, Tanzania</t>
+          <t>Dakar, Senegal</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-6.8781099319</v>
+        <v>14.7412099</v>
       </c>
       <c r="D8" t="n">
-        <v>39.2025985718</v>
+        <v>-17.4889771</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TZ</t>
+          <t>SN</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -697,30 +697,30 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Dar es Salaam</t>
+          <t>Dakar</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>JIB</t>
+          <t>DAR</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Djibouti City, Djibouti</t>
+          <t>Dar Es Salaam, Tanzania</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11.5473003387</v>
+        <v>-6.8781099319</v>
       </c>
       <c r="D9" t="n">
-        <v>43.1595001221</v>
+        <v>39.2025985718</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DJ</t>
+          <t>TZ</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -730,30 +730,30 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Djibouti</t>
+          <t>Dar es Salaam</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>DUR</t>
+          <t>JIB</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Durban, South Africa</t>
+          <t>Djibouti City, Djibouti</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-29.6144444444</v>
+        <v>11.5473003387</v>
       </c>
       <c r="D10" t="n">
-        <v>31.1197222222</v>
+        <v>43.1595001221</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>DJ</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -763,30 +763,30 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Durban</t>
+          <t>Djibouti</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>GBE</t>
+          <t>DUR</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gaborone, Botswana</t>
+          <t>Durban, South Africa</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-24.6282</v>
+        <v>-29.6144444444</v>
       </c>
       <c r="D11" t="n">
-        <v>25.9231</v>
+        <v>31.1197222222</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>BW</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -796,30 +796,30 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Gaborone</t>
+          <t>Durban</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>HRE</t>
+          <t>GBE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Harare, Zimbabwe</t>
+          <t>Gaborone, Botswana</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-17.9318008423</v>
+        <v>-24.6282</v>
       </c>
       <c r="D12" t="n">
-        <v>31.0928001404</v>
+        <v>25.9231</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ZW</t>
+          <t>BW</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -829,30 +829,30 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Harare</t>
+          <t>Gaborone</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>JNB</t>
+          <t>HRE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Johannesburg, South Africa</t>
+          <t>Harare, Zimbabwe</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-26.133333</v>
+        <v>-17.9318008423</v>
       </c>
       <c r="D13" t="n">
-        <v>28.25</v>
+        <v>31.0928001404</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>ZW</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -862,30 +862,30 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Johannesburg</t>
+          <t>Harare</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>KGL</t>
+          <t>JNB</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kigali, Rwanda</t>
+          <t>Johannesburg, South Africa</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-1.9686299563</v>
+        <v>-26.133333</v>
       </c>
       <c r="D14" t="n">
-        <v>30.1394996643</v>
+        <v>28.25</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RW</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -895,30 +895,30 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Kigali</t>
+          <t>Johannesburg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>LOS</t>
+          <t>KGL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lagos, Nigeria</t>
+          <t>Kigali, Rwanda</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6.5773701668</v>
+        <v>-1.9686299563</v>
       </c>
       <c r="D15" t="n">
-        <v>3.321160078</v>
+        <v>30.1394996643</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NG</t>
+          <t>RW</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -928,30 +928,30 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Lagos</t>
+          <t>Kigali</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>LAD</t>
+          <t>LOS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Luanda, Angola</t>
+          <t>Lagos, Nigeria</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-8.858369827300001</v>
+        <v>6.5773701668</v>
       </c>
       <c r="D16" t="n">
-        <v>13.2312002182</v>
+        <v>3.321160078</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AO</t>
+          <t>NG</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -961,30 +961,30 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Luanda</t>
+          <t>Lagos</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>MPM</t>
+          <t>LAD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Maputo, Mozambique</t>
+          <t>Luanda, Angola</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-25.9207992554</v>
+        <v>-8.858369827300001</v>
       </c>
       <c r="D17" t="n">
-        <v>32.5726013184</v>
+        <v>13.2312002182</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>MZ</t>
+          <t>AO</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -994,30 +994,30 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Maputo</t>
+          <t>Luanda</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>MBA</t>
+          <t>MPM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mombasa, Kenya</t>
+          <t>Maputo, Mozambique</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-4.0348300934</v>
+        <v>-25.9207992554</v>
       </c>
       <c r="D18" t="n">
-        <v>39.5942001343</v>
+        <v>32.5726013184</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>KE</t>
+          <t>MZ</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1027,26 +1027,26 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Mombasa</t>
+          <t>Maputo</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>NBO</t>
+          <t>MBA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Nairobi, Kenya</t>
+          <t>Mombasa, Kenya</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-1.319239974</v>
+        <v>-4.0348300934</v>
       </c>
       <c r="D19" t="n">
-        <v>36.9277992249</v>
+        <v>39.5942001343</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1060,30 +1060,30 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Nairobi</t>
+          <t>Mombasa</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>OUA</t>
+          <t>NBO</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ouagadougou, Burkina Faso</t>
+          <t>Nairobi, Kenya</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>12.3531999588</v>
+        <v>-1.319239974</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.5124200583</v>
+        <v>36.9277992249</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>BF</t>
+          <t>KE</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1093,30 +1093,30 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Ouagadougou</t>
+          <t>Nairobi</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>MRU</t>
+          <t>ORN</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Port Louis, Mauritius</t>
+          <t>Oran, Algeria</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-20.4302005768</v>
+        <v>35.6911</v>
       </c>
       <c r="D21" t="n">
-        <v>57.6836013794</v>
+        <v>-0.6415999999999999</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>MU</t>
+          <t>DZ</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1126,30 +1126,30 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Port Louis</t>
+          <t>Oran</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>RUN</t>
+          <t>OUA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Réunion, France</t>
+          <t>Ouagadougou, Burkina Faso</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-20.8871002197</v>
+        <v>12.3531999588</v>
       </c>
       <c r="D22" t="n">
-        <v>55.5102996826</v>
+        <v>-1.5124200583</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RE</t>
+          <t>BF</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1159,30 +1159,30 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Saint-Denis</t>
+          <t>Ouagadougou</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>MRU</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tunis, Tunisia</t>
+          <t>Port Louis, Mauritius</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>36.8510017395</v>
+        <v>-20.4302005768</v>
       </c>
       <c r="D23" t="n">
-        <v>10.2271995544</v>
+        <v>57.6836013794</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>MU</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1192,30 +1192,30 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Tunis</t>
+          <t>Port Louis</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>FIH</t>
+          <t>RUN</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kinshasa, DR Congo</t>
+          <t>Réunion, France</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-4.3857498169</v>
+        <v>-20.8871002197</v>
       </c>
       <c r="D24" t="n">
-        <v>15.4446001053</v>
+        <v>55.5102996826</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>RE</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1225,30 +1225,30 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Kinshasa</t>
+          <t>Saint-Denis</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>ORN</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Oran, Algeria</t>
+          <t>Tunis, Tunisia</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>35.6911</v>
+        <v>36.8510017395</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.6415999999999999</v>
+        <v>10.2271995544</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DZ</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1258,30 +1258,30 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Oran</t>
+          <t>Tunis</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>AAE</t>
+          <t>FIH</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Annaba, Algeria</t>
+          <t>Kinshasa, DR Congo</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>36.85596</v>
+        <v>-4.3857498169</v>
       </c>
       <c r="D26" t="n">
-        <v>7.79207</v>
+        <v>15.4446001053</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>DZ</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Annaba</t>
+          <t>Kinshasa</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
+          <t>Shenzhen, China</t>
         </is>
       </c>
       <c r="C109" t="n">

</xml_diff>

<commit_message>
update generated data Triggered by ad455f3795be6a8babacce84006eb7689306b3b6
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G303"/>
+  <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6524,56 +6524,56 @@
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Port-Au-Prince, Haiti</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>18.5799999237</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D197" t="n">
-        <v>-72.2925033569</v>
+        <v>-78.3575</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D198" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D199" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D200" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,26 +6649,26 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D201" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D202" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,30 +6715,30 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D203" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -6748,92 +6748,92 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D204" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D205" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D206" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D207" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,26 +6880,26 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D208" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="D209" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="D210" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,30 +6979,30 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D211" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D212" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,26 +7045,26 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D213" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D214" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,30 +7111,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D215" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7144,63 +7144,63 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-21.698299408</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D216" t="n">
-        <v>-41.301700592</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D217" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D218" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D219" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D220" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D221" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D222" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D223" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D224" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D225" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D226" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D227" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D228" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D229" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D230" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,30 +7639,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D231" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7672,26 +7672,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D232" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D233" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D234" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D235" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,30 +7804,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D236" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7837,59 +7837,59 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D237" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D238" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D239" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,26 +7936,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D240" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D241" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,30 +8002,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D242" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D243" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D244" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D245" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D246" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D247" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D248" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D249" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D250" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D251" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D252" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D253" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D254" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D255" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,26 +8464,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D256" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D257" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,30 +8530,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D258" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D259" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,26 +8596,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D260" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D261" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,30 +8662,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D262" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D263" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D264" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,26 +8761,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D265" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D266" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,30 +8827,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D268" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D269" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,26 +8926,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D270" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D271" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,30 +8992,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D272" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D273" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D274" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D275" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,26 +9124,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D276" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D277" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,30 +9190,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D278" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D279" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D280" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,26 +9289,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D281" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9322,30 +9322,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D282" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D283" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,26 +9388,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D284" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D285" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D286" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,30 +9487,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D287" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D288" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,26 +9553,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D289" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9586,30 +9586,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D290" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9619,63 +9619,63 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>20.5217990875</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D291" t="n">
-        <v>-103.3109970093</v>
+        <v>138.5335637</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-34.9431729</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D292" t="n">
-        <v>138.5335637</v>
+        <v>174.792007446</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9685,30 +9685,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-37.0080986023</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D293" t="n">
-        <v>174.792007446</v>
+        <v>153.117004394</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9718,26 +9718,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-27.3841991425</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D294" t="n">
-        <v>153.117004394</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9751,30 +9751,30 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-35.3069000244</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D295" t="n">
-        <v>149.1950073242</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -9784,92 +9784,92 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-43.4893989563</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D296" t="n">
-        <v>172.5319976807</v>
+        <v>144.796005249</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>13.4834003448</v>
+        <v>-42.883209</v>
       </c>
       <c r="D297" t="n">
-        <v>144.796005249</v>
+        <v>147.331665</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-42.883209</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D298" t="n">
-        <v>147.331665</v>
+        <v>144.843002319</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9883,30 +9883,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D299" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9916,30 +9916,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D300" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9949,26 +9949,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D301" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9982,30 +9982,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D302" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -10014,39 +10014,6 @@
         </is>
       </c>
       <c r="G302" t="inlineStr">
-        <is>
-          <t>Sydney</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" s="1" t="inlineStr">
-        <is>
-          <t>PPT</t>
-        </is>
-      </c>
-      <c r="B303" t="inlineStr">
-        <is>
-          <t>Tahiti, French Polynesia</t>
-        </is>
-      </c>
-      <c r="C303" t="n">
-        <v>-17.5536994934</v>
-      </c>
-      <c r="D303" t="n">
-        <v>-149.606994629</v>
-      </c>
-      <c r="E303" t="inlineStr">
-        <is>
-          <t>PF</t>
-        </is>
-      </c>
-      <c r="F303" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G303" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by e962eff690467612b55ee12afc802a514f4542d3
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G302"/>
+  <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5864,23 +5864,23 @@
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>CCP</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Concepción, Chile</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-36.8201</v>
+        <v>-31.31</v>
       </c>
       <c r="D177" t="n">
-        <v>-73.0444</v>
+        <v>-64.208333</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5890,30 +5890,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Concepción</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-31.31</v>
+        <v>-15.59611</v>
       </c>
       <c r="D178" t="n">
-        <v>-64.208333</v>
+        <v>-56.09667</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5923,26 +5923,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-15.59611</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D179" t="n">
-        <v>-56.09667</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5956,26 +5956,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-25.5284996033</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D180" t="n">
-        <v>-49.1758003235</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5989,26 +5989,26 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-27.6702785492</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D181" t="n">
-        <v>-48.5525016785</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -6022,30 +6022,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-3.7762799263</v>
+        <v>6.825648</v>
       </c>
       <c r="D182" t="n">
-        <v>-38.5326004028</v>
+        <v>-58.163756</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -6055,30 +6055,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6.825648</v>
+        <v>-16.69727</v>
       </c>
       <c r="D183" t="n">
-        <v>-58.163756</v>
+        <v>-49.26851</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -6088,96 +6088,96 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-16.69727</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D184" t="n">
-        <v>-49.26851</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>14.5832996368</v>
+        <v>-2.1894</v>
       </c>
       <c r="D185" t="n">
-        <v>-90.5274963379</v>
+        <v>-79.8891</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-2.1894</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D186" t="n">
-        <v>-79.8891</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6187,26 +6187,26 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-27.6116676331</v>
+        <v>-26.304408</v>
       </c>
       <c r="D187" t="n">
-        <v>-48.6727790833</v>
+        <v>-48.846383</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -6220,26 +6220,26 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-26.304408</v>
+        <v>-7.2242</v>
       </c>
       <c r="D188" t="n">
-        <v>-48.846383</v>
+        <v>-39.313</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -6253,30 +6253,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-7.2242</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D189" t="n">
-        <v>-39.313</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6286,30 +6286,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-12.021900177</v>
+        <v>-3.11286</v>
       </c>
       <c r="D190" t="n">
-        <v>-77.1143035889</v>
+        <v>-60.01949</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6319,30 +6319,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-3.11286</v>
+        <v>6.16454</v>
       </c>
       <c r="D191" t="n">
-        <v>-60.01949</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6352,30 +6352,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>6.16454</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D192" t="n">
-        <v>-75.42310000000001</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6385,30 +6385,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-38.9490013123</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D193" t="n">
-        <v>-68.1557006836</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6418,30 +6418,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>9.0713596344</v>
+        <v>5.452831</v>
       </c>
       <c r="D194" t="n">
-        <v>-79.3834991455</v>
+        <v>-55.187783</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6451,30 +6451,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>5.452831</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D195" t="n">
-        <v>-55.187783</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6484,30 +6484,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-29.9944000244</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D196" t="n">
-        <v>-51.1713981628</v>
+        <v>-78.3575</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6517,30 +6517,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D197" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6550,26 +6550,26 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D198" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D199" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D200" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,30 +6649,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D201" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D202" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,92 +6715,92 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D203" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D204" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D205" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6814,26 +6814,26 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D206" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D207" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,30 +6880,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="D208" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="D209" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D210" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,26 +6979,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D211" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D212" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,30 +7045,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D213" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D214" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,63 +7111,63 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>-21.698299408</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D215" t="n">
-        <v>-41.301700592</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D216" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7177,30 +7177,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D217" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D218" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D219" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D220" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D221" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D222" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D223" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D224" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D225" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D226" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D227" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D228" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D229" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D230" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,26 +7639,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D231" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7672,30 +7672,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D232" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D233" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D234" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D235" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,59 +7804,59 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D236" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D237" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7870,26 +7870,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D238" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D239" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,30 +7936,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D240" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D241" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,26 +8002,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D242" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D243" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D244" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D245" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D246" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D247" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D248" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D249" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D250" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D251" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D252" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D253" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D254" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D255" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,30 +8464,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D256" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D257" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,26 +8530,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D258" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D259" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,30 +8596,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D260" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D261" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,26 +8662,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D262" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D263" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D264" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,30 +8761,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D265" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,26 +8827,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D268" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D269" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,30 +8926,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D270" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D271" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,26 +8992,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D272" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D273" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D274" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D275" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,30 +9124,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D276" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D277" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,26 +9190,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D278" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D279" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D280" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,30 +9289,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D281" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9322,26 +9322,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D282" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D283" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,30 +9388,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D284" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D285" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D286" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,26 +9487,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D287" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D288" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,30 +9553,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D289" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9586,63 +9586,63 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>20.5217990875</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D290" t="n">
-        <v>-103.3109970093</v>
+        <v>138.5335637</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-34.9431729</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D291" t="n">
-        <v>138.5335637</v>
+        <v>174.792007446</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9652,30 +9652,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-37.0080986023</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D292" t="n">
-        <v>174.792007446</v>
+        <v>153.117004394</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9685,26 +9685,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-27.3841991425</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D293" t="n">
-        <v>153.117004394</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9718,30 +9718,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-35.3069000244</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D294" t="n">
-        <v>149.1950073242</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9751,92 +9751,92 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-43.4893989563</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D295" t="n">
-        <v>172.5319976807</v>
+        <v>144.796005249</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>13.4834003448</v>
+        <v>-42.883209</v>
       </c>
       <c r="D296" t="n">
-        <v>144.796005249</v>
+        <v>147.331665</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-42.883209</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D297" t="n">
-        <v>147.331665</v>
+        <v>144.843002319</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9850,30 +9850,30 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D298" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9883,30 +9883,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D299" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9916,26 +9916,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D300" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9949,30 +9949,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D301" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9981,39 +9981,6 @@
         </is>
       </c>
       <c r="G301" t="inlineStr">
-        <is>
-          <t>Sydney</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" s="1" t="inlineStr">
-        <is>
-          <t>PPT</t>
-        </is>
-      </c>
-      <c r="B302" t="inlineStr">
-        <is>
-          <t>Tahiti, French Polynesia</t>
-        </is>
-      </c>
-      <c r="C302" t="n">
-        <v>-17.5536994934</v>
-      </c>
-      <c r="D302" t="n">
-        <v>-149.606994629</v>
-      </c>
-      <c r="E302" t="inlineStr">
-        <is>
-          <t>PF</t>
-        </is>
-      </c>
-      <c r="F302" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G302" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 818f7d730e085317bdd4fd9072f909c0ff96f4f1
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G301"/>
+  <dimension ref="A1:G303"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5501,56 +5501,56 @@
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>-22.738</v>
+        <v>44.82946</v>
       </c>
       <c r="D166" t="n">
-        <v>-47.334</v>
+        <v>-0.58355</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Bordeaux</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>-18.348611</v>
+        <v>-22.738</v>
       </c>
       <c r="D167" t="n">
-        <v>-70.33888899999999</v>
+        <v>-47.334</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -5560,30 +5560,30 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>-25.2399997711</v>
+        <v>-18.348611</v>
       </c>
       <c r="D168" t="n">
-        <v>-57.5200004578</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5593,30 +5593,30 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-1.4563</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="D169" t="n">
-        <v>-48.5013</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5626,26 +5626,26 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>-19.624444</v>
+        <v>-1.4563</v>
       </c>
       <c r="D170" t="n">
-        <v>-43.971944</v>
+        <v>-48.5013</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5659,26 +5659,26 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-26.89245</v>
+        <v>-19.624444</v>
       </c>
       <c r="D171" t="n">
-        <v>-49.07696</v>
+        <v>-43.971944</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -5692,30 +5692,30 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>4.70159</v>
+        <v>-26.89245</v>
       </c>
       <c r="D172" t="n">
-        <v>-74.1469</v>
+        <v>-49.07696</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5725,30 +5725,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-15.79824</v>
+        <v>4.70159</v>
       </c>
       <c r="D173" t="n">
-        <v>-47.90859</v>
+        <v>-74.1469</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5758,30 +5758,30 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-34.8222</v>
+        <v>-15.79824</v>
       </c>
       <c r="D174" t="n">
-        <v>-58.5358</v>
+        <v>-47.90859</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5791,30 +5791,30 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-26.7762</v>
+        <v>-34.8222</v>
       </c>
       <c r="D175" t="n">
-        <v>-51.0125</v>
+        <v>-58.5358</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -5824,26 +5824,26 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-22.90662</v>
+        <v>-26.7762</v>
       </c>
       <c r="D176" t="n">
-        <v>-47.08576</v>
+        <v>-51.0125</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5857,30 +5857,30 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-31.31</v>
+        <v>-22.90662</v>
       </c>
       <c r="D177" t="n">
-        <v>-64.208333</v>
+        <v>-47.08576</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5890,30 +5890,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>-15.59611</v>
+        <v>-31.31</v>
       </c>
       <c r="D178" t="n">
-        <v>-56.09667</v>
+        <v>-64.208333</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5923,26 +5923,26 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-25.5284996033</v>
+        <v>-15.59611</v>
       </c>
       <c r="D179" t="n">
-        <v>-49.1758003235</v>
+        <v>-56.09667</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -5956,26 +5956,26 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-27.6702785492</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D180" t="n">
-        <v>-48.5525016785</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -5989,26 +5989,26 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-3.7762799263</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D181" t="n">
-        <v>-38.5326004028</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -6022,30 +6022,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>6.825648</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D182" t="n">
-        <v>-58.163756</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -6055,30 +6055,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>-16.69727</v>
+        <v>6.825648</v>
       </c>
       <c r="D183" t="n">
-        <v>-49.26851</v>
+        <v>-58.163756</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -6088,96 +6088,96 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>14.5832996368</v>
+        <v>-16.69727</v>
       </c>
       <c r="D184" t="n">
-        <v>-90.5274963379</v>
+        <v>-49.26851</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-2.1894</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D185" t="n">
-        <v>-79.8891</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-27.6116676331</v>
+        <v>-2.1894</v>
       </c>
       <c r="D186" t="n">
-        <v>-48.6727790833</v>
+        <v>-79.8891</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -6187,26 +6187,26 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-26.304408</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D187" t="n">
-        <v>-48.846383</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -6220,26 +6220,26 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-7.2242</v>
+        <v>-26.304408</v>
       </c>
       <c r="D188" t="n">
-        <v>-39.313</v>
+        <v>-48.846383</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -6253,30 +6253,30 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-12.021900177</v>
+        <v>-7.2242</v>
       </c>
       <c r="D189" t="n">
-        <v>-77.1143035889</v>
+        <v>-39.313</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6286,30 +6286,30 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-3.11286</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D190" t="n">
-        <v>-60.01949</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -6319,30 +6319,30 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>6.16454</v>
+        <v>-3.11286</v>
       </c>
       <c r="D191" t="n">
-        <v>-75.42310000000001</v>
+        <v>-60.01949</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6352,30 +6352,30 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-38.9490013123</v>
+        <v>6.16454</v>
       </c>
       <c r="D192" t="n">
-        <v>-68.1557006836</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -6385,30 +6385,30 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>9.0713596344</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D193" t="n">
-        <v>-79.3834991455</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -6418,30 +6418,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>5.452831</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D194" t="n">
-        <v>-55.187783</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6451,30 +6451,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-29.9944000244</v>
+        <v>5.452831</v>
       </c>
       <c r="D195" t="n">
-        <v>-51.1713981628</v>
+        <v>-55.187783</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6484,30 +6484,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-0.1291666667</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D196" t="n">
-        <v>-78.3575</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6517,30 +6517,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>-8.126489639300001</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D197" t="n">
-        <v>-34.9235992432</v>
+        <v>-78.3575</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6550,26 +6550,26 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-21.1363887787</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D198" t="n">
-        <v>-47.7766685486</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -6583,26 +6583,26 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>-22.8099994659</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D199" t="n">
-        <v>-43.2505569458</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -6616,26 +6616,26 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>-12.9086112976</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D200" t="n">
-        <v>-38.3224983215</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -6649,30 +6649,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>9.9938602448</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D201" t="n">
-        <v>-84.2088012695</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6682,30 +6682,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-33.3930015564</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D202" t="n">
-        <v>-70.7857971191</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6715,92 +6715,92 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>18.4297008514</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D203" t="n">
-        <v>-69.6688995361</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-20.807157</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D204" t="n">
-        <v>-49.378994</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-23.1791</v>
+        <v>-20.807157</v>
       </c>
       <c r="D205" t="n">
-        <v>-45.8872</v>
+        <v>-49.378994</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6814,26 +6814,26 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.1791</v>
       </c>
       <c r="D206" t="n">
-        <v>-46.4730567932</v>
+        <v>-45.8872</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -6847,26 +6847,26 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>-23.54389</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D207" t="n">
-        <v>-46.63445</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -6880,30 +6880,30 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>12.007116</v>
+        <v>-23.54389</v>
       </c>
       <c r="D208" t="n">
-        <v>-61.7882288</v>
+        <v>-46.63445</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -6913,30 +6913,30 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>14.0608</v>
+        <v>12.007116</v>
       </c>
       <c r="D209" t="n">
-        <v>-87.21720000000001</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -6946,30 +6946,30 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>-26.8251</v>
+        <v>14.0608</v>
       </c>
       <c r="D210" t="n">
-        <v>-49.2695</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -6979,26 +6979,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-18.8836116791</v>
+        <v>-26.8251</v>
       </c>
       <c r="D211" t="n">
-        <v>-48.225276947</v>
+        <v>-49.2695</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -7012,26 +7012,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-20.64871</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D212" t="n">
-        <v>-41.90857</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -7045,30 +7045,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>12.1888999939</v>
+        <v>-20.64871</v>
       </c>
       <c r="D213" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.90857</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7078,30 +7078,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-21.698299408</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D214" t="n">
-        <v>-41.301700592</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7111,63 +7111,63 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>31.7226009369</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D215" t="n">
-        <v>35.9931983948</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D216" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -7177,30 +7177,30 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D217" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7210,30 +7210,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D218" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7243,30 +7243,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D219" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7276,30 +7276,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D220" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7309,30 +7309,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D221" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7342,30 +7342,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D222" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7375,30 +7375,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D223" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7408,30 +7408,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D224" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7441,30 +7441,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D225" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7474,30 +7474,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D226" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7507,30 +7507,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D227" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7540,30 +7540,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D228" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7573,30 +7573,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D229" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7606,30 +7606,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D230" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7639,26 +7639,26 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D231" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -7672,30 +7672,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D232" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7705,30 +7705,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D233" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7738,30 +7738,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D234" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7771,30 +7771,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D235" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7804,59 +7804,59 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D236" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D237" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -7870,26 +7870,26 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D238" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7903,26 +7903,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D239" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7936,30 +7936,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D240" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7969,30 +7969,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D241" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8002,26 +8002,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D242" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8035,26 +8035,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D243" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8068,26 +8068,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D244" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8101,26 +8101,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D245" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8134,26 +8134,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D246" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8167,26 +8167,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D247" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8200,26 +8200,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D248" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8233,26 +8233,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D249" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8266,26 +8266,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D250" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8299,26 +8299,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D251" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8332,26 +8332,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D252" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8365,26 +8365,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D253" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8398,26 +8398,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D254" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8431,26 +8431,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D255" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8464,30 +8464,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D256" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8497,30 +8497,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D257" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8530,26 +8530,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D258" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8563,26 +8563,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D259" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8596,30 +8596,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D260" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8629,30 +8629,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D261" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8662,26 +8662,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D262" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8695,26 +8695,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D263" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8728,26 +8728,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D264" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8761,30 +8761,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D265" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8794,30 +8794,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8827,26 +8827,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D267" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8860,26 +8860,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D268" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8893,26 +8893,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D269" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8926,30 +8926,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D270" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8959,30 +8959,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D271" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8992,26 +8992,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D272" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9025,26 +9025,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D273" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9058,26 +9058,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D274" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9091,26 +9091,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D275" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9124,30 +9124,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D276" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9157,30 +9157,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D277" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9190,26 +9190,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D278" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9223,26 +9223,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D279" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9256,26 +9256,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D280" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9289,30 +9289,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D281" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9322,26 +9322,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D282" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9355,26 +9355,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D283" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9388,30 +9388,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D284" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9421,30 +9421,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D285" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9454,30 +9454,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D286" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9487,26 +9487,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D287" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9520,26 +9520,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D288" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9553,30 +9553,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D289" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9586,92 +9586,92 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>-34.9431729</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D290" t="n">
-        <v>138.5335637</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>-37.0080986023</v>
+        <v>29.429461</v>
       </c>
       <c r="D291" t="n">
-        <v>174.792007446</v>
+        <v>-98.487061</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>-27.3841991425</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D292" t="n">
-        <v>153.117004394</v>
+        <v>138.5335637</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9685,30 +9685,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>-35.3069000244</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D293" t="n">
-        <v>149.1950073242</v>
+        <v>174.792007446</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9718,30 +9718,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>-43.4893989563</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D294" t="n">
-        <v>172.5319976807</v>
+        <v>153.117004394</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9751,63 +9751,63 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>13.4834003448</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D295" t="n">
-        <v>144.796005249</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-42.883209</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D296" t="n">
-        <v>147.331665</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9817,63 +9817,63 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D297" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-22.0146007538</v>
+        <v>-42.883209</v>
       </c>
       <c r="D298" t="n">
-        <v>166.212997436</v>
+        <v>147.331665</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9883,26 +9883,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-31.9402999878</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D299" t="n">
-        <v>115.967002869</v>
+        <v>144.843002319</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9916,30 +9916,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-33.9460983276</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D300" t="n">
-        <v>151.177001953</v>
+        <v>166.212997436</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9949,38 +9949,104 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
+          <t>PER</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Perth, WA, Australia</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>-31.9402999878</v>
+      </c>
+      <c r="D301" t="n">
+        <v>115.967002869</v>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>Perth</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="inlineStr">
+        <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D302" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B301" t="inlineStr">
+      <c r="B303" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C301" t="n">
+      <c r="C303" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D301" t="n">
+      <c r="D303" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E301" t="inlineStr">
+      <c r="E303" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F301" t="inlineStr">
+      <c r="F303" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G301" t="inlineStr">
+      <c r="G303" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by e0d90546f8da2fd0432b5b53c3e8aba36a3d13a0
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -3436,12 +3436,12 @@
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>WHU</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Datong, China</t>
+          <t>Wuhu, China</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -3453,12 +3453,12 @@
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>WHU</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Wuhu, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -3470,90 +3470,106 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr"/>
+          <t>Kochi, India</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>9.9312</v>
+      </c>
+      <c r="D103" t="n">
+        <v>76.26730000000001</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Kochi</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>XMN</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>9.9312</v>
-      </c>
-      <c r="D104" t="n">
-        <v>76.26730000000001</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Asia Pacific</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>Kochi</t>
-        </is>
-      </c>
+          <t>Xiamen, China</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>XMN</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Xiamen, China</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
+          <t>Denpasar, Indonesia</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>-8.748169899000001</v>
+      </c>
+      <c r="D105" t="n">
+        <v>115.1669998169</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Asia Pacific</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Denpasar</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="D106" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -3563,52 +3579,36 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="D107" t="n">
-        <v>75.55094</v>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Asia Pacific</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>Kannur</t>
-        </is>
-      </c>
+          <t>Shenzhen, China</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>

</xml_diff>

<commit_message>
update generated data Triggered by c58c974f165a5223ef41fbf1fcc7aaee6c7d8e32
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G306"/>
+  <dimension ref="A1:G307"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9726,56 +9726,56 @@
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>-34.9431729</v>
+        <v>41.50069</v>
       </c>
       <c r="D295" t="n">
-        <v>138.5335637</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D296" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9785,30 +9785,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D297" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9818,26 +9818,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D298" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9851,30 +9851,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D299" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9884,92 +9884,92 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D300" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D301" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D302" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9983,30 +9983,30 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D303" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -10016,30 +10016,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D304" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -10049,26 +10049,26 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D305" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -10082,38 +10082,71 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C306" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D306" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B306" t="inlineStr">
+      <c r="B307" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C306" t="n">
+      <c r="C307" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D306" t="n">
+      <c r="D307" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E306" t="inlineStr">
+      <c r="E307" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F306" t="inlineStr">
+      <c r="F307" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G306" t="inlineStr">
+      <c r="G307" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by d03d3faa579b37af73b964a9e10e7c9365ba0a20
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G310"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9826,56 +9826,56 @@
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-34.9431729</v>
+        <v>35.93543</v>
       </c>
       <c r="D299" t="n">
-        <v>138.5335637</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D300" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9885,30 +9885,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D301" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9918,26 +9918,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D302" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9951,30 +9951,30 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D303" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -9984,92 +9984,92 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D304" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D305" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D306" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -10083,30 +10083,30 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D307" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -10116,30 +10116,30 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D308" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -10149,26 +10149,26 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D309" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -10182,38 +10182,71 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D310" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B310" t="inlineStr">
+      <c r="B311" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C310" t="n">
+      <c r="C311" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D310" t="n">
+      <c r="D311" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E310" t="inlineStr">
+      <c r="E311" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr">
+      <c r="F311" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G310" t="inlineStr">
+      <c r="G311" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 165958d743268e9b912268d7d4e971b79962ea68
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -3653,12 +3653,12 @@
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>WUX</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Wuxi, China</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -3670,12 +3670,12 @@
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>WUX</t>
+          <t>YNJ</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Wuxi, China</t>
+          <t>Yanbian, China</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -3687,12 +3687,12 @@
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>YNJ</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Yanbian, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -3704,40 +3704,56 @@
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>AMS</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr"/>
-      <c r="E113" t="inlineStr"/>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
+          <t>Amsterdam, Netherlands</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>52.3086013794</v>
+      </c>
+      <c r="D113" t="n">
+        <v>4.7638897896</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>NL</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Amsterdam</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>AMS</t>
+          <t>ATH</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Amsterdam, Netherlands</t>
+          <t>Athens, Greece</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>52.3086013794</v>
+        <v>37.9364013672</v>
       </c>
       <c r="D114" t="n">
-        <v>4.7638897896</v>
+        <v>23.9444999695</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -3747,30 +3763,30 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Amsterdam</t>
+          <t>Athens</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>ATH</t>
+          <t>BCN</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Athens, Greece</t>
+          <t>Barcelona, Spain</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>37.9364013672</v>
+        <v>41.2971000671</v>
       </c>
       <c r="D115" t="n">
-        <v>23.9444999695</v>
+        <v>2.0784599781</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -3780,30 +3796,30 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Athens</t>
+          <t>Barcelona</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>BCN</t>
+          <t>BEG</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Barcelona, Spain</t>
+          <t>Belgrade, Serbia</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>41.2971000671</v>
+        <v>44.8184013367</v>
       </c>
       <c r="D116" t="n">
-        <v>2.0784599781</v>
+        <v>20.3090991974</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -3813,30 +3829,30 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Belgrade</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>BEG</t>
+          <t>TXL</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Belgrade, Serbia</t>
+          <t>Berlin, Germany</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>44.8184013367</v>
+        <v>52.5597000122</v>
       </c>
       <c r="D117" t="n">
-        <v>20.3090991974</v>
+        <v>13.2876996994</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -3846,30 +3862,30 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Belgrade</t>
+          <t>Berlin</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>TXL</t>
+          <t>BTS</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Berlin, Germany</t>
+          <t>Bratislava, Slovakia</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>52.5597000122</v>
+        <v>48.1486</v>
       </c>
       <c r="D118" t="n">
-        <v>13.2876996994</v>
+        <v>17.1077</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -3879,30 +3895,30 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Berlin</t>
+          <t>Bratislava</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>BRU</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Brussels, Belgium</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>48.1486</v>
+        <v>50.9014015198</v>
       </c>
       <c r="D119" t="n">
-        <v>17.1077</v>
+        <v>4.4844398499</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>BE</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -3912,30 +3928,30 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Brussels</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>BRU</t>
+          <t>OTP</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Brussels, Belgium</t>
+          <t>Bucharest, Romania</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>50.9014015198</v>
+        <v>44.5722007751</v>
       </c>
       <c r="D120" t="n">
-        <v>4.4844398499</v>
+        <v>26.1021995544</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -3945,30 +3961,30 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>Brussels</t>
+          <t>Bucharest</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>OTP</t>
+          <t>BUD</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Bucharest, Romania</t>
+          <t>Budapest, Hungary</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>44.5722007751</v>
+        <v>47.4369010925</v>
       </c>
       <c r="D121" t="n">
-        <v>26.1021995544</v>
+        <v>19.2555999756</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>HU</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -3978,30 +3994,30 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>Bucharest</t>
+          <t>Budapest</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>BUD</t>
+          <t>KIV</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Budapest, Hungary</t>
+          <t>Chișinău, Moldova</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>47.4369010925</v>
+        <v>46.9277000427</v>
       </c>
       <c r="D122" t="n">
-        <v>19.2555999756</v>
+        <v>28.9309997559</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>HU</t>
+          <t>MD</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -4011,30 +4027,30 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Budapest</t>
+          <t>Chișinău</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>KIV</t>
+          <t>CPH</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Chișinău, Moldova</t>
+          <t>Copenhagen, Denmark</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>46.9277000427</v>
+        <v>55.6179008484</v>
       </c>
       <c r="D123" t="n">
-        <v>28.9309997559</v>
+        <v>12.6560001373</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>DK</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -4044,30 +4060,30 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Chișinău</t>
+          <t>Copenhagen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>CPH</t>
+          <t>ORK</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Copenhagen, Denmark</t>
+          <t>Cork, Ireland</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>55.6179008484</v>
+        <v>51.8413009644</v>
       </c>
       <c r="D124" t="n">
-        <v>12.6560001373</v>
+        <v>-8.491109848000001</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -4077,26 +4093,26 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Copenhagen</t>
+          <t>Cork</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>ORK</t>
+          <t>DUB</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Cork, Ireland</t>
+          <t>Dublin, Ireland</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>51.8413009644</v>
+        <v>53.4212989807</v>
       </c>
       <c r="D125" t="n">
-        <v>-8.491109848000001</v>
+        <v>-6.270070076</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -4110,30 +4126,30 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Cork</t>
+          <t>Dublin</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>DUB</t>
+          <t>DUS</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Dublin, Ireland</t>
+          <t>Düsseldorf, Germany</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>53.4212989807</v>
+        <v>51.2895011902</v>
       </c>
       <c r="D126" t="n">
-        <v>-6.270070076</v>
+        <v>6.7667798996</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -4143,30 +4159,30 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>Düsseldorf</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>DUS</t>
+          <t>EDI</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Düsseldorf, Germany</t>
+          <t>Edinburgh, United Kingdom</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>51.2895011902</v>
+        <v>55.9500007629</v>
       </c>
       <c r="D127" t="n">
-        <v>6.7667798996</v>
+        <v>-3.3724999428</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -4176,30 +4192,30 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Düsseldorf</t>
+          <t>Edinburgh</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>EDI</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Edinburgh, United Kingdom</t>
+          <t>Frankfurt, Germany</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>55.9500007629</v>
+        <v>50.0264015198</v>
       </c>
       <c r="D128" t="n">
-        <v>-3.3724999428</v>
+        <v>8.543129921</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -4209,30 +4225,30 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Edinburgh</t>
+          <t>Frankfurt</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>GVA</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Frankfurt, Germany</t>
+          <t>Geneva, Switzerland</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>50.0264015198</v>
+        <v>46.2380981445</v>
       </c>
       <c r="D129" t="n">
-        <v>8.543129921</v>
+        <v>6.1089501381</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -4242,30 +4258,30 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Frankfurt</t>
+          <t>Geneva</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>GVA</t>
+          <t>GOT</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Geneva, Switzerland</t>
+          <t>Gothenburg, Sweden</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>46.2380981445</v>
+        <v>57.6627998352</v>
       </c>
       <c r="D130" t="n">
-        <v>6.1089501381</v>
+        <v>12.279800415</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4275,30 +4291,30 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Geneva</t>
+          <t>Gothenburg</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>GOT</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Gothenburg, Sweden</t>
+          <t>Hamburg, Germany</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>57.6627998352</v>
+        <v>53.6304016113</v>
       </c>
       <c r="D131" t="n">
-        <v>12.279800415</v>
+        <v>9.9882297516</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -4308,30 +4324,30 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Gothenburg</t>
+          <t>Hamburg</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Hamburg, Germany</t>
+          <t>Helsinki, Finland</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>53.6304016113</v>
+        <v>60.317199707</v>
       </c>
       <c r="D132" t="n">
-        <v>9.9882297516</v>
+        <v>24.963300705</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>FI</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -4341,30 +4357,30 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Hamburg</t>
+          <t>Helsinki</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>HEL</t>
+          <t>IST</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Helsinki, Finland</t>
+          <t>Istanbul, Turkey</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>60.317199707</v>
+        <v>40.9768981934</v>
       </c>
       <c r="D133" t="n">
-        <v>24.963300705</v>
+        <v>28.8145999908</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>FI</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -4374,26 +4390,26 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Helsinki</t>
+          <t>Istanbul</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>IST</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Istanbul, Turkey</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>40.9768981934</v>
+        <v>38.32377</v>
       </c>
       <c r="D134" t="n">
-        <v>28.8145999908</v>
+        <v>27.14317</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -4407,30 +4423,30 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Istanbul</t>
+          <t>Izmir</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>KBP</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Kyiv, Ukraine</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>38.32377</v>
+        <v>50.3450012207</v>
       </c>
       <c r="D135" t="n">
-        <v>27.14317</v>
+        <v>30.8946990967</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -4440,30 +4456,30 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Kyiv</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>KBP</t>
+          <t>LIS</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Kyiv, Ukraine</t>
+          <t>Lisbon, Portugal</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>50.3450012207</v>
+        <v>38.7812995911</v>
       </c>
       <c r="D136" t="n">
-        <v>30.8946990967</v>
+        <v>-9.135919570900001</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -4473,30 +4489,30 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Kyiv</t>
+          <t>Lisbon</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>LIS</t>
+          <t>LHR</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Lisbon, Portugal</t>
+          <t>London, United Kingdom</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>38.7812995911</v>
+        <v>51.4706001282</v>
       </c>
       <c r="D137" t="n">
-        <v>-9.135919570900001</v>
+        <v>-0.4619410038</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -4506,30 +4522,30 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Lisbon</t>
+          <t>London</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>LHR</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>London, United Kingdom</t>
+          <t>Luxembourg City, Luxembourg</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>51.4706001282</v>
+        <v>49.6265983582</v>
       </c>
       <c r="D138" t="n">
-        <v>-0.4619410038</v>
+        <v>6.211520195</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>LU</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -4539,30 +4555,30 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Luxembourg City</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>MAD</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Luxembourg City, Luxembourg</t>
+          <t>Madrid, Spain</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>49.6265983582</v>
+        <v>40.4936</v>
       </c>
       <c r="D139" t="n">
-        <v>6.211520195</v>
+        <v>-3.56676</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>LU</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -4572,30 +4588,30 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Luxembourg City</t>
+          <t>Madrid</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>MAD</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Madrid, Spain</t>
+          <t>Manchester, United Kingdom</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>40.4936</v>
+        <v>53.3536987305</v>
       </c>
       <c r="D140" t="n">
-        <v>-3.56676</v>
+        <v>-2.2749500275</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -4605,30 +4621,30 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Manchester</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>MRS</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Manchester, United Kingdom</t>
+          <t>Marseille, France</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>53.3536987305</v>
+        <v>43.439271922</v>
       </c>
       <c r="D141" t="n">
-        <v>-2.2749500275</v>
+        <v>5.2214241028</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -4638,30 +4654,30 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Manchester</t>
+          <t>Marseille</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>MRS</t>
+          <t>MXP</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Marseille, France</t>
+          <t>Milan, Italy</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>43.439271922</v>
+        <v>45.6305999756</v>
       </c>
       <c r="D142" t="n">
-        <v>5.2214241028</v>
+        <v>8.7281103134</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -4671,30 +4687,30 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Milan</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>MXP</t>
+          <t>MSQ</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Milan, Italy</t>
+          <t>Minsk, Belarus</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>45.6305999756</v>
+        <v>53.9006</v>
       </c>
       <c r="D143" t="n">
-        <v>8.7281103134</v>
+        <v>27.599</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>BY</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -4704,30 +4720,30 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Minsk</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>MSQ</t>
+          <t>DME</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Minsk, Belarus</t>
+          <t>Moscow, Russia</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>53.9006</v>
+        <v>55.4087982178</v>
       </c>
       <c r="D144" t="n">
-        <v>27.599</v>
+        <v>37.9062995911</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>BY</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4737,30 +4753,30 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Minsk</t>
+          <t>Moscow</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>DME</t>
+          <t>MUC</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Moscow, Russia</t>
+          <t>Munich, Germany</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>55.4087982178</v>
+        <v>48.3538017273</v>
       </c>
       <c r="D145" t="n">
-        <v>37.9062995911</v>
+        <v>11.7861003876</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -4770,30 +4786,30 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Moscow</t>
+          <t>Munich</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>MUC</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Munich, Germany</t>
+          <t>Nicosia, Cyprus</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>48.3538017273</v>
+        <v>34.8750991821</v>
       </c>
       <c r="D146" t="n">
-        <v>11.7861003876</v>
+        <v>33.6249008179</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>CY</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -4803,30 +4819,30 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Munich</t>
+          <t>Nicosia</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>OSL</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Nicosia, Cyprus</t>
+          <t>Oslo, Norway</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>34.8750991821</v>
+        <v>60.193901062</v>
       </c>
       <c r="D147" t="n">
-        <v>33.6249008179</v>
+        <v>11.100399971</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>CY</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4836,30 +4852,30 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Nicosia</t>
+          <t>Oslo</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>OSL</t>
+          <t>PMO</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Oslo, Norway</t>
+          <t>Palermo, Italy</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>60.193901062</v>
+        <v>38.16114</v>
       </c>
       <c r="D148" t="n">
-        <v>11.100399971</v>
+        <v>13.31546</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -4869,30 +4885,30 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>Palermo</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>PMO</t>
+          <t>CDG</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Palermo, Italy</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>38.16114</v>
+        <v>49.0127983093</v>
       </c>
       <c r="D149" t="n">
-        <v>13.31546</v>
+        <v>2.5499999523</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -4902,30 +4918,30 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paris</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
         <is>
-          <t>CDG</t>
+          <t>PRG</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Paris, France</t>
+          <t>Prague, Czech Republic</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>49.0127983093</v>
+        <v>50.1007995605</v>
       </c>
       <c r="D150" t="n">
-        <v>2.5499999523</v>
+        <v>14.2600002289</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>CZ</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -4935,30 +4951,30 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Prague</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
         <is>
-          <t>PRG</t>
+          <t>KEF</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Prague, Czech Republic</t>
+          <t>Reykjavík, Iceland</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>50.1007995605</v>
+        <v>63.9850006104</v>
       </c>
       <c r="D151" t="n">
-        <v>14.2600002289</v>
+        <v>-22.6056003571</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>CZ</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4968,30 +4984,30 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Prague</t>
+          <t>Reykjavík</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>KEF</t>
+          <t>RIX</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Reykjavík, Iceland</t>
+          <t>Riga, Latvia</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>63.9850006104</v>
+        <v>56.9235992432</v>
       </c>
       <c r="D152" t="n">
-        <v>-22.6056003571</v>
+        <v>23.9710998535</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>LV</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -5001,30 +5017,30 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Reykjavík</t>
+          <t>Riga</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>RIX</t>
+          <t>FCO</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Riga, Latvia</t>
+          <t>Rome, Italy</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>56.9235992432</v>
+        <v>41.8045005798</v>
       </c>
       <c r="D153" t="n">
-        <v>23.9710998535</v>
+        <v>12.2508001328</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>LV</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -5034,30 +5050,30 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Riga</t>
+          <t>Rome</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>FCO</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Rome, Italy</t>
+          <t>Saint Petersburg, Russia</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>41.8045005798</v>
+        <v>59.8003005981</v>
       </c>
       <c r="D154" t="n">
-        <v>12.2508001328</v>
+        <v>30.2625007629</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -5067,30 +5083,30 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Saint Petersburg</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
         <is>
-          <t>LED</t>
+          <t>SOF</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Saint Petersburg, Russia</t>
+          <t>Sofia, Bulgaria</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>59.8003005981</v>
+        <v>42.6966934204</v>
       </c>
       <c r="D155" t="n">
-        <v>30.2625007629</v>
+        <v>23.4114360809</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>BG</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -5100,30 +5116,30 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Saint Petersburg</t>
+          <t>Sofia</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
         <is>
-          <t>SOF</t>
+          <t>ARN</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Sofia, Bulgaria</t>
+          <t>Stockholm, Sweden</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>42.6966934204</v>
+        <v>59.6519012451</v>
       </c>
       <c r="D156" t="n">
-        <v>23.4114360809</v>
+        <v>17.9186000824</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>BG</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -5133,30 +5149,30 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Stockholm</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Stockholm, Sweden</t>
+          <t>Stuttgart, Germany</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>59.6519012451</v>
+        <v>48.783333</v>
       </c>
       <c r="D157" t="n">
-        <v>17.9186000824</v>
+        <v>9.183332999999999</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -5166,30 +5182,30 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Stockholm</t>
+          <t>Stuttgart</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>TLL</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Stuttgart, Germany</t>
+          <t>Tallinn, Estonia</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>48.783333</v>
+        <v>59.4132995605</v>
       </c>
       <c r="D158" t="n">
-        <v>9.183332999999999</v>
+        <v>24.8327999115</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EE</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -5199,30 +5215,30 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Tallinn</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>TLL</t>
+          <t>TBS</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Tallinn, Estonia</t>
+          <t>Tbilisi, Georgia</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>59.4132995605</v>
+        <v>41.6692008972</v>
       </c>
       <c r="D159" t="n">
-        <v>24.8327999115</v>
+        <v>44.95470047</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>EE</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -5232,30 +5248,30 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Tallinn</t>
+          <t>Tbilisi</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>TBS</t>
+          <t>SKG</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Tbilisi, Georgia</t>
+          <t>Thessaloniki, Greece</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>41.6692008972</v>
+        <v>40.5196990967</v>
       </c>
       <c r="D160" t="n">
-        <v>44.95470047</v>
+        <v>22.9708995819</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -5265,30 +5281,30 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Tbilisi</t>
+          <t>Thessaloniki</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>SKG</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Thessaloniki, Greece</t>
+          <t>Tirana, Albania</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>40.5196990967</v>
+        <v>41.4146995544</v>
       </c>
       <c r="D161" t="n">
-        <v>22.9708995819</v>
+        <v>19.7206001282</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -5298,30 +5314,30 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Thessaloniki</t>
+          <t>Tirana</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>KLD</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Tirana, Albania</t>
+          <t>Tver, Russian Federation</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>41.4146995544</v>
+        <v>56.8587</v>
       </c>
       <c r="D162" t="n">
-        <v>19.7206001282</v>
+        <v>35.9176</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -5331,30 +5347,30 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Tirana</t>
+          <t>Tver</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>KLD</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Tver, Russian Federation</t>
+          <t>Vienna, Austria</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>56.8587</v>
+        <v>48.1102981567</v>
       </c>
       <c r="D163" t="n">
-        <v>35.9176</v>
+        <v>16.5697002411</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5364,30 +5380,30 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>Tver</t>
+          <t>Vienna</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>VIE</t>
+          <t>VNO</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Vienna, Austria</t>
+          <t>Vilnius, Lithuania</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>48.1102981567</v>
+        <v>54.6341018677</v>
       </c>
       <c r="D164" t="n">
-        <v>16.5697002411</v>
+        <v>25.2858009338</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>LT</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5397,30 +5413,30 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Vienna</t>
+          <t>Vilnius</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>VNO</t>
+          <t>WAW</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Vilnius, Lithuania</t>
+          <t>Warsaw, Poland</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>54.6341018677</v>
+        <v>52.1656990051</v>
       </c>
       <c r="D165" t="n">
-        <v>25.2858009338</v>
+        <v>20.9671001434</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5430,96 +5446,96 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>Warsaw</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>WAW</t>
+          <t>SVX</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Warsaw, Poland</t>
+          <t>Yekaterinburg, Russia</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>52.1656990051</v>
+        <v>56.8431</v>
       </c>
       <c r="D166" t="n">
-        <v>20.9671001434</v>
+        <v>60.6454</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Warsaw</t>
+          <t>Yekaterinburg</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>SVX</t>
+          <t>ZAG</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Yekaterinburg, Russia</t>
+          <t>Zagreb, Croatia</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>56.8431</v>
+        <v>45.7429008484</v>
       </c>
       <c r="D167" t="n">
-        <v>60.6454</v>
+        <v>16.0687999725</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Yekaterinburg</t>
+          <t>Zagreb</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>ZAG</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Zagreb, Croatia</t>
+          <t>Zürich, Switzerland</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>45.7429008484</v>
+        <v>47.4646987915</v>
       </c>
       <c r="D168" t="n">
-        <v>16.0687999725</v>
+        <v>8.549169540399999</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -5529,30 +5545,30 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Zagreb</t>
+          <t>Zurich</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Zürich, Switzerland</t>
+          <t>Lyon, France</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>47.4646987915</v>
+        <v>45.7263</v>
       </c>
       <c r="D169" t="n">
-        <v>8.549169540399999</v>
+        <v>5.0908</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -5562,26 +5578,26 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Zurich</t>
+          <t>Lyon</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Lyon, France</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>45.7263</v>
+        <v>44.82946</v>
       </c>
       <c r="D170" t="n">
-        <v>5.0908</v>
+        <v>-0.58355</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -5595,63 +5611,63 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Bordeaux</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>BOD</t>
+          <t>QWJ</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Bordeaux, France</t>
+          <t>Americana, Brazil</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>44.82946</v>
+        <v>-22.738</v>
       </c>
       <c r="D171" t="n">
-        <v>-0.58355</v>
+        <v>-47.334</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Americana</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>QWJ</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Americana, Brazil</t>
+          <t>Arica, Chile</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>-22.738</v>
+        <v>-18.348611</v>
       </c>
       <c r="D172" t="n">
-        <v>-47.334</v>
+        <v>-70.33888899999999</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -5661,30 +5677,30 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>Americana</t>
+          <t>Arica</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>ASU</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Arica, Chile</t>
+          <t>Asunción, Paraguay</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>-18.348611</v>
+        <v>-25.2399997711</v>
       </c>
       <c r="D173" t="n">
-        <v>-70.33888899999999</v>
+        <v>-57.5200004578</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>PY</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5694,30 +5710,30 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Arica</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>ASU</t>
+          <t>BEL</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Asunción, Paraguay</t>
+          <t>Belém, Brazil</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>-25.2399997711</v>
+        <v>-1.4563</v>
       </c>
       <c r="D174" t="n">
-        <v>-57.5200004578</v>
+        <v>-48.5013</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>PY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -5727,26 +5743,26 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Belém</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>BEL</t>
+          <t>CNF</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Belém, Brazil</t>
+          <t>Belo Horizonte, Brazil</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>-1.4563</v>
+        <v>-19.624444</v>
       </c>
       <c r="D175" t="n">
-        <v>-48.5013</v>
+        <v>-43.971944</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -5760,26 +5776,26 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>Belém</t>
+          <t>Belo Horizonte</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>CNF</t>
+          <t>BNU</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Belo Horizonte, Brazil</t>
+          <t>Blumenau, Brazil</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>-19.624444</v>
+        <v>-26.89245</v>
       </c>
       <c r="D176" t="n">
-        <v>-43.971944</v>
+        <v>-49.07696</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -5793,30 +5809,30 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>Belo Horizonte</t>
+          <t>Blumenau</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>BNU</t>
+          <t>BOG</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Blumenau, Brazil</t>
+          <t>Bogotá, Colombia</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>-26.89245</v>
+        <v>4.70159</v>
       </c>
       <c r="D177" t="n">
-        <v>-49.07696</v>
+        <v>-74.1469</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5826,30 +5842,30 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>Blumenau</t>
+          <t>Bogotá</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>BOG</t>
+          <t>BSB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Brasilia, Brazil</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>4.70159</v>
+        <v>-15.79824</v>
       </c>
       <c r="D178" t="n">
-        <v>-74.1469</v>
+        <v>-47.90859</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -5859,30 +5875,30 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>Bogotá</t>
+          <t>Brasilia</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>BSB</t>
+          <t>EZE</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Brasilia, Brazil</t>
+          <t>Buenos Aires, Argentina</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>-15.79824</v>
+        <v>-34.8222</v>
       </c>
       <c r="D179" t="n">
-        <v>-47.90859</v>
+        <v>-58.5358</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -5892,30 +5908,30 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>Brasilia</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
         <is>
-          <t>EZE</t>
+          <t>CFC</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Buenos Aires, Argentina</t>
+          <t>Caçador, Brazil</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-34.8222</v>
+        <v>-26.7762</v>
       </c>
       <c r="D180" t="n">
-        <v>-58.5358</v>
+        <v>-51.0125</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5925,26 +5941,26 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Cacador</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
         <is>
-          <t>CFC</t>
+          <t>VCP</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Caçador, Brazil</t>
+          <t>Campinas, Brazil</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>-26.7762</v>
+        <v>-22.90662</v>
       </c>
       <c r="D181" t="n">
-        <v>-51.0125</v>
+        <v>-47.08576</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -5958,30 +5974,30 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>Cacador</t>
+          <t>Campinas</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
         <is>
-          <t>VCP</t>
+          <t>COR</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Campinas, Brazil</t>
+          <t>Córdoba, Argentina</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-22.90662</v>
+        <v>-31.31</v>
       </c>
       <c r="D182" t="n">
-        <v>-47.08576</v>
+        <v>-64.208333</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -5991,30 +6007,30 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
         <is>
-          <t>COR</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Córdoba, Argentina</t>
+          <t>Cuiabá, Brazil</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>-31.31</v>
+        <v>-15.59611</v>
       </c>
       <c r="D183" t="n">
-        <v>-64.208333</v>
+        <v>-56.09667</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -6024,26 +6040,26 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Cuiaba</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Cuiabá, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-15.59611</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="D184" t="n">
-        <v>-56.09667</v>
+        <v>-49.1758003235</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -6057,26 +6073,26 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Curitiba</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-25.5284996033</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="D185" t="n">
-        <v>-49.1758003235</v>
+        <v>-48.5525016785</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -6090,26 +6106,26 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianopolis</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-27.6702785492</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="D186" t="n">
-        <v>-48.5525016785</v>
+        <v>-38.5326004028</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -6123,30 +6139,30 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Fortaleza</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>-3.7762799263</v>
+        <v>6.825648</v>
       </c>
       <c r="D187" t="n">
-        <v>-38.5326004028</v>
+        <v>-58.163756</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -6156,30 +6172,30 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Georgetown</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Goiânia, Brazil</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>6.825648</v>
+        <v>-16.69727</v>
       </c>
       <c r="D188" t="n">
-        <v>-58.163756</v>
+        <v>-49.26851</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6189,96 +6205,96 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Goiania</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Goiânia, Brazil</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-16.69727</v>
+        <v>14.5832996368</v>
       </c>
       <c r="D189" t="n">
-        <v>-49.26851</v>
+        <v>-90.5274963379</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Guatemala City</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>14.5832996368</v>
+        <v>-2.1894</v>
       </c>
       <c r="D190" t="n">
-        <v>-90.5274963379</v>
+        <v>-79.8891</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Guayaquil</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Itajaí, Brazil</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-2.1894</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="D191" t="n">
-        <v>-79.8891</v>
+        <v>-48.6727790833</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -6288,26 +6304,26 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Itajai</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Itajaí, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>-27.6116676331</v>
+        <v>-26.304408</v>
       </c>
       <c r="D192" t="n">
-        <v>-48.6727790833</v>
+        <v>-48.846383</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -6321,26 +6337,26 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Joinville</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>-26.304408</v>
+        <v>-7.2242</v>
       </c>
       <c r="D193" t="n">
-        <v>-48.846383</v>
+        <v>-39.313</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -6354,30 +6370,30 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>-7.2242</v>
+        <v>-12.021900177</v>
       </c>
       <c r="D194" t="n">
-        <v>-39.313</v>
+        <v>-77.1143035889</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -6387,30 +6403,30 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>-12.021900177</v>
+        <v>-3.11286</v>
       </c>
       <c r="D195" t="n">
-        <v>-77.1143035889</v>
+        <v>-60.01949</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -6420,30 +6436,30 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Manaus</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>-3.11286</v>
+        <v>6.16454</v>
       </c>
       <c r="D196" t="n">
-        <v>-60.01949</v>
+        <v>-75.42310000000001</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -6453,30 +6469,30 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Medellín</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Neuquén, Argentina</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>6.16454</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="D197" t="n">
-        <v>-75.42310000000001</v>
+        <v>-68.1557006836</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -6486,30 +6502,30 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Neuquen</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Neuquén, Argentina</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>-38.9490013123</v>
+        <v>9.0713596344</v>
       </c>
       <c r="D198" t="n">
-        <v>-68.1557006836</v>
+        <v>-79.3834991455</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -6519,30 +6535,30 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Panama City</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>9.0713596344</v>
+        <v>5.452831</v>
       </c>
       <c r="D199" t="n">
-        <v>-79.3834991455</v>
+        <v>-55.187783</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -6552,30 +6568,30 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Paramaribo</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>5.452831</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="D200" t="n">
-        <v>-55.187783</v>
+        <v>-51.1713981628</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -6585,30 +6601,30 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>-29.9944000244</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="D201" t="n">
-        <v>-51.1713981628</v>
+        <v>-78.3575</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -6618,30 +6634,30 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Quito</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="D202" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -6651,26 +6667,26 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="D203" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -6684,26 +6700,26 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="D204" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -6717,26 +6733,26 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>-22.8099994659</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="D205" t="n">
-        <v>-43.2505569458</v>
+        <v>-38.3224983215</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -6750,30 +6766,30 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D206" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -6783,30 +6799,30 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D207" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -6816,92 +6832,92 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D208" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D209" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D210" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -6915,26 +6931,26 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D211" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -6948,26 +6964,26 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D212" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -6981,30 +6997,30 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>-23.54389</v>
+        <v>12.007116</v>
       </c>
       <c r="D213" t="n">
-        <v>-46.63445</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -7014,30 +7030,30 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>12.007116</v>
+        <v>14.0608</v>
       </c>
       <c r="D214" t="n">
-        <v>-61.7882288</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -7047,30 +7063,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D215" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7080,26 +7096,26 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D216" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -7113,26 +7129,26 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D217" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -7146,92 +7162,92 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CUR</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Willemstad, Curaçao</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>-20.64871</v>
+        <v>12.1888999939</v>
       </c>
       <c r="D218" t="n">
-        <v>-41.90857</v>
+        <v>-68.95980072019999</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Willemstad</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D219" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>-21.698299408</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="D220" t="n">
-        <v>-41.301700592</v>
+        <v>-52.6566009521</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -7245,40 +7261,40 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Chapeco</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Chapeco, Brazil</t>
+          <t>Bridgetown, Barbados</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>-27.1341991425</v>
+        <v>13.103562</v>
       </c>
       <c r="D221" t="n">
-        <v>-52.6566009521</v>
+        <v>-59.603226</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Chapeco</t>
+          <t>Bridgetown</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 91be2f239a3a2e3f04d3fa416bd8bb116b4fbbee
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G313"/>
+  <dimension ref="A1:G314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9925,56 +9925,56 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-34.9431729</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D302" t="n">
-        <v>138.5335637</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D303" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -9984,30 +9984,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D304" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -10017,26 +10017,26 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D305" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -10050,30 +10050,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D306" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10083,92 +10083,92 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D307" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D308" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D309" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -10182,30 +10182,30 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D310" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -10215,30 +10215,30 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D311" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -10248,26 +10248,26 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D312" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -10281,38 +10281,71 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
+          <t>SYD</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Sydney, NSW, Australia</t>
+        </is>
+      </c>
+      <c r="C313" t="n">
+        <v>-33.9460983276</v>
+      </c>
+      <c r="D313" t="n">
+        <v>151.177001953</v>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="inlineStr">
+        <is>
           <t>PPT</t>
         </is>
       </c>
-      <c r="B313" t="inlineStr">
+      <c r="B314" t="inlineStr">
         <is>
           <t>Tahiti, French Polynesia</t>
         </is>
       </c>
-      <c r="C313" t="n">
+      <c r="C314" t="n">
         <v>-17.5536994934</v>
       </c>
-      <c r="D313" t="n">
+      <c r="D314" t="n">
         <v>-149.606994629</v>
       </c>
-      <c r="E313" t="inlineStr">
+      <c r="E314" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="F313" t="inlineStr">
+      <c r="F314" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G313" t="inlineStr">
+      <c r="G314" t="inlineStr">
         <is>
           <t>Tahiti</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 6fabb3dc3666d52ae5549cd1878365ef7ce4c616
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G309"/>
+  <dimension ref="A1:G310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10266,6 +10266,39 @@
         </is>
       </c>
     </row>
+    <row r="310">
+      <c r="A310" s="1" t="inlineStr">
+        <is>
+          <t>SUV</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Suva, Fiji</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>-18.11319</v>
+      </c>
+      <c r="D310" t="n">
+        <v>178.43859</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Suva</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by 8c2616090023538e1e5fc244bd8648a26c9c82d9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G310"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9873,56 +9873,56 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-34.9431729</v>
+        <v>61.158555</v>
       </c>
       <c r="D298" t="n">
-        <v>138.5335637</v>
+        <v>-149.890208</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D299" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9932,30 +9932,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D300" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9965,26 +9965,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D301" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9998,30 +9998,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D302" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -10031,92 +10031,92 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D303" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D304" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D305" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -10130,30 +10130,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D306" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10163,30 +10163,30 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D307" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -10196,26 +10196,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D308" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10229,30 +10229,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D309" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10262,38 +10262,71 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D310" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B310" t="inlineStr">
+      <c r="B311" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C310" t="n">
+      <c r="C311" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D310" t="n">
+      <c r="D311" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E310" t="inlineStr">
+      <c r="E311" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr">
+      <c r="F311" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G310" t="inlineStr">
+      <c r="G311" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 3cba77a4e382e5465c14bba516bf297f73da1bbb
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G309"/>
+  <dimension ref="A1:G310"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9840,56 +9840,56 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D297" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D298" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9899,30 +9899,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D299" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9932,26 +9932,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D300" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9965,30 +9965,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D301" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9998,92 +9998,92 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D302" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D303" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D304" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -10097,30 +10097,30 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D305" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -10130,30 +10130,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D306" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10163,26 +10163,26 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D307" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -10196,30 +10196,30 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D308" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -10229,38 +10229,71 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C309" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D309" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E309" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F309" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B309" t="inlineStr">
+      <c r="B310" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C309" t="n">
+      <c r="C310" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D309" t="n">
+      <c r="D310" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E309" t="inlineStr">
+      <c r="E310" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F309" t="inlineStr">
+      <c r="F310" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G309" t="inlineStr">
+      <c r="G310" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by faca57211382f8b7f0983c0fc5301ec9ccf03b16
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G310"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7167,56 +7167,56 @@
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>31.7226009369</v>
+        <v>12.007116</v>
       </c>
       <c r="D216" t="n">
-        <v>35.9931983948</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D217" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -7226,30 +7226,30 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D218" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -7259,30 +7259,30 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D219" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7292,30 +7292,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D220" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7325,30 +7325,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D221" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7358,30 +7358,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D222" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7391,30 +7391,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D223" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7424,30 +7424,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D224" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7457,30 +7457,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D225" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7490,30 +7490,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D226" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7523,30 +7523,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D227" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7556,30 +7556,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D228" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7589,30 +7589,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D229" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7622,30 +7622,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D230" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7655,30 +7655,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D231" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7688,26 +7688,26 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D232" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -7721,30 +7721,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D233" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7754,30 +7754,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D234" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7787,30 +7787,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D235" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7820,30 +7820,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D236" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7853,59 +7853,59 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D237" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D238" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -7919,26 +7919,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D239" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7952,26 +7952,26 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D240" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -7985,30 +7985,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D241" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -8018,30 +8018,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D242" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -8051,26 +8051,26 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D243" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8084,26 +8084,26 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D244" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -8117,26 +8117,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D245" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8150,26 +8150,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D246" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8183,26 +8183,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D247" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8216,26 +8216,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D248" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8249,26 +8249,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D249" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8282,26 +8282,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D250" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8315,26 +8315,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D251" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8348,26 +8348,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D252" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8381,26 +8381,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D253" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8414,26 +8414,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D254" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8447,26 +8447,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D255" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8480,26 +8480,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D256" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8513,30 +8513,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D257" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8546,30 +8546,30 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D258" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8579,26 +8579,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D259" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8612,26 +8612,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D260" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8645,30 +8645,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D261" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8678,30 +8678,30 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D262" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -8711,26 +8711,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D263" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8744,26 +8744,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D264" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8777,26 +8777,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D265" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8810,30 +8810,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D266" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8843,30 +8843,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D267" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8876,26 +8876,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D268" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8909,26 +8909,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D269" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8942,26 +8942,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D270" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8975,30 +8975,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D271" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -9008,30 +9008,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D272" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -9041,26 +9041,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D273" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9074,26 +9074,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D274" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9107,26 +9107,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D275" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9140,26 +9140,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D276" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9173,30 +9173,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D277" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9206,30 +9206,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D278" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9239,26 +9239,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D279" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9272,26 +9272,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D280" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9305,26 +9305,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D281" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9338,30 +9338,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D282" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9371,26 +9371,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D283" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9404,26 +9404,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D284" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9437,30 +9437,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D285" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9470,30 +9470,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D286" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9503,30 +9503,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D287" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9536,26 +9536,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D288" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9569,26 +9569,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D289" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9602,30 +9602,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D290" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9635,30 +9635,30 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D291" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9668,26 +9668,26 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="D292" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9701,26 +9701,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="D293" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9734,26 +9734,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="D294" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9767,26 +9767,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="D295" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9800,26 +9800,26 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D296" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9833,30 +9833,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>44.64601</v>
+        <v>61.158555</v>
       </c>
       <c r="D297" t="n">
-        <v>-63.66844</v>
+        <v>-149.890208</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9866,63 +9866,63 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D298" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D299" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9932,30 +9932,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D300" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9965,26 +9965,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D301" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9998,30 +9998,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D302" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -10031,92 +10031,92 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D303" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D304" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D305" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -10130,30 +10130,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D306" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10163,30 +10163,30 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D307" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -10196,26 +10196,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D308" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10229,30 +10229,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D309" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10262,38 +10262,71 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C310" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D310" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B310" t="inlineStr">
+      <c r="B311" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C310" t="n">
+      <c r="C311" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D310" t="n">
+      <c r="D311" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E310" t="inlineStr">
+      <c r="E311" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F310" t="inlineStr">
+      <c r="F311" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G310" t="inlineStr">
+      <c r="G311" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 296228b743a32e4ea840725c6373c6cb6b3564cd
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G312"/>
+  <dimension ref="A1:G313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7249,56 +7249,56 @@
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LPB</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>La Paz, Bolivia</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>31.7226009369</v>
+        <v>-16.4897</v>
       </c>
       <c r="D218" t="n">
-        <v>35.9931983948</v>
+        <v>-68.1193</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BO</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>La Paz</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D219" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -7308,30 +7308,30 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D220" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -7341,30 +7341,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D221" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7374,30 +7374,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D222" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7407,30 +7407,30 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D223" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -7440,30 +7440,30 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D224" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7473,30 +7473,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D225" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7506,30 +7506,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D226" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7539,30 +7539,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D227" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7572,30 +7572,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D228" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7605,30 +7605,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D229" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7638,30 +7638,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D230" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7671,30 +7671,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D231" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7704,30 +7704,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D232" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7737,30 +7737,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D233" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7770,26 +7770,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D234" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7803,30 +7803,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D235" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7836,30 +7836,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D236" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7869,30 +7869,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D237" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7902,30 +7902,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D238" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7935,59 +7935,59 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D239" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D240" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -8001,26 +8001,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D241" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -8034,26 +8034,26 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D242" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8067,30 +8067,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D243" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -8100,30 +8100,30 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D244" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -8133,26 +8133,26 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D245" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8166,26 +8166,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D246" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8199,26 +8199,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D247" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8232,26 +8232,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D248" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8265,26 +8265,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D249" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8298,26 +8298,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D250" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8331,26 +8331,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D251" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8364,26 +8364,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D252" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8397,26 +8397,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D253" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8430,26 +8430,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D254" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8463,26 +8463,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D255" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8496,26 +8496,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D256" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8529,26 +8529,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D257" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8562,26 +8562,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D258" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8595,30 +8595,30 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D259" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8628,30 +8628,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D260" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8661,26 +8661,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D261" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8694,26 +8694,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D262" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8727,30 +8727,30 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D263" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8760,30 +8760,30 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D264" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8793,26 +8793,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D265" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8826,26 +8826,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D266" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8859,26 +8859,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D267" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8892,30 +8892,30 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D268" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8925,30 +8925,30 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D269" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8958,26 +8958,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D270" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8991,26 +8991,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D271" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -9024,26 +9024,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D272" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -9057,30 +9057,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D273" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -9090,30 +9090,30 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D274" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -9123,26 +9123,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D275" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9156,26 +9156,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D276" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9189,26 +9189,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D277" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9222,26 +9222,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D278" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9255,30 +9255,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D279" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9288,30 +9288,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D280" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9321,26 +9321,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D281" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9354,26 +9354,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D282" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9387,26 +9387,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D283" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9420,30 +9420,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D284" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9453,26 +9453,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D285" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9486,26 +9486,26 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D286" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -9519,30 +9519,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D287" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9552,30 +9552,30 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D288" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9585,30 +9585,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D289" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9618,26 +9618,26 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D290" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -9651,26 +9651,26 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D291" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -9684,30 +9684,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D292" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9717,30 +9717,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D293" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9750,26 +9750,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="D294" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9783,26 +9783,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="D295" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9816,26 +9816,26 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="D296" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9849,26 +9849,26 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="D297" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9882,26 +9882,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D298" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9915,30 +9915,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>44.64601</v>
+        <v>61.158555</v>
       </c>
       <c r="D299" t="n">
-        <v>-63.66844</v>
+        <v>-149.890208</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9948,63 +9948,63 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D300" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D301" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -10014,30 +10014,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D302" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -10047,26 +10047,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D303" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -10080,30 +10080,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D304" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -10113,92 +10113,92 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D305" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D306" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D307" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -10212,30 +10212,30 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D308" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -10245,30 +10245,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D309" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10278,26 +10278,26 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D310" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -10311,30 +10311,30 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D311" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -10344,38 +10344,71 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C312" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D312" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B312" t="inlineStr">
+      <c r="B313" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C312" t="n">
+      <c r="C313" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D312" t="n">
+      <c r="D313" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E312" t="inlineStr">
+      <c r="E313" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F312" t="inlineStr">
+      <c r="F313" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G312" t="inlineStr">
+      <c r="G313" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 092c6d17d08a8297390d6ecba1eac0ea554e56f7
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G317"/>
+  <dimension ref="A1:G318"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7334,56 +7334,56 @@
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>PAP</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Port-au-Prince, Haiti</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>31.7226009369</v>
+        <v>18.5799999237</v>
       </c>
       <c r="D223" t="n">
-        <v>35.9931983948</v>
+        <v>-72.2925033569</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>HT</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Port-au-Prince</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D224" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -7393,30 +7393,30 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D225" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -7426,30 +7426,30 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D226" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7459,30 +7459,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D227" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7492,30 +7492,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D228" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7525,30 +7525,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D229" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7558,30 +7558,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D230" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7591,30 +7591,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D231" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7624,30 +7624,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D232" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7657,30 +7657,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D233" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7690,30 +7690,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D234" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7723,30 +7723,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D235" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7756,30 +7756,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D236" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7789,30 +7789,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D237" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7822,30 +7822,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D238" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7855,26 +7855,26 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D239" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -7888,30 +7888,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D240" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7921,30 +7921,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D241" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7954,30 +7954,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D242" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7987,30 +7987,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D243" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -8020,59 +8020,59 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D244" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D245" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -8086,26 +8086,26 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D246" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -8119,26 +8119,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D247" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8152,30 +8152,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D248" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8185,30 +8185,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D249" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8218,26 +8218,26 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D250" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -8251,26 +8251,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D251" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8284,26 +8284,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D252" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8317,26 +8317,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D253" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8350,26 +8350,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D254" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8383,26 +8383,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D255" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8416,26 +8416,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D256" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8449,26 +8449,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D257" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8482,26 +8482,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D258" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8515,26 +8515,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D259" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8548,26 +8548,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D260" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8581,26 +8581,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D261" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8614,26 +8614,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D262" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8647,26 +8647,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D263" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8680,30 +8680,30 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D264" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -8713,30 +8713,30 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D265" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -8746,26 +8746,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D266" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8779,26 +8779,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D267" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8812,30 +8812,30 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D268" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -8845,30 +8845,30 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D269" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -8878,26 +8878,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D270" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8911,26 +8911,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D271" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8944,26 +8944,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D272" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8977,30 +8977,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D273" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -9010,30 +9010,30 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D274" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -9043,26 +9043,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D275" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9076,26 +9076,26 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D276" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9109,26 +9109,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D277" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9142,30 +9142,30 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D278" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9175,30 +9175,30 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D279" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9208,26 +9208,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D280" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9241,26 +9241,26 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D281" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -9274,26 +9274,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D282" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9307,26 +9307,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D283" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9340,30 +9340,30 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D284" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9373,30 +9373,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D285" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9406,26 +9406,26 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D286" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -9439,26 +9439,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D287" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9472,26 +9472,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D288" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9505,30 +9505,30 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D289" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9538,26 +9538,26 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D290" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -9571,26 +9571,26 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D291" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -9604,30 +9604,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D292" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9637,30 +9637,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D293" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9670,30 +9670,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D294" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9703,26 +9703,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D295" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9736,26 +9736,26 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D296" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9769,30 +9769,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D297" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9802,30 +9802,30 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D298" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -9835,26 +9835,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="D299" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9868,26 +9868,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="D300" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9901,26 +9901,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="D301" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9934,26 +9934,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="D302" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9967,26 +9967,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D303" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -10000,30 +10000,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>44.64601</v>
+        <v>61.158555</v>
       </c>
       <c r="D304" t="n">
-        <v>-63.66844</v>
+        <v>-149.890208</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -10033,63 +10033,63 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D305" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D306" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10099,30 +10099,30 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D307" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -10132,26 +10132,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D308" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10165,30 +10165,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D309" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10198,92 +10198,92 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D310" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D311" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D312" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -10297,30 +10297,30 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D313" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -10330,30 +10330,30 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D314" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -10363,26 +10363,26 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D315" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -10396,30 +10396,30 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D316" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -10429,38 +10429,71 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C317" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D317" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B317" t="inlineStr">
+      <c r="B318" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C317" t="n">
+      <c r="C318" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D317" t="n">
+      <c r="D318" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E317" t="inlineStr">
+      <c r="E318" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F317" t="inlineStr">
+      <c r="F318" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G317" t="inlineStr">
+      <c r="G318" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 9ce795ba9a280858653c0af3cf1700230f04b89d
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G319"/>
+  <dimension ref="A1:G320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7384,56 +7384,56 @@
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>SJU</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>San Juan, Puerto Rico</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>31.7226009369</v>
+        <v>18.411391</v>
       </c>
       <c r="D225" t="n">
-        <v>35.9931983948</v>
+        <v>-66.10279300000001</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>San Juan</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D226" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -7443,30 +7443,30 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D227" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -7476,30 +7476,30 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D228" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7509,30 +7509,30 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D229" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -7542,30 +7542,30 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D230" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7575,30 +7575,30 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D231" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -7608,30 +7608,30 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D232" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7641,30 +7641,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D233" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7674,30 +7674,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D234" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7707,30 +7707,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D235" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7740,30 +7740,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D236" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7773,30 +7773,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D237" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7806,30 +7806,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D238" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7839,30 +7839,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D239" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7872,30 +7872,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D240" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7905,26 +7905,26 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D241" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -7938,30 +7938,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D242" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7971,30 +7971,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D243" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -8004,30 +8004,30 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D244" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -8037,30 +8037,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D245" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -8070,59 +8070,59 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D246" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D247" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8136,26 +8136,26 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D248" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -8169,26 +8169,26 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D249" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -8202,30 +8202,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D250" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8235,30 +8235,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D251" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8268,26 +8268,26 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D252" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -8301,26 +8301,26 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D253" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8334,26 +8334,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D254" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8367,26 +8367,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D255" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8400,26 +8400,26 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D256" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -8433,26 +8433,26 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D257" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8466,26 +8466,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D258" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8499,26 +8499,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D259" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8532,26 +8532,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D260" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8565,26 +8565,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D261" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8598,26 +8598,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D262" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8631,26 +8631,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D263" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8664,26 +8664,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D264" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8697,26 +8697,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D265" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8730,30 +8730,30 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D266" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -8763,30 +8763,30 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D267" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -8796,26 +8796,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D268" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8829,26 +8829,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D269" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8862,30 +8862,30 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D270" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8895,30 +8895,30 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D271" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -8928,26 +8928,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D272" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8961,26 +8961,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D273" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -8994,26 +8994,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D274" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -9027,30 +9027,30 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D275" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -9060,30 +9060,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D276" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9093,26 +9093,26 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D277" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -9126,26 +9126,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D278" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9159,26 +9159,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D279" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9192,30 +9192,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D280" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9225,30 +9225,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D281" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9258,26 +9258,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D282" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9291,26 +9291,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D283" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9324,26 +9324,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D284" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9357,26 +9357,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D285" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9390,30 +9390,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D286" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9423,30 +9423,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D287" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9456,26 +9456,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D288" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9489,26 +9489,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D289" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9522,26 +9522,26 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D290" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -9555,30 +9555,30 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D291" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9588,26 +9588,26 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D292" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9621,26 +9621,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D293" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9654,30 +9654,30 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D294" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -9687,30 +9687,30 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D295" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -9720,30 +9720,30 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D296" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9753,26 +9753,26 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D297" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9786,26 +9786,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D298" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9819,30 +9819,30 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D299" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9852,30 +9852,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D300" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9885,26 +9885,26 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="D301" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -9918,26 +9918,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="D302" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9951,26 +9951,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="D303" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -9984,26 +9984,26 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="D304" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -10017,26 +10017,26 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D305" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -10050,30 +10050,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>44.64601</v>
+        <v>61.158555</v>
       </c>
       <c r="D306" t="n">
-        <v>-63.66844</v>
+        <v>-149.890208</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10083,63 +10083,63 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D307" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D308" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -10149,30 +10149,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D309" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10182,26 +10182,26 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D310" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -10215,30 +10215,30 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D311" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -10248,92 +10248,92 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D312" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>-42.883209</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D313" t="n">
-        <v>147.331665</v>
+        <v>144.796005249</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>HBA</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hobart, Australia</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>-37.6733016968</v>
+        <v>-42.883209</v>
       </c>
       <c r="D314" t="n">
-        <v>144.843002319</v>
+        <v>147.331665</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -10347,30 +10347,30 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hobart</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D315" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -10380,30 +10380,30 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D316" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -10413,26 +10413,26 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D317" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -10446,30 +10446,30 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D318" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -10479,38 +10479,71 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
+          <t>PPT</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Tahiti, French Polynesia</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
+        <v>-17.5536994934</v>
+      </c>
+      <c r="D319" t="n">
+        <v>-149.606994629</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>Tahiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="inlineStr">
+        <is>
           <t>SUV</t>
         </is>
       </c>
-      <c r="B319" t="inlineStr">
+      <c r="B320" t="inlineStr">
         <is>
           <t>Suva, Fiji</t>
         </is>
       </c>
-      <c r="C319" t="n">
+      <c r="C320" t="n">
         <v>-18.11319</v>
       </c>
-      <c r="D319" t="n">
+      <c r="D320" t="n">
         <v>178.43859</v>
       </c>
-      <c r="E319" t="inlineStr">
+      <c r="E320" t="inlineStr">
         <is>
           <t>FJ</t>
         </is>
       </c>
-      <c r="F319" t="inlineStr">
+      <c r="F320" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G319" t="inlineStr">
+      <c r="G320" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by f420b2a1f2dc09a72770ec3dbe5411be146befee
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -7435,23 +7435,23 @@
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>PAP</t>
+          <t>SJU</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Port-au-Prince, Haiti</t>
+          <t>San Juan, Puerto Rico</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>18.5799999237</v>
+        <v>18.411391</v>
       </c>
       <c r="D228" t="n">
-        <v>-72.2925033569</v>
+        <v>-66.10279300000001</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>HT</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -7461,63 +7461,63 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Port-au-Prince</t>
+          <t>San Juan</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>SJU</t>
+          <t>BAQ</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>San Juan, Puerto Rico</t>
+          <t>Barranquilla, Colombia</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>18.411391</v>
+        <v>10.8896</v>
       </c>
       <c r="D229" t="n">
-        <v>-66.10279300000001</v>
+        <v>-74.7808</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>San Juan</t>
+          <t>Barranquilla</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BAQ</t>
+          <t>PMW</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Barranquilla, Colombia</t>
+          <t>Palmas, Brazil</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>10.8896</v>
+        <v>-10.2915000916</v>
       </c>
       <c r="D230" t="n">
-        <v>-74.7808</v>
+        <v>-48.3569984436</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7527,7 +7527,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Barranquilla</t>
+          <t>Palmas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by ad8c0b248b14a669b91cf25cf8f6039971822945
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G326"/>
+  <dimension ref="A1:G325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10471,19 +10471,19 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>HBA</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Hobart, Australia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>-42.883209</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D320" t="n">
-        <v>147.331665</v>
+        <v>144.843002319</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -10497,30 +10497,30 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Hobart</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D321" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -10530,30 +10530,30 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C322" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D322" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -10563,26 +10563,26 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C323" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D323" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -10596,30 +10596,30 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C324" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D324" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -10629,30 +10629,30 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Suva, Fiji</t>
         </is>
       </c>
       <c r="C325" t="n">
-        <v>-17.5536994934</v>
+        <v>-18.11319</v>
       </c>
       <c r="D325" t="n">
-        <v>-149.606994629</v>
+        <v>178.43859</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -10661,39 +10661,6 @@
         </is>
       </c>
       <c r="G325" t="inlineStr">
-        <is>
-          <t>Tahiti</t>
-        </is>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" s="1" t="inlineStr">
-        <is>
-          <t>SUV</t>
-        </is>
-      </c>
-      <c r="B326" t="inlineStr">
-        <is>
-          <t>Suva, Fiji</t>
-        </is>
-      </c>
-      <c r="C326" t="n">
-        <v>-18.11319</v>
-      </c>
-      <c r="D326" t="n">
-        <v>178.43859</v>
-      </c>
-      <c r="E326" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="F326" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G326" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 61f9c343c533cbf87044e6be83bdcd07eabd5168
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G325"/>
+  <dimension ref="A1:G324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7237,52 +7237,52 @@
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>CUR</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Willemstad, Curaçao</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>12.1888999939</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D222" t="n">
-        <v>-68.95980072019999</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Willemstad</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>-21.698299408</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="D223" t="n">
-        <v>-41.301700592</v>
+        <v>-52.6566009521</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -7296,228 +7296,228 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Chapeco</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Chapeco, Brazil</t>
+          <t>Bridgetown, Barbados</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>-27.1341991425</v>
+        <v>13.103562</v>
       </c>
       <c r="D224" t="n">
-        <v>-52.6566009521</v>
+        <v>-59.603226</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Chapeco</t>
+          <t>Bridgetown</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>BGI</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Bridgetown, Barbados</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>13.103562</v>
+        <v>12.007116</v>
       </c>
       <c r="D225" t="n">
-        <v>-59.603226</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Bridgetown</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>STI</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Santiago de los Caballeros, Dominican Republic</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>12.007116</v>
+        <v>19.4060993195</v>
       </c>
       <c r="D226" t="n">
-        <v>-61.7882288</v>
+        <v>-70.60469818120001</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Santiago de los Caballeros</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>STI</t>
+          <t>LPB</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros, Dominican Republic</t>
+          <t>La Paz, Bolivia</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>19.4060993195</v>
+        <v>-16.4897</v>
       </c>
       <c r="D227" t="n">
-        <v>-70.60469818120001</v>
+        <v>-68.1193</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BO</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros</t>
+          <t>La Paz</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>LPB</t>
+          <t>SJU</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>La Paz, Bolivia</t>
+          <t>San Juan, Puerto Rico</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>-16.4897</v>
+        <v>18.411391</v>
       </c>
       <c r="D228" t="n">
-        <v>-68.1193</v>
+        <v>-66.10279300000001</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>BO</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>La Paz</t>
+          <t>San Juan</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>SJU</t>
+          <t>BAQ</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>San Juan, Puerto Rico</t>
+          <t>Barranquilla, Colombia</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>18.411391</v>
+        <v>10.8896</v>
       </c>
       <c r="D229" t="n">
-        <v>-66.10279300000001</v>
+        <v>-74.7808</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>San Juan</t>
+          <t>Barranquilla</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>BAQ</t>
+          <t>PMW</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Barranquilla, Colombia</t>
+          <t>Palmas, Brazil</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>10.8896</v>
+        <v>-10.2915000916</v>
       </c>
       <c r="D230" t="n">
-        <v>-74.7808</v>
+        <v>-48.3569984436</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -7527,63 +7527,63 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Barranquilla</t>
+          <t>Palmas</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>PMW</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Palmas, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>-10.2915000916</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D231" t="n">
-        <v>-48.3569984436</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>Palmas</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D232" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -7593,30 +7593,30 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D233" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7626,30 +7626,30 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D234" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -7659,30 +7659,30 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D235" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -7692,30 +7692,30 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D236" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7725,30 +7725,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D237" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7758,30 +7758,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D238" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7791,30 +7791,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D239" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7824,30 +7824,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D240" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7857,30 +7857,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D241" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7890,30 +7890,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D242" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7923,30 +7923,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D243" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7956,30 +7956,30 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D244" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -7989,30 +7989,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D245" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -8022,30 +8022,30 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D246" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8055,26 +8055,26 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D247" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -8088,30 +8088,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D248" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8121,30 +8121,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D249" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8154,30 +8154,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D250" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8187,30 +8187,30 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D251" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -8220,59 +8220,59 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D252" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D253" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -8286,26 +8286,26 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D254" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -8319,26 +8319,26 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D255" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -8352,30 +8352,30 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D256" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8385,30 +8385,30 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D257" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -8418,26 +8418,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D258" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8451,26 +8451,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D259" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8484,26 +8484,26 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D260" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -8517,26 +8517,26 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D261" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -8550,26 +8550,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D262" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8583,26 +8583,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D263" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8616,26 +8616,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D264" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8649,26 +8649,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D265" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8682,26 +8682,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D266" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8715,26 +8715,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D267" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8748,26 +8748,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D268" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8781,26 +8781,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D269" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8814,26 +8814,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D270" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8847,26 +8847,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D271" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8880,30 +8880,30 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D272" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -8913,30 +8913,30 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D273" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -8946,26 +8946,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D274" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -8979,26 +8979,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D275" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9012,30 +9012,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D276" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9045,30 +9045,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D277" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9078,26 +9078,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D278" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9111,26 +9111,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D279" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9144,26 +9144,26 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D280" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -9177,30 +9177,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D281" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9210,30 +9210,30 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D282" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9243,26 +9243,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D283" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9276,26 +9276,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D284" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9309,26 +9309,26 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D285" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -9342,30 +9342,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D286" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9375,30 +9375,30 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D287" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -9408,26 +9408,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D288" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9441,26 +9441,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D289" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9474,26 +9474,26 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D290" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -9507,26 +9507,26 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D291" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -9540,30 +9540,30 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D292" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9573,30 +9573,30 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D293" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -9606,26 +9606,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D294" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9639,26 +9639,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D295" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9672,26 +9672,26 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D296" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -9705,30 +9705,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D297" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9738,26 +9738,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D298" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9771,26 +9771,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D299" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9804,30 +9804,30 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D300" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -9837,30 +9837,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D301" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9870,30 +9870,30 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D302" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -9903,26 +9903,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D303" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -9936,26 +9936,26 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D304" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -9969,30 +9969,30 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D305" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -10002,30 +10002,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="D306" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10035,26 +10035,26 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="D307" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -10068,26 +10068,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="D308" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10101,26 +10101,26 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="D309" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -10134,26 +10134,26 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D310" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -10167,26 +10167,26 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="D311" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -10200,30 +10200,30 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="D312" t="n">
-        <v>-149.890208</v>
+        <v>-63.66844</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -10233,63 +10233,63 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>44.64601</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D313" t="n">
-        <v>-63.66844</v>
+        <v>138.5335637</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>-34.9431729</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D314" t="n">
-        <v>138.5335637</v>
+        <v>174.792007446</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -10299,30 +10299,30 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>-37.0080986023</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D315" t="n">
-        <v>174.792007446</v>
+        <v>153.117004394</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -10332,26 +10332,26 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>-27.3841991425</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D316" t="n">
-        <v>153.117004394</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -10365,30 +10365,30 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>-35.3069000244</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D317" t="n">
-        <v>149.1950073242</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -10398,96 +10398,96 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>-43.4893989563</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D318" t="n">
-        <v>172.5319976807</v>
+        <v>144.796005249</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C319" t="n">
-        <v>13.4834003448</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D319" t="n">
-        <v>144.796005249</v>
+        <v>144.843002319</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>-37.6733016968</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D320" t="n">
-        <v>144.843002319</v>
+        <v>166.212997436</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -10497,30 +10497,30 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>-22.0146007538</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D321" t="n">
-        <v>166.212997436</v>
+        <v>115.967002869</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -10530,26 +10530,26 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C322" t="n">
-        <v>-31.9402999878</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D322" t="n">
-        <v>115.967002869</v>
+        <v>151.177001953</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -10563,30 +10563,30 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C323" t="n">
-        <v>-33.9460983276</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D323" t="n">
-        <v>151.177001953</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -10596,30 +10596,30 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Suva, Fiji</t>
         </is>
       </c>
       <c r="C324" t="n">
-        <v>-17.5536994934</v>
+        <v>-18.11319</v>
       </c>
       <c r="D324" t="n">
-        <v>-149.606994629</v>
+        <v>178.43859</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>FJ</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -10628,39 +10628,6 @@
         </is>
       </c>
       <c r="G324" t="inlineStr">
-        <is>
-          <t>Tahiti</t>
-        </is>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" s="1" t="inlineStr">
-        <is>
-          <t>SUV</t>
-        </is>
-      </c>
-      <c r="B325" t="inlineStr">
-        <is>
-          <t>Suva, Fiji</t>
-        </is>
-      </c>
-      <c r="C325" t="n">
-        <v>-18.11319</v>
-      </c>
-      <c r="D325" t="n">
-        <v>178.43859</v>
-      </c>
-      <c r="E325" t="inlineStr">
-        <is>
-          <t>FJ</t>
-        </is>
-      </c>
-      <c r="F325" t="inlineStr">
-        <is>
-          <t>Oceania</t>
-        </is>
-      </c>
-      <c r="G325" t="inlineStr">
         <is>
           <t>Suva</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 942ff53b340b76cc75a8b550a5797f97ceb5d6ef
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G326"/>
+  <dimension ref="A1:G327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10683,6 +10683,39 @@
         </is>
       </c>
     </row>
+    <row r="327">
+      <c r="A327" s="1" t="inlineStr">
+        <is>
+          <t>HBA</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Hobart, Australia</t>
+        </is>
+      </c>
+      <c r="C327" t="n">
+        <v>-42.883209</v>
+      </c>
+      <c r="D327" t="n">
+        <v>147.331665</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>Hobart</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by d19614b5f2a23f0136f88e5589b0956afc3c7fd4
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G329"/>
+  <dimension ref="A1:G330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7666,56 +7666,56 @@
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>ARU</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Aracatuba, Brazil</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>31.7226009369</v>
+        <v>-21.1413002014</v>
       </c>
       <c r="D235" t="n">
-        <v>35.9931983948</v>
+        <v>-50.4247016907</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Aracatuba</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>38.7463989258</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D236" t="n">
-        <v>48.8180007935</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7725,30 +7725,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>33.2625007629</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D237" t="n">
-        <v>44.2346000671</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7758,30 +7758,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>40.4674987793</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D238" t="n">
-        <v>50.0466995239</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7791,30 +7791,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>30.5491008759</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D239" t="n">
-        <v>47.6621017456</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7824,30 +7824,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>33.8208999634</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D240" t="n">
-        <v>35.4883995056</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7857,30 +7857,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>26.471200943</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D241" t="n">
-        <v>49.7979011536</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7890,30 +7890,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>25.2605946</v>
+        <v>26.471200943</v>
       </c>
       <c r="D242" t="n">
-        <v>51.6137665</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7923,30 +7923,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>25.2527999878</v>
+        <v>25.2605946</v>
       </c>
       <c r="D243" t="n">
-        <v>55.3643989563</v>
+        <v>51.6137665</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7956,30 +7956,30 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>36.1901</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D244" t="n">
-        <v>43.993</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -7989,30 +7989,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>32.78492</v>
+        <v>36.1901</v>
       </c>
       <c r="D245" t="n">
-        <v>34.96069</v>
+        <v>43.993</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -8022,30 +8022,30 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>21.679599762</v>
+        <v>32.78492</v>
       </c>
       <c r="D246" t="n">
-        <v>39.15650177</v>
+        <v>34.96069</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8055,30 +8055,30 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>29.226600647</v>
+        <v>21.679599762</v>
       </c>
       <c r="D247" t="n">
-        <v>47.9688987732</v>
+        <v>39.15650177</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -8088,30 +8088,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>26.2707996368</v>
+        <v>29.226600647</v>
       </c>
       <c r="D248" t="n">
-        <v>50.6335983276</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8121,30 +8121,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>23.5932998657</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D249" t="n">
-        <v>58.2844009399</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8154,30 +8154,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>31.989722</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D250" t="n">
-        <v>44.404167</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8187,26 +8187,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>30.9358005524</v>
+        <v>31.989722</v>
       </c>
       <c r="D251" t="n">
-        <v>46.0900993347</v>
+        <v>44.404167</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8220,30 +8220,30 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>32.2719</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D252" t="n">
-        <v>35.0194</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8253,30 +8253,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>24.9575996399</v>
+        <v>32.2719</v>
       </c>
       <c r="D253" t="n">
-        <v>46.6987991333</v>
+        <v>35.0194</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8286,30 +8286,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>35.5668</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D254" t="n">
-        <v>45.4161</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8319,30 +8319,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>32.0113983154</v>
+        <v>35.5668</v>
       </c>
       <c r="D255" t="n">
-        <v>34.8866996765</v>
+        <v>45.4161</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8352,59 +8352,59 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>38.94449997</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D256" t="n">
-        <v>-77.45580292</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="D257" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8418,26 +8418,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D258" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8451,26 +8451,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="D259" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8484,30 +8484,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="D260" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8517,30 +8517,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="D261" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8550,26 +8550,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D262" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8583,26 +8583,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="D263" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8616,26 +8616,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D264" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8649,26 +8649,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D265" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8682,26 +8682,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D266" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8715,26 +8715,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D267" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8748,26 +8748,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D268" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8781,26 +8781,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D269" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8814,26 +8814,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="D270" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8847,26 +8847,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D271" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8880,26 +8880,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D272" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8913,26 +8913,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="D273" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -8946,26 +8946,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="D274" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -8979,26 +8979,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="D275" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9012,30 +9012,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D276" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9045,30 +9045,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D277" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9078,26 +9078,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D278" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9111,26 +9111,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>32.30059814</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D279" t="n">
-        <v>-86.39399718999999</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9144,30 +9144,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>45.4706001282</v>
+        <v>32.30059814</v>
       </c>
       <c r="D280" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9177,30 +9177,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D281" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9210,26 +9210,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D282" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9243,26 +9243,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D283" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9276,26 +9276,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D284" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9309,30 +9309,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D285" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9342,30 +9342,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D286" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9375,26 +9375,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D287" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9408,26 +9408,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="D288" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9441,26 +9441,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="D289" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9474,30 +9474,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="D290" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9507,30 +9507,30 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D291" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9540,26 +9540,26 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D292" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9573,26 +9573,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="D293" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9606,26 +9606,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D294" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9639,26 +9639,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D295" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9672,30 +9672,30 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D296" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9705,30 +9705,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D297" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9738,26 +9738,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D298" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9771,26 +9771,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D299" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9804,26 +9804,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D300" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9837,30 +9837,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D301" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9870,26 +9870,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D302" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9903,26 +9903,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="D303" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -9936,30 +9936,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D304" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -9969,30 +9969,30 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D305" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -10002,30 +10002,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="D306" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10035,26 +10035,26 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="D307" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -10068,26 +10068,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="D308" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10101,30 +10101,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="D309" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10134,30 +10134,30 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D310" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -10167,26 +10167,26 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="D311" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -10200,26 +10200,26 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="D312" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -10233,26 +10233,26 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="D313" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -10266,26 +10266,26 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="D314" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -10299,26 +10299,26 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D315" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -10332,30 +10332,30 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>44.64601</v>
+        <v>61.158555</v>
       </c>
       <c r="D316" t="n">
-        <v>-63.66844</v>
+        <v>-149.890208</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -10365,63 +10365,63 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>-34.9431729</v>
+        <v>44.64601</v>
       </c>
       <c r="D317" t="n">
-        <v>138.5335637</v>
+        <v>-63.66844</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Adelaide</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>AKL</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Auckland, New Zealand</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C318" t="n">
-        <v>-37.0080986023</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D318" t="n">
-        <v>174.792007446</v>
+        <v>138.5335637</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -10431,30 +10431,30 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Auckland</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>BNE</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Brisbane, QLD, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C319" t="n">
-        <v>-27.3841991425</v>
+        <v>-37.0080986023</v>
       </c>
       <c r="D319" t="n">
-        <v>153.117004394</v>
+        <v>174.792007446</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -10464,26 +10464,26 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>Brisbane</t>
+          <t>Auckland</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>CBR</t>
+          <t>BNE</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Canberra, ACT, Australia</t>
+          <t>Brisbane, QLD, Australia</t>
         </is>
       </c>
       <c r="C320" t="n">
-        <v>-35.3069000244</v>
+        <v>-27.3841991425</v>
       </c>
       <c r="D320" t="n">
-        <v>149.1950073242</v>
+        <v>153.117004394</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -10497,30 +10497,30 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>Canberra</t>
+          <t>Brisbane</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>CBR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Christchurch, New Zealand</t>
+          <t>Canberra, ACT, Australia</t>
         </is>
       </c>
       <c r="C321" t="n">
-        <v>-43.4893989563</v>
+        <v>-35.3069000244</v>
       </c>
       <c r="D321" t="n">
-        <v>172.5319976807</v>
+        <v>149.1950073242</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>NZ</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -10530,96 +10530,96 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>Christchurch</t>
+          <t>Canberra</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>GUM</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Hagatna, Guam</t>
+          <t>Christchurch, New Zealand</t>
         </is>
       </c>
       <c r="C322" t="n">
-        <v>13.4834003448</v>
+        <v>-43.4893989563</v>
       </c>
       <c r="D322" t="n">
-        <v>144.796005249</v>
+        <v>172.5319976807</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>NZ</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>Hagatna</t>
+          <t>Christchurch</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>MEL</t>
+          <t>GUM</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Melbourne, VIC, Australia</t>
+          <t>Hagatna, Guam</t>
         </is>
       </c>
       <c r="C323" t="n">
-        <v>-37.6733016968</v>
+        <v>13.4834003448</v>
       </c>
       <c r="D323" t="n">
-        <v>144.843002319</v>
+        <v>144.796005249</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Oceania</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>Hagatna</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>NOU</t>
+          <t>MEL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Noumea, New Caledonia</t>
+          <t>Melbourne, VIC, Australia</t>
         </is>
       </c>
       <c r="C324" t="n">
-        <v>-22.0146007538</v>
+        <v>-37.6733016968</v>
       </c>
       <c r="D324" t="n">
-        <v>166.212997436</v>
+        <v>144.843002319</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -10629,30 +10629,30 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>Noumea</t>
+          <t>Melbourne</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>PER</t>
+          <t>NOU</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Perth, WA, Australia</t>
+          <t>Noumea, New Caledonia</t>
         </is>
       </c>
       <c r="C325" t="n">
-        <v>-31.9402999878</v>
+        <v>-22.0146007538</v>
       </c>
       <c r="D325" t="n">
-        <v>115.967002869</v>
+        <v>166.212997436</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -10662,26 +10662,26 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>Perth</t>
+          <t>Noumea</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>SYD</t>
+          <t>PER</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Sydney, NSW, Australia</t>
+          <t>Perth, WA, Australia</t>
         </is>
       </c>
       <c r="C326" t="n">
-        <v>-33.9460983276</v>
+        <v>-31.9402999878</v>
       </c>
       <c r="D326" t="n">
-        <v>151.177001953</v>
+        <v>115.967002869</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -10695,30 +10695,30 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>Perth</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>SYD</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Tahiti, French Polynesia</t>
+          <t>Sydney, NSW, Australia</t>
         </is>
       </c>
       <c r="C327" t="n">
-        <v>-17.5536994934</v>
+        <v>-33.9460983276</v>
       </c>
       <c r="D327" t="n">
-        <v>-149.606994629</v>
+        <v>151.177001953</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -10728,30 +10728,30 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>Tahiti</t>
+          <t>Sydney</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Suva, Fiji</t>
+          <t>Tahiti, French Polynesia</t>
         </is>
       </c>
       <c r="C328" t="n">
-        <v>-18.11319</v>
+        <v>-17.5536994934</v>
       </c>
       <c r="D328" t="n">
-        <v>178.43859</v>
+        <v>-149.606994629</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>FJ</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -10761,38 +10761,71 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>Suva</t>
+          <t>Tahiti</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
+          <t>SUV</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Suva, Fiji</t>
+        </is>
+      </c>
+      <c r="C329" t="n">
+        <v>-18.11319</v>
+      </c>
+      <c r="D329" t="n">
+        <v>178.43859</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>FJ</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>Oceania</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>Suva</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="inlineStr">
+        <is>
           <t>HBA</t>
         </is>
       </c>
-      <c r="B329" t="inlineStr">
+      <c r="B330" t="inlineStr">
         <is>
           <t>Hobart, Australia</t>
         </is>
       </c>
-      <c r="C329" t="n">
+      <c r="C330" t="n">
         <v>-42.883209</v>
       </c>
-      <c r="D329" t="n">
+      <c r="D330" t="n">
         <v>147.331665</v>
       </c>
-      <c r="E329" t="inlineStr">
+      <c r="E330" t="inlineStr">
         <is>
           <t>AU</t>
         </is>
       </c>
-      <c r="F329" t="inlineStr">
+      <c r="F330" t="inlineStr">
         <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="G329" t="inlineStr">
+      <c r="G330" t="inlineStr">
         <is>
           <t>Hobart</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 52f31f4948dcef75610f52b3b66eeea4ab51f4b9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -1373,10 +1373,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>5.292598</v>
+        <v>6.842178</v>
       </c>
       <c r="D29" t="n">
-        <v>-3.999133</v>
+        <v>-5.259932</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>ABIDJAN</t>
+          <t>Yamoussoukro</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>ABIDJAN</t>
+          <t>Abidjan</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 10b0b795f754b5e916ad7bbfd8f63c356c8cc1c2
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ABIDJAN, Ivory Coast</t>
+          <t>Yamoussoukro, Ivory Coast</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ABIDJAN, Ivory Coast</t>
+          <t>Abidjan, Ivory Coast</t>
         </is>
       </c>
       <c r="C30" t="n">

</xml_diff>

<commit_message>
update generated data Triggered by 29280fb8adb1c9356ef6cba1e84487adcda15e6b
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G330"/>
+  <dimension ref="A1:G329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6973,23 +6973,23 @@
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>-12.9086112976</v>
+        <v>9.9938602448</v>
       </c>
       <c r="D214" t="n">
-        <v>-38.3224983215</v>
+        <v>-84.2088012695</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -6999,30 +6999,30 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="D215" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -7032,92 +7032,92 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="D216" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="D217" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="D218" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -7131,26 +7131,26 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="D219" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -7164,26 +7164,26 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="D220" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -7197,30 +7197,30 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>-23.54389</v>
+        <v>14.0608</v>
       </c>
       <c r="D221" t="n">
-        <v>-46.63445</v>
+        <v>-87.21720000000001</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -7230,30 +7230,30 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbó, Brazil</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="D222" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -7263,26 +7263,26 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Timbó, Brazil</t>
+          <t>Uberlândia, Brazil</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="D223" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -7296,26 +7296,26 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Uberlândia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="D224" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -7329,26 +7329,26 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>-20.64871</v>
+        <v>-21.698299408</v>
       </c>
       <c r="D225" t="n">
-        <v>-41.90857</v>
+        <v>-41.301700592</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -7362,26 +7362,26 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>-21.698299408</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="D226" t="n">
-        <v>-41.301700592</v>
+        <v>-52.6566009521</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -7395,228 +7395,228 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Chapeco</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Chapeco, Brazil</t>
+          <t>Bridgetown, Barbados</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>-27.1341991425</v>
+        <v>13.103562</v>
       </c>
       <c r="D227" t="n">
-        <v>-52.6566009521</v>
+        <v>-59.603226</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>Chapeco</t>
+          <t>Bridgetown</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>BGI</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Bridgetown, Barbados</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>13.103562</v>
+        <v>12.007116</v>
       </c>
       <c r="D228" t="n">
-        <v>-59.603226</v>
+        <v>-61.7882288</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>Bridgetown</t>
+          <t>St. George's</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>STI</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Santiago de los Caballeros, Dominican Republic</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>12.007116</v>
+        <v>19.4060993195</v>
       </c>
       <c r="D229" t="n">
-        <v>-61.7882288</v>
+        <v>-70.60469818120001</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Santiago de los Caballeros</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>STI</t>
+          <t>LPB</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros, Dominican Republic</t>
+          <t>La Paz, Bolivia</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>19.4060993195</v>
+        <v>-16.4897</v>
       </c>
       <c r="D230" t="n">
-        <v>-70.60469818120001</v>
+        <v>-68.1193</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BO</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros</t>
+          <t>La Paz</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>LPB</t>
+          <t>SJU</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>La Paz, Bolivia</t>
+          <t>San Juan, Puerto Rico</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>-16.4897</v>
+        <v>18.411391</v>
       </c>
       <c r="D231" t="n">
-        <v>-68.1193</v>
+        <v>-66.10279300000001</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>BO</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>La Paz</t>
+          <t>San Juan</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>SJU</t>
+          <t>BAQ</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>San Juan, Puerto Rico</t>
+          <t>Barranquilla, Colombia</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>18.411391</v>
+        <v>10.8896</v>
       </c>
       <c r="D232" t="n">
-        <v>-66.10279300000001</v>
+        <v>-74.7808</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>San Juan</t>
+          <t>Barranquilla</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>BAQ</t>
+          <t>PMW</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Barranquilla, Colombia</t>
+          <t>Palmas, Brazil</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>10.8896</v>
+        <v>-10.2915000916</v>
       </c>
       <c r="D233" t="n">
-        <v>-74.7808</v>
+        <v>-48.3569984436</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -7626,26 +7626,26 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>Barranquilla</t>
+          <t>Palmas</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>PMW</t>
+          <t>ARU</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Palmas, Brazil</t>
+          <t>Aracatuba, Brazil</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>-10.2915000916</v>
+        <v>-21.1413002014</v>
       </c>
       <c r="D234" t="n">
-        <v>-48.3569984436</v>
+        <v>-50.4247016907</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -7659,63 +7659,63 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>Palmas</t>
+          <t>Aracatuba</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>ARU</t>
+          <t>AMM</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Aracatuba, Brazil</t>
+          <t>Amman, Jordan</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>-21.1413002014</v>
+        <v>31.7226009369</v>
       </c>
       <c r="D235" t="n">
-        <v>-50.4247016907</v>
+        <v>35.9931983948</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>JO</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>Aracatuba</t>
+          <t>Amman</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>AMM</t>
+          <t>LLK</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Amman, Jordan</t>
+          <t>Astara, Azerbaijan</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>31.7226009369</v>
+        <v>38.7463989258</v>
       </c>
       <c r="D236" t="n">
-        <v>35.9931983948</v>
+        <v>48.8180007935</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -7725,30 +7725,30 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Astara</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>LLK</t>
+          <t>BGW</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Astara, Azerbaijan</t>
+          <t>Baghdad, Iraq</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>38.7463989258</v>
+        <v>33.2625007629</v>
       </c>
       <c r="D237" t="n">
-        <v>48.8180007935</v>
+        <v>44.2346000671</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -7758,30 +7758,30 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>Astara</t>
+          <t>Baghdad</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>BGW</t>
+          <t>GYD</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Baghdad, Iraq</t>
+          <t>Baku, Azerbaijan</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>33.2625007629</v>
+        <v>40.4674987793</v>
       </c>
       <c r="D238" t="n">
-        <v>44.2346000671</v>
+        <v>50.0466995239</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -7791,30 +7791,30 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Baku</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>GYD</t>
+          <t>BSR</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Baku, Azerbaijan</t>
+          <t>Basra, Iraq</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>40.4674987793</v>
+        <v>30.5491008759</v>
       </c>
       <c r="D239" t="n">
-        <v>50.0466995239</v>
+        <v>47.6621017456</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -7824,30 +7824,30 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>Baku</t>
+          <t>Basra</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>BEY</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Basra, Iraq</t>
+          <t>Beirut, Lebanon</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>30.5491008759</v>
+        <v>33.8208999634</v>
       </c>
       <c r="D240" t="n">
-        <v>47.6621017456</v>
+        <v>35.4883995056</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -7857,30 +7857,30 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Beirut</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>BEY</t>
+          <t>DMM</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Beirut, Lebanon</t>
+          <t>Dammam, Saudi Arabia</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>33.8208999634</v>
+        <v>26.471200943</v>
       </c>
       <c r="D241" t="n">
-        <v>35.4883995056</v>
+        <v>49.7979011536</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -7890,30 +7890,30 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>Beirut</t>
+          <t>Dammam</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>DMM</t>
+          <t>DOH</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Dammam, Saudi Arabia</t>
+          <t>Doha, Qatar</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>26.471200943</v>
+        <v>25.2605946</v>
       </c>
       <c r="D242" t="n">
-        <v>49.7979011536</v>
+        <v>51.6137665</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>QA</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -7923,30 +7923,30 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>Dammam</t>
+          <t>Doha</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>DOH</t>
+          <t>DXB</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Doha, Qatar</t>
+          <t>Dubai, United Arab Emirates</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>25.2605946</v>
+        <v>25.2527999878</v>
       </c>
       <c r="D243" t="n">
-        <v>51.6137665</v>
+        <v>55.3643989563</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>QA</t>
+          <t>AE</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7956,30 +7956,30 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>Doha</t>
+          <t>Dubai</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>DXB</t>
+          <t>EBL</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Dubai, United Arab Emirates</t>
+          <t>Erbil, Iraq</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>25.2527999878</v>
+        <v>36.1901</v>
       </c>
       <c r="D244" t="n">
-        <v>55.3643989563</v>
+        <v>43.993</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>AE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -7989,30 +7989,30 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>Dubai</t>
+          <t>Erbil</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>EBL</t>
+          <t>HFA</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Erbil, Iraq</t>
+          <t>Haifa, Israel</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>36.1901</v>
+        <v>32.78492</v>
       </c>
       <c r="D245" t="n">
-        <v>43.993</v>
+        <v>34.96069</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -8022,30 +8022,30 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>Erbil</t>
+          <t>Haifa</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>HFA</t>
+          <t>JED</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Haifa, Israel</t>
+          <t>Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>32.78492</v>
+        <v>21.679599762</v>
       </c>
       <c r="D246" t="n">
-        <v>34.96069</v>
+        <v>39.15650177</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8055,30 +8055,30 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Jeddah</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>JED</t>
+          <t>KWI</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Jeddah, Saudi Arabia</t>
+          <t>Kuwait City, Kuwait</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>21.679599762</v>
+        <v>29.226600647</v>
       </c>
       <c r="D247" t="n">
-        <v>39.15650177</v>
+        <v>47.9688987732</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>KW</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -8088,30 +8088,30 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Kuwait City</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>KWI</t>
+          <t>BAH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Kuwait City, Kuwait</t>
+          <t>Manama, Bahrain</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>29.226600647</v>
+        <v>26.2707996368</v>
       </c>
       <c r="D248" t="n">
-        <v>47.9688987732</v>
+        <v>50.6335983276</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>KW</t>
+          <t>BH</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -8121,30 +8121,30 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>Kuwait City</t>
+          <t>Manama</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>BAH</t>
+          <t>MCT</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Manama, Bahrain</t>
+          <t>Muscat, Oman</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>26.2707996368</v>
+        <v>23.5932998657</v>
       </c>
       <c r="D249" t="n">
-        <v>50.6335983276</v>
+        <v>58.2844009399</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>BH</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -8154,30 +8154,30 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>Manama</t>
+          <t>Muscat</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>MCT</t>
+          <t>NJF</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Muscat, Oman</t>
+          <t>Najaf, Iraq</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>23.5932998657</v>
+        <v>31.989722</v>
       </c>
       <c r="D250" t="n">
-        <v>58.2844009399</v>
+        <v>44.404167</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8187,26 +8187,26 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>Muscat</t>
+          <t>Najaf</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>NJF</t>
+          <t>XNH</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Najaf, Iraq</t>
+          <t>Nasiriyah, Iraq</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>31.989722</v>
+        <v>30.9358005524</v>
       </c>
       <c r="D251" t="n">
-        <v>44.404167</v>
+        <v>46.0900993347</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -8220,30 +8220,30 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>Najaf</t>
+          <t>Nasiriyah</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>XNH</t>
+          <t>ZDM</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Nasiriyah, Iraq</t>
+          <t>Ramallah</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>30.9358005524</v>
+        <v>32.2719</v>
       </c>
       <c r="D252" t="n">
-        <v>46.0900993347</v>
+        <v>35.0194</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -8253,30 +8253,30 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>Nasiriyah</t>
+          <t>Ramallah</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>ZDM</t>
+          <t>RUH</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh, Saudi Arabia</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>32.2719</v>
+        <v>24.9575996399</v>
       </c>
       <c r="D253" t="n">
-        <v>35.0194</v>
+        <v>46.6987991333</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>SA</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -8286,30 +8286,30 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>Ramallah</t>
+          <t>Riyadh</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>RUH</t>
+          <t>ISU</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Riyadh, Saudi Arabia</t>
+          <t>Sulaymaniyah, Iraq</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>24.9575996399</v>
+        <v>35.5668</v>
       </c>
       <c r="D254" t="n">
-        <v>46.6987991333</v>
+        <v>45.4161</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>SA</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8319,30 +8319,30 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>Riyadh</t>
+          <t>Sulaymaniyah</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>ISU</t>
+          <t>TLV</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Sulaymaniyah, Iraq</t>
+          <t>Tel Aviv, Israel</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>35.5668</v>
+        <v>32.0113983154</v>
       </c>
       <c r="D255" t="n">
-        <v>45.4161</v>
+        <v>34.8866996765</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -8352,59 +8352,59 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Sulaymaniyah</t>
+          <t>Tel Aviv</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>TLV</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Tel Aviv, Israel</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>32.0113983154</v>
+        <v>38.94449997</v>
       </c>
       <c r="D256" t="n">
-        <v>34.8866996765</v>
+        <v>-77.45580292</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>Tel Aviv</t>
+          <t>Ashburn</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="D257" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -8418,26 +8418,26 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C258" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="D258" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -8451,26 +8451,26 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C259" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="D259" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -8484,30 +8484,30 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C260" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="D260" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -8517,30 +8517,30 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C261" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="D261" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -8550,26 +8550,26 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C262" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="D262" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -8583,26 +8583,26 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C263" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="D263" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -8616,26 +8616,26 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C264" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="D264" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -8649,26 +8649,26 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C265" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="D265" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -8682,26 +8682,26 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C266" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="D266" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -8715,26 +8715,26 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C267" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="D267" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -8748,26 +8748,26 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C268" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="D268" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -8781,26 +8781,26 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C269" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="D269" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -8814,26 +8814,26 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C270" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="D270" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -8847,26 +8847,26 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C271" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="D271" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -8880,26 +8880,26 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C272" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="D272" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -8913,26 +8913,26 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C273" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="D273" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -8946,26 +8946,26 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C274" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="D274" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -8979,26 +8979,26 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C275" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="D275" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -9012,30 +9012,30 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C276" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="D276" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -9045,30 +9045,30 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C277" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="D277" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9078,26 +9078,26 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C278" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="D278" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -9111,26 +9111,26 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MGM</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montgomery, AL, United States</t>
         </is>
       </c>
       <c r="C279" t="n">
-        <v>44.8819999695</v>
+        <v>32.30059814</v>
       </c>
       <c r="D279" t="n">
-        <v>-93.22180175779999</v>
+        <v>-86.39399718999999</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -9144,30 +9144,30 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montgomery</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>MGM</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Montgomery, AL, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C280" t="n">
-        <v>32.30059814</v>
+        <v>45.4706001282</v>
       </c>
       <c r="D280" t="n">
-        <v>-86.39399718999999</v>
+        <v>-73.7407989502</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -9177,30 +9177,30 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>Montgomery</t>
+          <t>Montréal</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C281" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="D281" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -9210,26 +9210,26 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C282" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="D282" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -9243,26 +9243,26 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C283" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="D283" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -9276,26 +9276,26 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C284" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="D284" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -9309,30 +9309,30 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C285" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="D285" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9342,30 +9342,30 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C286" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="D286" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -9375,26 +9375,26 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C287" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="D287" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -9408,26 +9408,26 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C288" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="D288" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -9441,26 +9441,26 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C289" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="D289" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -9474,30 +9474,30 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C290" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="D290" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -9507,30 +9507,30 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C291" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="D291" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -9540,26 +9540,26 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C292" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="D292" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -9573,26 +9573,26 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C293" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="D293" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -9606,26 +9606,26 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C294" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="D294" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -9639,26 +9639,26 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C295" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="D295" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -9672,30 +9672,30 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C296" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="D296" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -9705,30 +9705,30 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C297" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="D297" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -9738,26 +9738,26 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C298" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="D298" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9771,26 +9771,26 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C299" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="D299" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -9804,26 +9804,26 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C300" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="D300" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -9837,30 +9837,30 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C301" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="D301" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -9870,26 +9870,26 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C302" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="D302" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -9903,26 +9903,26 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C303" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="D303" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -9936,30 +9936,30 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C304" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="D304" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -9969,30 +9969,30 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C305" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="D305" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -10002,30 +10002,30 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C306" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="D306" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -10035,26 +10035,26 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C307" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="D307" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -10068,26 +10068,26 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C308" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="D308" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -10101,30 +10101,30 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C309" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="D309" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10134,30 +10134,30 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C310" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="D310" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -10167,26 +10167,26 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C311" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="D311" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -10200,26 +10200,26 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C312" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="D312" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -10233,26 +10233,26 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C313" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="D313" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -10266,26 +10266,26 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C314" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="D314" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -10299,26 +10299,26 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C315" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="D315" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -10332,30 +10332,30 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C316" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="D316" t="n">
-        <v>-149.890208</v>
+        <v>-63.66844</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -10365,63 +10365,63 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>ADL</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Adelaide, SA, Australia</t>
         </is>
       </c>
       <c r="C317" t="n">
-        <v>44.64601</v>
+        <v>-34.9431729</v>
       </c>
       <c r="D317" t="n">
-        <v>-63.66844</v>
+        <v>138.5335637</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Oceania</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Adelaide</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>ADL</t>
+          <t>AKL</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Adelaide, SA, Australia</t>
+          <t>Auckland, New Zealand</t>
         </is>
       </c>
       <c r="C318" t="n">
-     